<commit_message>
Adición de nuevas descripciones para reportes, tareas de gradle por tags y refactorización de Test
</commit_message>
<xml_diff>
--- a/src/test/resources/Descriptions/DC_AUT_002_CashManagmentTest.xlsx
+++ b/src/test/resources/Descriptions/DC_AUT_002_CashManagmentTest.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20394"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8346FF26-1993-483D-ACCD-705F53171C85}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9ECBD9C-C822-4EB4-8BFB-208DB94BCF78}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="331" uniqueCount="102">
   <si>
     <t>Escenario</t>
   </si>
@@ -311,6 +311,30 @@
   </si>
   <si>
     <t>El usuario ingresa el "Apellido Materno".||El sistema permite ingresar al información de forma correcta.</t>
+  </si>
+  <si>
+    <t>El usuario da clic en el botón "Crear".||El sistema muestra la pantalla de confirmación con el banner verde y el mensaje:
+"El registro del beneficiario fue exitoso y quedará activado 30 minutos.
+Número de operación: "</t>
+  </si>
+  <si>
+    <t>El usuario selecciona el valor "Contribuciones Gubernamentales" del campo "Tipo de beneficiario".||El sistema permite seleccionar el valor del campo "Tipo de beneficiario" y se habilita el botón "Continuar".</t>
+  </si>
+  <si>
+    <t>El usuario da clic en el botón "Continuar".||El sistema muestra la página "Asignar el impuesto
+(Paso 2 de 3)"</t>
+  </si>
+  <si>
+    <t>El usuario da clic en la lista desplegable del campo "Tipo de impuesto".||El sistema muestra varios valores:</t>
+  </si>
+  <si>
+    <t>El usuario selecciona el valor "Contribuciones Gubernamentales del Estado de México" del campo "Tipo de impuesto".||El sistema permite seleccionar el valor del campo "Tipo de impuesto" y se habilita el botón "Continuar".</t>
+  </si>
+  <si>
+    <t>El usuario valida la información de solo lectura: Sección "Tipo de beneficiario". Sección "Impuesto". Campo "Tipo de impuesto". El sistema muestra la página "Ingresa datos de autenticación".||El sistema muestra la página "Ingresa datos de autenticación".</t>
+  </si>
+  <si>
+    <t>El usuario selecciona el valor "Contribuciones Gubernamentales de la Ciudad de México" del campo "Tipo de impuesto".||El sistema permite seleccionar el valor del campo "Tipo de impuesto" y se habilita el botón "Continuar".</t>
   </si>
 </sst>
 </file>
@@ -353,11 +377,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -641,8 +668,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AF159"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J5" workbookViewId="0">
-      <selection activeCell="L7" sqref="L7"/>
+    <sheetView tabSelected="1" topLeftCell="P7" workbookViewId="0">
+      <selection activeCell="Q8" sqref="Q8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1182,7 +1209,42 @@
       <c r="K7" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="L7" s="2"/>
+      <c r="L7" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="M7" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="N7" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="O7" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="P7" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="Q7" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="R7" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="S7" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="T7" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="U7" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="V7" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="W7" s="2" t="s">
+        <v>95</v>
+      </c>
     </row>
     <row r="8" spans="1:32" ht="120" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
@@ -1216,7 +1278,33 @@
       <c r="K8" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="L8" s="2"/>
+      <c r="L8" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="M8" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="N8" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="O8" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="P8" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="Q8" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="R8" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="S8" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="T8" s="2" t="s">
+        <v>95</v>
+      </c>
     </row>
     <row r="9" spans="1:32" ht="120" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
@@ -1250,7 +1338,33 @@
       <c r="K9" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="L9" s="2"/>
+      <c r="L9" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="M9" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="N9" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="O9" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="P9" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="Q9" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="R9" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="S9" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="T9" s="2" t="s">
+        <v>95</v>
+      </c>
     </row>
     <row r="10" spans="1:32" ht="120" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">

</xml_diff>

<commit_message>
Creación de clases y métodos en Task
</commit_message>
<xml_diff>
--- a/src/test/resources/Descriptions/DC_AUT_002_CashManagmentTest.xlsx
+++ b/src/test/resources/Descriptions/DC_AUT_002_CashManagmentTest.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20394"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0715CD46-4343-40D9-AD5E-C6A2B77CBA69}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58B86EBC-B79A-4898-B65B-394CDCA89FC8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2310,7 +2310,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -2433,14 +2433,260 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="16">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color auto="1"/>
@@ -2729,8 +2975,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AR159"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView tabSelected="1" topLeftCell="A32" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3530,25 +3776,25 @@
       <c r="G10" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="H10" s="42" t="s">
+      <c r="H10" s="43" t="s">
         <v>37</v>
       </c>
-      <c r="I10" s="42" t="s">
+      <c r="I10" s="43" t="s">
         <v>80</v>
       </c>
-      <c r="J10" s="42" t="s">
+      <c r="J10" s="43" t="s">
         <v>81</v>
       </c>
-      <c r="K10" s="42" t="s">
+      <c r="K10" s="43" t="s">
         <v>82</v>
       </c>
-      <c r="L10" s="42" t="s">
+      <c r="L10" s="43" t="s">
         <v>118</v>
       </c>
       <c r="M10" s="6" t="s">
         <v>119</v>
       </c>
-      <c r="N10" s="42" t="s">
+      <c r="N10" s="43" t="s">
         <v>120</v>
       </c>
       <c r="O10" s="11" t="s">
@@ -3560,7 +3806,7 @@
       <c r="Q10" s="6" t="s">
         <v>115</v>
       </c>
-      <c r="R10" s="42" t="s">
+      <c r="R10" s="43" t="s">
         <v>116</v>
       </c>
       <c r="S10" s="9" t="s">
@@ -3593,25 +3839,25 @@
       <c r="G11" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="H11" s="42" t="s">
+      <c r="H11" s="43" t="s">
         <v>37</v>
       </c>
-      <c r="I11" s="42" t="s">
+      <c r="I11" s="43" t="s">
         <v>80</v>
       </c>
-      <c r="J11" s="42" t="s">
+      <c r="J11" s="43" t="s">
         <v>81</v>
       </c>
-      <c r="K11" s="42" t="s">
+      <c r="K11" s="43" t="s">
         <v>82</v>
       </c>
-      <c r="L11" s="42" t="s">
+      <c r="L11" s="43" t="s">
         <v>118</v>
       </c>
       <c r="M11" s="6" t="s">
         <v>119</v>
       </c>
-      <c r="N11" s="42" t="s">
+      <c r="N11" s="43" t="s">
         <v>120</v>
       </c>
       <c r="O11" s="11" t="s">
@@ -3623,7 +3869,7 @@
       <c r="Q11" s="6" t="s">
         <v>115</v>
       </c>
-      <c r="R11" s="42" t="s">
+      <c r="R11" s="43" t="s">
         <v>116</v>
       </c>
       <c r="S11" s="9" t="s">
@@ -3716,46 +3962,46 @@
       <c r="G13" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="H13" s="2" t="s">
+      <c r="H13" s="43" t="s">
         <v>37</v>
       </c>
-      <c r="I13" s="2" t="s">
+      <c r="I13" s="43" t="s">
         <v>123</v>
       </c>
-      <c r="J13" s="2" t="s">
+      <c r="J13" s="6" t="s">
         <v>124</v>
       </c>
-      <c r="K13" s="2" t="s">
+      <c r="K13" s="43" t="s">
         <v>134</v>
       </c>
-      <c r="L13" s="2" t="s">
+      <c r="L13" s="43" t="s">
         <v>135</v>
       </c>
-      <c r="M13" s="2" t="s">
+      <c r="M13" s="6" t="s">
         <v>136</v>
       </c>
-      <c r="N13" s="2" t="s">
+      <c r="N13" s="6" t="s">
         <v>137</v>
       </c>
-      <c r="O13" s="2" t="s">
+      <c r="O13" s="43" t="s">
         <v>138</v>
       </c>
-      <c r="P13" s="2" t="s">
+      <c r="P13" s="35" t="s">
         <v>139</v>
       </c>
-      <c r="Q13" s="2" t="s">
+      <c r="Q13" s="11" t="s">
         <v>140</v>
       </c>
       <c r="R13" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="S13" s="2" t="s">
+      <c r="S13" s="6" t="s">
         <v>130</v>
       </c>
-      <c r="T13" s="2" t="s">
+      <c r="T13" s="9" t="s">
         <v>56</v>
       </c>
-      <c r="U13" s="2" t="s">
+      <c r="U13" s="9" t="s">
         <v>131</v>
       </c>
       <c r="V13" s="2" t="s">
@@ -3785,28 +4031,28 @@
       <c r="G14" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="H14" s="2" t="s">
+      <c r="H14" s="43" t="s">
         <v>37</v>
       </c>
-      <c r="I14" s="2" t="s">
+      <c r="I14" s="43" t="s">
         <v>123</v>
       </c>
-      <c r="J14" s="2" t="s">
+      <c r="J14" s="6" t="s">
         <v>124</v>
       </c>
-      <c r="K14" s="2" t="s">
+      <c r="K14" s="43" t="s">
         <v>134</v>
       </c>
-      <c r="L14" s="2" t="s">
+      <c r="L14" s="43" t="s">
         <v>135</v>
       </c>
-      <c r="M14" s="2" t="s">
+      <c r="M14" s="6" t="s">
         <v>136</v>
       </c>
-      <c r="N14" s="2" t="s">
+      <c r="N14" s="6" t="s">
         <v>137</v>
       </c>
-      <c r="O14" s="2" t="s">
+      <c r="O14" s="43" t="s">
         <v>138</v>
       </c>
       <c r="P14" s="2" t="s">
@@ -3815,13 +4061,13 @@
       <c r="Q14" s="2" t="s">
         <v>144</v>
       </c>
-      <c r="R14" s="2" t="s">
+      <c r="R14" s="6" t="s">
         <v>130</v>
       </c>
-      <c r="S14" s="2" t="s">
+      <c r="S14" s="9" t="s">
         <v>56</v>
       </c>
-      <c r="T14" s="2" t="s">
+      <c r="T14" s="9" t="s">
         <v>131</v>
       </c>
       <c r="U14" s="2" t="s">
@@ -3917,19 +4163,19 @@
       <c r="G16" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="H16" s="2" t="s">
+      <c r="H16" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="I16" s="2" t="s">
+      <c r="I16" s="6" t="s">
         <v>146</v>
       </c>
-      <c r="J16" s="2" t="s">
+      <c r="J16" s="6" t="s">
         <v>157</v>
       </c>
-      <c r="K16" s="2" t="s">
+      <c r="K16" s="6" t="s">
         <v>158</v>
       </c>
-      <c r="L16" s="2" t="s">
+      <c r="L16" s="6" t="s">
         <v>159</v>
       </c>
       <c r="M16" s="2" t="s">
@@ -3995,19 +4241,19 @@
       <c r="G17" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="H17" s="2" t="s">
+      <c r="H17" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="I17" s="2" t="s">
+      <c r="I17" s="6" t="s">
         <v>146</v>
       </c>
-      <c r="J17" s="2" t="s">
+      <c r="J17" s="6" t="s">
         <v>157</v>
       </c>
-      <c r="K17" s="2" t="s">
+      <c r="K17" s="6" t="s">
         <v>158</v>
       </c>
-      <c r="L17" s="2" t="s">
+      <c r="L17" s="6" t="s">
         <v>159</v>
       </c>
       <c r="M17" s="2" t="s">
@@ -4292,22 +4538,22 @@
       <c r="T20" s="3" t="s">
         <v>213</v>
       </c>
-      <c r="U20" s="3" t="s">
+      <c r="U20" s="7" t="s">
         <v>214</v>
       </c>
-      <c r="V20" s="2" t="s">
+      <c r="V20" s="13" t="s">
         <v>173</v>
       </c>
-      <c r="W20" s="2" t="s">
+      <c r="W20" s="13" t="s">
         <v>56</v>
       </c>
-      <c r="X20" s="2" t="s">
+      <c r="X20" s="13" t="s">
         <v>131</v>
       </c>
-      <c r="Y20" s="3" t="s">
+      <c r="Y20" s="15" t="s">
         <v>215</v>
       </c>
-      <c r="Z20" s="2" t="s">
+      <c r="Z20" s="13" t="s">
         <v>204</v>
       </c>
       <c r="AA20" s="3"/>
@@ -4376,22 +4622,22 @@
       <c r="U21" s="3" t="s">
         <v>218</v>
       </c>
-      <c r="V21" s="2" t="s">
+      <c r="V21" s="13" t="s">
         <v>219</v>
       </c>
-      <c r="W21" s="2" t="s">
+      <c r="W21" s="6" t="s">
         <v>173</v>
       </c>
-      <c r="X21" s="2" t="s">
+      <c r="X21" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="Y21" s="2" t="s">
+      <c r="Y21" s="6" t="s">
         <v>131</v>
       </c>
-      <c r="Z21" s="3" t="s">
+      <c r="Z21" s="7" t="s">
         <v>215</v>
       </c>
-      <c r="AA21" s="2" t="s">
+      <c r="AA21" s="6" t="s">
         <v>204</v>
       </c>
       <c r="AB21" s="3"/>
@@ -4435,10 +4681,10 @@
       <c r="M22" s="2" t="s">
         <v>208</v>
       </c>
-      <c r="N22" s="3" t="s">
-        <v>209</v>
-      </c>
-      <c r="O22" s="3" t="s">
+      <c r="N22" s="7" t="s">
+        <v>231</v>
+      </c>
+      <c r="O22" s="46" t="s">
         <v>164</v>
       </c>
       <c r="P22" s="3" t="s">
@@ -4459,7 +4705,7 @@
       <c r="U22" s="3" t="s">
         <v>223</v>
       </c>
-      <c r="V22" s="2" t="s">
+      <c r="V22" s="6" t="s">
         <v>219</v>
       </c>
       <c r="W22" s="2" t="s">
@@ -4591,7 +4837,7 @@
       <c r="J24" s="2" t="s">
         <v>230</v>
       </c>
-      <c r="K24" s="6" t="s">
+      <c r="K24" s="42" t="s">
         <v>206</v>
       </c>
       <c r="L24" s="6" t="s">
@@ -4621,10 +4867,10 @@
       <c r="T24" s="10" t="s">
         <v>213</v>
       </c>
-      <c r="U24" s="10" t="s">
+      <c r="U24" s="44" t="s">
         <v>223</v>
       </c>
-      <c r="V24" s="2" t="s">
+      <c r="V24" s="6" t="s">
         <v>219</v>
       </c>
       <c r="W24" s="2" t="s">
@@ -4705,7 +4951,7 @@
       <c r="U25" s="10" t="s">
         <v>217</v>
       </c>
-      <c r="V25" s="10" t="s">
+      <c r="V25" s="45" t="s">
         <v>218</v>
       </c>
       <c r="W25" s="2" t="s">
@@ -8779,7 +9025,19 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="H10:O11 U10:U11 Q10:R11">
-    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="5" priority="5"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H13:O14">
+    <cfRule type="duplicateValues" dxfId="4" priority="4"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H18:O19">
+    <cfRule type="duplicateValues" dxfId="3" priority="3"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H20:S21">
+    <cfRule type="duplicateValues" dxfId="2" priority="2"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H24:AA24 H22:AA22">
+    <cfRule type="duplicateValues" dxfId="1" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Adición de descripciones para reportes de AUT_002_CashManagment
</commit_message>
<xml_diff>
--- a/src/test/resources/Descriptions/DC_AUT_002_CashManagmentTest.xlsx
+++ b/src/test/resources/Descriptions/DC_AUT_002_CashManagmentTest.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20394"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58B86EBC-B79A-4898-B65B-394CDCA89FC8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B063176-3A7D-4C6B-AE10-9030803BE324}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1195" uniqueCount="364">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1496" uniqueCount="445">
   <si>
     <t>Escenario</t>
   </si>
@@ -2106,6 +2106,309 @@
 Botón ""Ir al inicio"
 Botón "Crear otro beneficiario"</t>
   </si>
+  <si>
+    <t>El usuario da clic en la pestaña "Cuentas Cheque USD"||El sistema muestra la lista de cuentas de cheques USD.</t>
+  </si>
+  <si>
+    <t>El usuario valida el campo "Número de cuenta cheque USD".||El sistema muestra el número de la cuenta cheque USD de forma correcta.</t>
+  </si>
+  <si>
+    <t>TC_002_50_administradorConsultaCuentasChequeUSDPDF</t>
+  </si>
+  <si>
+    <t>TC_002_51_administradorConsultaCuentasChequeUSDXML</t>
+  </si>
+  <si>
+    <t>El usuario valida las cuentas de cheques de la pestaña "Cuentas Cheque MXN"||El sistema muestra la lista de cuentas de cheques MXN.</t>
+  </si>
+  <si>
+    <t>El usuario da clic en una cuenta cheque MXN.||El sistema muestra el detalle de la cuenta cheque MXN.</t>
+  </si>
+  <si>
+    <t>El usuario da clic en una cuenta cheque USD.||El sistema muestra el detalle de la cuenta cheque USD.</t>
+  </si>
+  <si>
+    <t>El usuario valida el campo "Número de cuenta cheque MXN".||El sistema muestra el número de la cuenta cheque MXN de forma correcta.</t>
+  </si>
+  <si>
+    <t>TC_002_52_administradorConsultaCuentasChequeMXNXML</t>
+  </si>
+  <si>
+    <t>TC_002_53_administradorConsultaCuentasChequeMXNPDF</t>
+  </si>
+  <si>
+    <t>El usuario da clic en un número de crédito.||El sistema muestra el detalle del número de crédito de Línea operativa.</t>
+  </si>
+  <si>
+    <t>El usuario da clic en la opción "Descargar reporte".||El sistema muestra la página "Opciones de descarga" con las opciones "Manual" y "Plantilla".</t>
+  </si>
+  <si>
+    <t>El usuario selecciona la opción "Manual".||El sistema muestra las opciones:
+Tipo de formato
+Tipo de separador
+Archivo con encabezado
+Selecciona campos del reporte
+Guardar plantilla de reporte (La plantilla se guardará al momento de la descarga)
+Botón "Limpiar Selección"
+Botón "Cancelar"
+Botón "Descargar"</t>
+  </si>
+  <si>
+    <t>El usuario valida las opciones del campo "Tipo de formato".||El sistema muestra los formatos:
+TXT
+CSV</t>
+  </si>
+  <si>
+    <t>El usuario selecciona la opción del campo "Tipo de formato": CSV||El sistema permite seleccionar la opción de forma correcta.</t>
+  </si>
+  <si>
+    <t>El usuario valida las opciones del campo "Tipo de separador".||El sistema muestra los formatos:
+Coma [,]
+Pipe [ |]
+Punto y coma [ ;]
+Tabulador [ &lt;--&gt;]
+Longitud fija</t>
+  </si>
+  <si>
+    <t>El usuario selecciona la opción del campo "Tipo de separador": Punto y coma [ ;]||El sistema permite seleccionar la opción de forma correcta.</t>
+  </si>
+  <si>
+    <t>El usuario valida la opción "Archivo con encabezado"||El sistema muestra la opción "Archivo con encabezado" deshabilitado.</t>
+  </si>
+  <si>
+    <t>El usuario mantiene deshabilitada la opción "Archivo con encabezado"||El sistema mantiene deshabilitado el radio botton de forma correcta.</t>
+  </si>
+  <si>
+    <t>El usuario valida el check "Seleccionar todos los campos de la plantilla".||El sistema muestra el check de la opción "Seleccionar todos los campos de la plantilla" deshabilitado.</t>
+  </si>
+  <si>
+    <t>El usuario activa el check "Seleccionar todos los campos de la plantilla".||El sistema permite habilitar los campos de forma correcta.</t>
+  </si>
+  <si>
+    <t>El usuario da clic en el botón "Descargar".||El sistema permite descargar el reporte de cuentas de Línea Operativa en formato CSV de forma correcta .</t>
+  </si>
+  <si>
+    <t>TC_002_54_administradorConsultaCuentasLineaOperativaCSV</t>
+  </si>
+  <si>
+    <t>El usuario da clic en un número de crédito.||El sistema muestra el detalle del número de crédito de Préstamos personales.</t>
+  </si>
+  <si>
+    <t>El usuario selecciona la opción del campo "Tipo de formato": TXT||El sistema permite seleccionar la opción de forma correcta.</t>
+  </si>
+  <si>
+    <t>El usuario selecciona la opción del campo "Tipo de separador": Pipe [ |]||El sistema permite seleccionar la opción de forma correcta.</t>
+  </si>
+  <si>
+    <t>El usuario da clic en el botón "Descargar".||El sistema permite descargar el reporte de cuentas de Préstamos Personales en formato TXT de forma correcta .</t>
+  </si>
+  <si>
+    <t>TC_002_55_administradorConsultaCuentasPrestamosPersonalesTXT</t>
+  </si>
+  <si>
+    <t>El usuario da clic en un número de contrato.||El sistema muestra el detalle del número de contrato de fondos de inversión.</t>
+  </si>
+  <si>
+    <t>El usuario selecciona la opción del campo "Tipo de separador": Coma [,]||El sistema permite seleccionar la opción de forma correcta.</t>
+  </si>
+  <si>
+    <t>El usuario da clic en el botón "Descargar".||El sistema permite descargar el reporte de cuentas de Fondos de Inversión en formato CSV de forma correcta .</t>
+  </si>
+  <si>
+    <t>TC_002_56_administradorConsultaCuentasFondosInversionCSV</t>
+  </si>
+  <si>
+    <t>El usuario da clic en un número de crédito.||El sistema muestra el detalle del número de crédito hipotecario.</t>
+  </si>
+  <si>
+    <t>El usuario selecciona la opción del campo "Tipo de separador": Longitud fija||El sistema permite seleccionar la opción de forma correcta mostrando la longitud de todos los campos en la sección "Selecciona campos del reporte".</t>
+  </si>
+  <si>
+    <t>TC_002_57_administradorConsultaCreditosHipotecariosTXT</t>
+  </si>
+  <si>
+    <t>El sisitema da clic en un número de contrato de inversiones.||El sistema muestra el detalle del número de contrato de inversiones.</t>
+  </si>
+  <si>
+    <t>El usuario selecciona la opción del campo "Tipo de separador": Tabulador [ &lt;--&gt;]||El sistema permite seleccionar la opción de forma correcta.</t>
+  </si>
+  <si>
+    <t>TC_002_58_administradorConsultaCuentasInversionCSV</t>
+  </si>
+  <si>
+    <t>El usuario da clic en el menú "Tarjetas de Crédito"||El sistema muestra la lista de Tarjetas de Crédito .</t>
+  </si>
+  <si>
+    <t>El usuario da clic en un número de tarjeta.||El sistema muestra el detalle del número de tarjeta de crédito.</t>
+  </si>
+  <si>
+    <t>TC_002_59_administradorConsultaCuentasTDCMXNTXT</t>
+  </si>
+  <si>
+    <t>TC_002_60_administradorConsultaCuentasChequeUSDCSV</t>
+  </si>
+  <si>
+    <t>TC_002_61_administradorConsultaCuentasChequeMXNTXT</t>
+  </si>
+  <si>
+    <t>TC_002_62_administradorConsultaCuentasLineaOperativa</t>
+  </si>
+  <si>
+    <t>El usuario valida que se muestre el campo "País".||El sistema muestra el campo "País" de forma correcta.</t>
+  </si>
+  <si>
+    <t>El usuario valida que se muestre el campo "Ciudad".||El sistema muestra el campo "Ciudad" de forma correcta.</t>
+  </si>
+  <si>
+    <t>El usuario valida que se muestre el campo "Estado de la cuenta".||El sistema muestra el campo "Estado de la cuenta" de forma correcta.</t>
+  </si>
+  <si>
+    <t>El usuario valida que se muestre el campo "Tasa ordinaria".||El sistema muestra el campo "Tasa ordinaria" de forma correcta.</t>
+  </si>
+  <si>
+    <t>El usuario valida que se muestre el campo "Tasa moratoria".||El sistema muestra el campo "Tasa moratoria" de forma correcta.</t>
+  </si>
+  <si>
+    <t>El usuario valida que se muestre el campo "Importe autorizado".||El sistema muestra la columna "Importe autorizado" del movimiento con el siguiente formato:
+Signo $
+Separación de miles y millones con separador de coma (,)
+Signo de punto para decimales (.)
+2 decimales</t>
+  </si>
+  <si>
+    <t>El usuario valida que se muestre el campo "Capital disponible".||El sistema muestra la columna "Capital disponible" del movimiento con el siguiente formato:
+Signo $
+Separación de miles y millones con separador de coma (,)
+Signo de punto para decimales (.)
+2 decimales</t>
+  </si>
+  <si>
+    <t>El usuario valida que se muestre el campo "Capital dispuesto".||El sistema muestra la columna "Capital dispuesto" del movimiento con el siguiente formato:
+Signo $
+Separación de miles y millones con separador de coma (,)
+Signo de punto para decimales (.)
+2 decimales</t>
+  </si>
+  <si>
+    <t>El usuario valida que se muestre el campo "Interés ordinario".||El sistema muestra la columna "Interés ordinario" del movimiento con el siguiente formato:
+Signo $
+Separación de miles y millones con separador de coma (,)
+Signo de punto para decimales (.)
+2 decimales</t>
+  </si>
+  <si>
+    <t>El usuario valida que se muestre el campo "Interés moratorio".||El sistema muestra la columna "Interés moratorio" del movimiento con el siguiente formato:
+Signo $
+Separación de miles y millones con separador de coma (,)
+Signo de punto para decimales (.)
+2 decimales</t>
+  </si>
+  <si>
+    <t>El usuario valida que se muestre el campo "Comisiones".||El sistema muestra la columna "Comisiones" del movimiento con el siguiente formato:
+Signo $
+Separación de miles y millones con separador de coma (,)
+Signo de punto para decimales (.)
+2 decimales</t>
+  </si>
+  <si>
+    <t>El usuario valida que se muestre el campo "IVA de comisiones".||El sistema muestra la columna "IVA de comisiones" del movimiento con el siguiente formato:
+Signo $
+Separación de miles y millones con separador de coma (,)
+Signo de punto para decimales (.)
+2 decimales</t>
+  </si>
+  <si>
+    <t>El usuario valida que se muestre el campo "Saldo a la fecha".||El sistema muestra la columna "Saldo a la fecha" del movimiento con el siguiente formato:
+Signo $
+Separación de miles y millones con separador de coma (,)
+Signo de punto para decimales (.)
+2 decimales</t>
+  </si>
+  <si>
+    <t>El usuario valida que se muestre el campo "Fecha de vencimiento contrato".||El sistema muestra el campo "Fecha de vencimiento contrato" en formato DD/MMM/AAAA".</t>
+  </si>
+  <si>
+    <t>El usuario valida que se muestre el campo "Fecha de vencimiento de la línea".||El sistema muestra el campo "Fecha de vencimiento de la línea" en formato DD/MMM/AAAA".</t>
+  </si>
+  <si>
+    <t>El usuario valida que se muestre el campo "Valor actual TIIE".||El sistema muestra el campo "Valor actual TIIE" de forma correcta.</t>
+  </si>
+  <si>
+    <t>El usuario da clic en la opción "Ocultar detalles".||El sistema permite que la opción "Ocultar detalles" oculte la sección de Saldos.</t>
+  </si>
+  <si>
+    <t>El usuario valida que se muestre el campo de búsqueda "Seleccione fecha inicio".||El sistema muestra el campo de fecha habilitado.</t>
+  </si>
+  <si>
+    <t>El usuario valida que se muestre el campo de búsqueda "Seleccione fecha fin".||El sistema muestra el campo de fecha deshabilitado.</t>
+  </si>
+  <si>
+    <t>El usuario valida que se muestre el botón "Descargar reporte".||El sistema muestra el botón de "Descargar reporte" de forma correcta.</t>
+  </si>
+  <si>
+    <t>El usuario valida que se muestre la columna "Fecha del movimiento".||El sistema muestra la columna "Fecha del movimiento" en formato DD/MMM/AAAA".</t>
+  </si>
+  <si>
+    <t>El usuario valida que se muestre la columna "Referencia".||El sistema muestra la columna "Referencia" de forma correcta.</t>
+  </si>
+  <si>
+    <t>El usuario valida que se muestre la columna "Importe operación".||El sistema muestra la columna "Importe operación" del movimiento con el siguiente formato:
+Signo $
+Separación de miles y millones con separador de coma (,)
+Signo de punto para decimales (.)
+2 decimales</t>
+  </si>
+  <si>
+    <t>El usuario valida que se muestre la columna "Tipo transacción".||El sistema muestra la columna "Tipo transacción" de forma correcta.</t>
+  </si>
+  <si>
+    <t>El usuario valida que se muestre la columna "Tipo operación".||El sistema muestra la columna "Tipo de operación" con los valores "CARGO" o "ABONO".</t>
+  </si>
+  <si>
+    <t>El usuario indica una fecha de inicio en el campo de búsqueda "Seleccione fecha inicio".||El sistema muestra la fecha de inicio de forma correcta.</t>
+  </si>
+  <si>
+    <t>El usuario indica una fecha fin en el campo de búsqueda "Seleccione fecha fin".||El sistema muestra la fecha fin de forma correcta y el resultado de la búsqueda de movimientos en la siguiente tabla:
+Columna "Fecha del movimiento"
+Columna "Referencia"
+Columna "Importe operación"
+Columna "Tipo transacción"
+Columna "Tipo operación"</t>
+  </si>
+  <si>
+    <t>El usuario da clic en el botón "Opciones" con el icono (…).||El sistema muestra la pantalla modal de forma correcta.</t>
+  </si>
+  <si>
+    <t>El usuario da clic en el botón "Imprimir".||El sistema muestra la descarga del archivo PDF de forma correcta.</t>
+  </si>
+  <si>
+    <t>El usuario valida el campo "Ciudad".||El sistema muestra la ciudad de forma correcta.</t>
+  </si>
+  <si>
+    <t>El usuario valida el campo "Cuenta cheque".||El sistema muestra la cuenta cheque de forma correcta.</t>
+  </si>
+  <si>
+    <t>El usuario valida el campo "Fecha última pago".||El sistema muestra la fecha último pago de forma correcta en formato DD/MMM/AAAA".</t>
+  </si>
+  <si>
+    <t>El usuario valida el campo "Importe último pago".||El sistema muestra el campo "Importe último pago" del movimiento con el siguiente formato:
+Signo $
+Separación de miles y millones con separador de coma (,)
+Signo de punto para decimales (.)
+2 decimales</t>
+  </si>
+  <si>
+    <t>El usuario valida el campo "Plazo del crédito".||El sistema muestra el plazo del crédito de forma correcta.</t>
+  </si>
+  <si>
+    <t>El usuario valida el campo "Número de pagos pendientes".||El sistema muestra el número de pagos pendientes de forma correcta.</t>
+  </si>
+  <si>
+    <t>El usuario valida el campo "Nombre del cliente".||El sistema muestra el nombre del cliente de forma correcta.</t>
+  </si>
+  <si>
+    <t>El usuario valida el campo "Tasa".||El sistema muestra la tasa de forma correcta.</t>
+  </si>
 </sst>
 </file>
 
@@ -2127,7 +2430,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2158,8 +2461,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="12">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -2306,11 +2615,35 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </right>
+      <top style="thin">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -2448,21 +2781,23 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="16">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="5">
     <dxf>
       <font>
         <color auto="1"/>
@@ -2534,148 +2869,6 @@
           <color auto="1"/>
         </bottom>
       </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
     </dxf>
     <dxf>
       <font>
@@ -2975,8 +3168,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AR159"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A32" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25"/>
+    <sheetView tabSelected="1" topLeftCell="T62" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="T64" sqref="T64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3020,6 +3213,11 @@
     <col min="37" max="37" width="44.140625" customWidth="1"/>
     <col min="38" max="38" width="48.42578125" customWidth="1"/>
     <col min="39" max="39" width="39.42578125" customWidth="1"/>
+    <col min="40" max="40" width="56.85546875" customWidth="1"/>
+    <col min="41" max="41" width="53" customWidth="1"/>
+    <col min="42" max="42" width="62" customWidth="1"/>
+    <col min="43" max="43" width="58.28515625" customWidth="1"/>
+    <col min="44" max="44" width="49.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:44" x14ac:dyDescent="0.25">
@@ -6860,7 +7058,7 @@
       <c r="AM48" s="3"/>
       <c r="AN48" s="3"/>
     </row>
-    <row r="49" spans="1:40" ht="105" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:42" ht="105" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
         <v>358</v>
       </c>
@@ -6942,7 +7140,7 @@
       <c r="AM49" s="3"/>
       <c r="AN49" s="3"/>
     </row>
-    <row r="50" spans="1:40" ht="105" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:42" ht="105" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
         <v>359</v>
       </c>
@@ -6965,13 +7163,13 @@
       <c r="H50" s="20" t="s">
         <v>321</v>
       </c>
-      <c r="I50" s="20" t="s">
+      <c r="I50" s="28" t="s">
         <v>355</v>
       </c>
-      <c r="J50" s="20" t="s">
+      <c r="J50" s="28" t="s">
         <v>356</v>
       </c>
-      <c r="K50" s="20" t="s">
+      <c r="K50" s="28" t="s">
         <v>357</v>
       </c>
       <c r="L50" s="20" t="s">
@@ -7026,28 +7224,68 @@
       <c r="AM50" s="3"/>
       <c r="AN50" s="3"/>
     </row>
-    <row r="51" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A51" s="2"/>
+    <row r="51" spans="1:42" ht="105" x14ac:dyDescent="0.25">
+      <c r="A51" s="2" t="s">
+        <v>366</v>
+      </c>
       <c r="B51" s="2"/>
-      <c r="C51" s="2"/>
-      <c r="D51" s="2"/>
-      <c r="E51" s="2"/>
-      <c r="F51" s="2"/>
-      <c r="G51" s="2"/>
-      <c r="H51" s="2"/>
-      <c r="I51" s="2"/>
-      <c r="J51" s="2"/>
-      <c r="K51" s="2"/>
-      <c r="L51" s="2"/>
-      <c r="M51" s="18"/>
-      <c r="N51" s="18"/>
-      <c r="O51" s="18"/>
-      <c r="P51" s="18"/>
-      <c r="Q51" s="18"/>
-      <c r="R51" s="18"/>
-      <c r="S51" s="18"/>
-      <c r="T51" s="16"/>
-      <c r="U51" s="16"/>
+      <c r="C51" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="D51" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="E51" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="F51" s="26" t="s">
+        <v>35</v>
+      </c>
+      <c r="G51" s="20" t="s">
+        <v>36</v>
+      </c>
+      <c r="H51" s="47" t="s">
+        <v>321</v>
+      </c>
+      <c r="I51" s="6" t="s">
+        <v>364</v>
+      </c>
+      <c r="J51" s="6" t="s">
+        <v>370</v>
+      </c>
+      <c r="K51" s="6" t="s">
+        <v>365</v>
+      </c>
+      <c r="L51" s="48" t="s">
+        <v>325</v>
+      </c>
+      <c r="M51" s="21" t="s">
+        <v>326</v>
+      </c>
+      <c r="N51" s="23" t="s">
+        <v>327</v>
+      </c>
+      <c r="O51" s="23" t="s">
+        <v>328</v>
+      </c>
+      <c r="P51" s="21" t="s">
+        <v>329</v>
+      </c>
+      <c r="Q51" s="21" t="s">
+        <v>330</v>
+      </c>
+      <c r="R51" s="21" t="s">
+        <v>331</v>
+      </c>
+      <c r="S51" s="21" t="s">
+        <v>332</v>
+      </c>
+      <c r="T51" s="17" t="s">
+        <v>333</v>
+      </c>
+      <c r="U51" s="16" t="s">
+        <v>334</v>
+      </c>
       <c r="V51" s="16"/>
       <c r="W51" s="16"/>
       <c r="X51" s="16"/>
@@ -7068,29 +7306,71 @@
       <c r="AM51" s="3"/>
       <c r="AN51" s="3"/>
     </row>
-    <row r="52" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A52" s="2"/>
+    <row r="52" spans="1:42" ht="105" x14ac:dyDescent="0.25">
+      <c r="A52" s="2" t="s">
+        <v>367</v>
+      </c>
       <c r="B52" s="2"/>
-      <c r="C52" s="2"/>
-      <c r="D52" s="2"/>
-      <c r="E52" s="2"/>
-      <c r="F52" s="2"/>
-      <c r="G52" s="2"/>
-      <c r="H52" s="2"/>
-      <c r="I52" s="2"/>
-      <c r="J52" s="2"/>
-      <c r="K52" s="2"/>
-      <c r="L52" s="2"/>
-      <c r="M52" s="16"/>
-      <c r="N52" s="16"/>
-      <c r="O52" s="16"/>
-      <c r="P52" s="16"/>
-      <c r="Q52" s="16"/>
-      <c r="R52" s="16"/>
-      <c r="S52" s="16"/>
-      <c r="T52" s="16"/>
-      <c r="U52" s="16"/>
-      <c r="V52" s="16"/>
+      <c r="C52" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="D52" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="E52" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="F52" s="26" t="s">
+        <v>35</v>
+      </c>
+      <c r="G52" s="20" t="s">
+        <v>36</v>
+      </c>
+      <c r="H52" s="47" t="s">
+        <v>321</v>
+      </c>
+      <c r="I52" s="6" t="s">
+        <v>364</v>
+      </c>
+      <c r="J52" s="6" t="s">
+        <v>370</v>
+      </c>
+      <c r="K52" s="6" t="s">
+        <v>365</v>
+      </c>
+      <c r="L52" s="48" t="s">
+        <v>325</v>
+      </c>
+      <c r="M52" s="21" t="s">
+        <v>326</v>
+      </c>
+      <c r="N52" s="23" t="s">
+        <v>327</v>
+      </c>
+      <c r="O52" s="23" t="s">
+        <v>328</v>
+      </c>
+      <c r="P52" s="21" t="s">
+        <v>329</v>
+      </c>
+      <c r="Q52" s="21" t="s">
+        <v>330</v>
+      </c>
+      <c r="R52" s="21" t="s">
+        <v>331</v>
+      </c>
+      <c r="S52" s="21" t="s">
+        <v>332</v>
+      </c>
+      <c r="T52" s="16" t="s">
+        <v>334</v>
+      </c>
+      <c r="U52" s="16" t="s">
+        <v>335</v>
+      </c>
+      <c r="V52" s="16" t="s">
+        <v>336</v>
+      </c>
       <c r="W52" s="16"/>
       <c r="X52" s="16"/>
       <c r="Y52" s="16"/>
@@ -7110,28 +7390,68 @@
       <c r="AM52" s="3"/>
       <c r="AN52" s="3"/>
     </row>
-    <row r="53" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A53" s="2"/>
+    <row r="53" spans="1:42" ht="105" x14ac:dyDescent="0.25">
+      <c r="A53" s="2" t="s">
+        <v>372</v>
+      </c>
       <c r="B53" s="2"/>
-      <c r="C53" s="2"/>
-      <c r="D53" s="2"/>
-      <c r="E53" s="2"/>
-      <c r="F53" s="2"/>
-      <c r="G53" s="2"/>
-      <c r="H53" s="2"/>
-      <c r="I53" s="2"/>
-      <c r="J53" s="2"/>
-      <c r="K53" s="2"/>
-      <c r="L53" s="2"/>
-      <c r="M53" s="16"/>
-      <c r="N53" s="16"/>
-      <c r="O53" s="16"/>
-      <c r="P53" s="16"/>
-      <c r="Q53" s="16"/>
-      <c r="R53" s="16"/>
-      <c r="S53" s="16"/>
-      <c r="T53" s="16"/>
-      <c r="U53" s="16"/>
+      <c r="C53" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="D53" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="E53" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="F53" s="26" t="s">
+        <v>35</v>
+      </c>
+      <c r="G53" s="20" t="s">
+        <v>36</v>
+      </c>
+      <c r="H53" s="47" t="s">
+        <v>321</v>
+      </c>
+      <c r="I53" s="6" t="s">
+        <v>368</v>
+      </c>
+      <c r="J53" s="6" t="s">
+        <v>369</v>
+      </c>
+      <c r="K53" s="6" t="s">
+        <v>371</v>
+      </c>
+      <c r="L53" s="48" t="s">
+        <v>325</v>
+      </c>
+      <c r="M53" s="21" t="s">
+        <v>326</v>
+      </c>
+      <c r="N53" s="23" t="s">
+        <v>327</v>
+      </c>
+      <c r="O53" s="23" t="s">
+        <v>328</v>
+      </c>
+      <c r="P53" s="21" t="s">
+        <v>329</v>
+      </c>
+      <c r="Q53" s="21" t="s">
+        <v>330</v>
+      </c>
+      <c r="R53" s="21" t="s">
+        <v>331</v>
+      </c>
+      <c r="S53" s="21" t="s">
+        <v>332</v>
+      </c>
+      <c r="T53" s="17" t="s">
+        <v>333</v>
+      </c>
+      <c r="U53" s="16" t="s">
+        <v>334</v>
+      </c>
       <c r="V53" s="16"/>
       <c r="W53" s="16"/>
       <c r="X53" s="16"/>
@@ -7152,29 +7472,71 @@
       <c r="AM53" s="3"/>
       <c r="AN53" s="3"/>
     </row>
-    <row r="54" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A54" s="2"/>
+    <row r="54" spans="1:42" ht="105" x14ac:dyDescent="0.25">
+      <c r="A54" s="2" t="s">
+        <v>373</v>
+      </c>
       <c r="B54" s="2"/>
-      <c r="C54" s="2"/>
-      <c r="D54" s="2"/>
-      <c r="E54" s="2"/>
-      <c r="F54" s="2"/>
-      <c r="G54" s="2"/>
-      <c r="H54" s="2"/>
-      <c r="I54" s="2"/>
-      <c r="J54" s="2"/>
-      <c r="K54" s="2"/>
-      <c r="L54" s="2"/>
-      <c r="M54" s="16"/>
-      <c r="N54" s="16"/>
-      <c r="O54" s="16"/>
-      <c r="P54" s="16"/>
-      <c r="Q54" s="16"/>
-      <c r="R54" s="16"/>
-      <c r="S54" s="16"/>
-      <c r="T54" s="16"/>
-      <c r="U54" s="16"/>
-      <c r="V54" s="16"/>
+      <c r="C54" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="D54" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="E54" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="F54" s="26" t="s">
+        <v>35</v>
+      </c>
+      <c r="G54" s="20" t="s">
+        <v>36</v>
+      </c>
+      <c r="H54" s="47" t="s">
+        <v>321</v>
+      </c>
+      <c r="I54" s="6" t="s">
+        <v>368</v>
+      </c>
+      <c r="J54" s="6" t="s">
+        <v>369</v>
+      </c>
+      <c r="K54" s="13" t="s">
+        <v>371</v>
+      </c>
+      <c r="L54" s="49" t="s">
+        <v>325</v>
+      </c>
+      <c r="M54" s="25" t="s">
+        <v>326</v>
+      </c>
+      <c r="N54" s="23" t="s">
+        <v>327</v>
+      </c>
+      <c r="O54" s="23" t="s">
+        <v>328</v>
+      </c>
+      <c r="P54" s="21" t="s">
+        <v>329</v>
+      </c>
+      <c r="Q54" s="21" t="s">
+        <v>330</v>
+      </c>
+      <c r="R54" s="21" t="s">
+        <v>331</v>
+      </c>
+      <c r="S54" s="21" t="s">
+        <v>332</v>
+      </c>
+      <c r="T54" s="16" t="s">
+        <v>334</v>
+      </c>
+      <c r="U54" s="16" t="s">
+        <v>335</v>
+      </c>
+      <c r="V54" s="16" t="s">
+        <v>336</v>
+      </c>
       <c r="W54" s="16"/>
       <c r="X54" s="16"/>
       <c r="Y54" s="16"/>
@@ -7194,28 +7556,68 @@
       <c r="AM54" s="3"/>
       <c r="AN54" s="3"/>
     </row>
-    <row r="55" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A55" s="2"/>
+    <row r="55" spans="1:42" ht="180" x14ac:dyDescent="0.25">
+      <c r="A55" s="2" t="s">
+        <v>386</v>
+      </c>
       <c r="B55" s="2"/>
-      <c r="C55" s="2"/>
-      <c r="D55" s="2"/>
-      <c r="E55" s="2"/>
-      <c r="F55" s="2"/>
-      <c r="G55" s="2"/>
-      <c r="H55" s="2"/>
-      <c r="I55" s="2"/>
-      <c r="J55" s="2"/>
-      <c r="K55" s="2"/>
-      <c r="L55" s="2"/>
-      <c r="M55" s="16"/>
-      <c r="N55" s="16"/>
-      <c r="O55" s="16"/>
-      <c r="P55" s="16"/>
-      <c r="Q55" s="16"/>
-      <c r="R55" s="16"/>
-      <c r="S55" s="16"/>
-      <c r="T55" s="16"/>
-      <c r="U55" s="16"/>
+      <c r="C55" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="D55" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="E55" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="F55" s="26" t="s">
+        <v>35</v>
+      </c>
+      <c r="G55" s="20" t="s">
+        <v>36</v>
+      </c>
+      <c r="H55" s="47" t="s">
+        <v>321</v>
+      </c>
+      <c r="I55" s="2" t="s">
+        <v>322</v>
+      </c>
+      <c r="J55" s="2" t="s">
+        <v>374</v>
+      </c>
+      <c r="K55" s="6" t="s">
+        <v>375</v>
+      </c>
+      <c r="L55" s="6" t="s">
+        <v>376</v>
+      </c>
+      <c r="M55" s="7" t="s">
+        <v>377</v>
+      </c>
+      <c r="N55" s="16" t="s">
+        <v>378</v>
+      </c>
+      <c r="O55" s="16" t="s">
+        <v>379</v>
+      </c>
+      <c r="P55" s="16" t="s">
+        <v>380</v>
+      </c>
+      <c r="Q55" s="7" t="s">
+        <v>381</v>
+      </c>
+      <c r="R55" s="7" t="s">
+        <v>382</v>
+      </c>
+      <c r="S55" s="7" t="s">
+        <v>383</v>
+      </c>
+      <c r="T55" s="7" t="s">
+        <v>384</v>
+      </c>
+      <c r="U55" s="16" t="s">
+        <v>385</v>
+      </c>
       <c r="V55" s="16"/>
       <c r="W55" s="16"/>
       <c r="X55" s="16"/>
@@ -7236,28 +7638,68 @@
       <c r="AM55" s="3"/>
       <c r="AN55" s="3"/>
     </row>
-    <row r="56" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A56" s="2"/>
+    <row r="56" spans="1:42" ht="180" x14ac:dyDescent="0.25">
+      <c r="A56" s="2" t="s">
+        <v>391</v>
+      </c>
       <c r="B56" s="2"/>
-      <c r="C56" s="2"/>
-      <c r="D56" s="2"/>
-      <c r="E56" s="2"/>
-      <c r="F56" s="2"/>
-      <c r="G56" s="2"/>
-      <c r="H56" s="2"/>
-      <c r="I56" s="2"/>
-      <c r="J56" s="2"/>
-      <c r="K56" s="2"/>
-      <c r="L56" s="2"/>
-      <c r="M56" s="16"/>
-      <c r="N56" s="16"/>
-      <c r="O56" s="16"/>
-      <c r="P56" s="16"/>
-      <c r="Q56" s="16"/>
-      <c r="R56" s="16"/>
-      <c r="S56" s="16"/>
-      <c r="T56" s="16"/>
-      <c r="U56" s="16"/>
+      <c r="C56" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="D56" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="E56" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="F56" s="26" t="s">
+        <v>35</v>
+      </c>
+      <c r="G56" s="20" t="s">
+        <v>36</v>
+      </c>
+      <c r="H56" s="47" t="s">
+        <v>321</v>
+      </c>
+      <c r="I56" s="2" t="s">
+        <v>340</v>
+      </c>
+      <c r="J56" s="2" t="s">
+        <v>387</v>
+      </c>
+      <c r="K56" s="6" t="s">
+        <v>375</v>
+      </c>
+      <c r="L56" s="6" t="s">
+        <v>376</v>
+      </c>
+      <c r="M56" s="7" t="s">
+        <v>377</v>
+      </c>
+      <c r="N56" s="16" t="s">
+        <v>388</v>
+      </c>
+      <c r="O56" s="16" t="s">
+        <v>379</v>
+      </c>
+      <c r="P56" s="16" t="s">
+        <v>389</v>
+      </c>
+      <c r="Q56" s="7" t="s">
+        <v>381</v>
+      </c>
+      <c r="R56" s="7" t="s">
+        <v>382</v>
+      </c>
+      <c r="S56" s="7" t="s">
+        <v>383</v>
+      </c>
+      <c r="T56" s="7" t="s">
+        <v>384</v>
+      </c>
+      <c r="U56" s="16" t="s">
+        <v>390</v>
+      </c>
       <c r="V56" s="16"/>
       <c r="W56" s="16"/>
       <c r="X56" s="16"/>
@@ -7278,28 +7720,68 @@
       <c r="AM56" s="3"/>
       <c r="AN56" s="3"/>
     </row>
-    <row r="57" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A57" s="2"/>
+    <row r="57" spans="1:42" ht="180" x14ac:dyDescent="0.25">
+      <c r="A57" s="2" t="s">
+        <v>395</v>
+      </c>
       <c r="B57" s="2"/>
-      <c r="C57" s="2"/>
-      <c r="D57" s="2"/>
-      <c r="E57" s="2"/>
-      <c r="F57" s="2"/>
-      <c r="G57" s="2"/>
-      <c r="H57" s="2"/>
-      <c r="I57" s="2"/>
-      <c r="J57" s="2"/>
-      <c r="K57" s="2"/>
-      <c r="L57" s="2"/>
-      <c r="M57" s="16"/>
-      <c r="N57" s="16"/>
-      <c r="O57" s="16"/>
-      <c r="P57" s="16"/>
-      <c r="Q57" s="16"/>
-      <c r="R57" s="16"/>
-      <c r="S57" s="16"/>
-      <c r="T57" s="16"/>
-      <c r="U57" s="16"/>
+      <c r="C57" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="D57" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="E57" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="F57" s="26" t="s">
+        <v>35</v>
+      </c>
+      <c r="G57" s="20" t="s">
+        <v>36</v>
+      </c>
+      <c r="H57" s="47" t="s">
+        <v>321</v>
+      </c>
+      <c r="I57" s="2" t="s">
+        <v>345</v>
+      </c>
+      <c r="J57" s="2" t="s">
+        <v>392</v>
+      </c>
+      <c r="K57" s="6" t="s">
+        <v>375</v>
+      </c>
+      <c r="L57" s="6" t="s">
+        <v>376</v>
+      </c>
+      <c r="M57" s="7" t="s">
+        <v>377</v>
+      </c>
+      <c r="N57" s="16" t="s">
+        <v>378</v>
+      </c>
+      <c r="O57" s="16" t="s">
+        <v>379</v>
+      </c>
+      <c r="P57" s="16" t="s">
+        <v>393</v>
+      </c>
+      <c r="Q57" s="7" t="s">
+        <v>381</v>
+      </c>
+      <c r="R57" s="7" t="s">
+        <v>382</v>
+      </c>
+      <c r="S57" s="7" t="s">
+        <v>383</v>
+      </c>
+      <c r="T57" s="7" t="s">
+        <v>384</v>
+      </c>
+      <c r="U57" s="16" t="s">
+        <v>394</v>
+      </c>
       <c r="V57" s="16"/>
       <c r="W57" s="16"/>
       <c r="X57" s="16"/>
@@ -7320,28 +7802,68 @@
       <c r="AM57" s="3"/>
       <c r="AN57" s="3"/>
     </row>
-    <row r="58" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A58" s="2"/>
+    <row r="58" spans="1:42" ht="180" x14ac:dyDescent="0.25">
+      <c r="A58" s="2" t="s">
+        <v>398</v>
+      </c>
       <c r="B58" s="2"/>
-      <c r="C58" s="2"/>
-      <c r="D58" s="2"/>
-      <c r="E58" s="2"/>
-      <c r="F58" s="2"/>
-      <c r="G58" s="2"/>
-      <c r="H58" s="2"/>
-      <c r="I58" s="2"/>
-      <c r="J58" s="2"/>
-      <c r="K58" s="2"/>
-      <c r="L58" s="2"/>
-      <c r="M58" s="16"/>
-      <c r="N58" s="16"/>
-      <c r="O58" s="16"/>
-      <c r="P58" s="16"/>
-      <c r="Q58" s="16"/>
-      <c r="R58" s="16"/>
-      <c r="S58" s="16"/>
-      <c r="T58" s="16"/>
-      <c r="U58" s="16"/>
+      <c r="C58" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="D58" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="E58" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="F58" s="26" t="s">
+        <v>35</v>
+      </c>
+      <c r="G58" s="20" t="s">
+        <v>36</v>
+      </c>
+      <c r="H58" s="47" t="s">
+        <v>321</v>
+      </c>
+      <c r="I58" s="2" t="s">
+        <v>350</v>
+      </c>
+      <c r="J58" s="2" t="s">
+        <v>396</v>
+      </c>
+      <c r="K58" s="6" t="s">
+        <v>375</v>
+      </c>
+      <c r="L58" s="6" t="s">
+        <v>376</v>
+      </c>
+      <c r="M58" s="7" t="s">
+        <v>377</v>
+      </c>
+      <c r="N58" s="16" t="s">
+        <v>388</v>
+      </c>
+      <c r="O58" s="16" t="s">
+        <v>379</v>
+      </c>
+      <c r="P58" s="16" t="s">
+        <v>397</v>
+      </c>
+      <c r="Q58" s="7" t="s">
+        <v>381</v>
+      </c>
+      <c r="R58" s="7" t="s">
+        <v>382</v>
+      </c>
+      <c r="S58" s="7" t="s">
+        <v>383</v>
+      </c>
+      <c r="T58" s="7" t="s">
+        <v>384</v>
+      </c>
+      <c r="U58" s="16" t="s">
+        <v>390</v>
+      </c>
       <c r="V58" s="16"/>
       <c r="W58" s="16"/>
       <c r="X58" s="16"/>
@@ -7351,28 +7873,68 @@
       <c r="AB58" s="16"/>
       <c r="AC58" s="4"/>
     </row>
-    <row r="59" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A59" s="2"/>
+    <row r="59" spans="1:42" ht="180" x14ac:dyDescent="0.25">
+      <c r="A59" s="2" t="s">
+        <v>401</v>
+      </c>
       <c r="B59" s="2"/>
-      <c r="C59" s="2"/>
-      <c r="D59" s="2"/>
-      <c r="E59" s="2"/>
-      <c r="F59" s="2"/>
-      <c r="G59" s="2"/>
-      <c r="H59" s="2"/>
-      <c r="I59" s="2"/>
-      <c r="J59" s="2"/>
-      <c r="K59" s="2"/>
-      <c r="L59" s="2"/>
-      <c r="M59" s="16"/>
-      <c r="N59" s="16"/>
-      <c r="O59" s="16"/>
-      <c r="P59" s="16"/>
-      <c r="Q59" s="16"/>
-      <c r="R59" s="16"/>
-      <c r="S59" s="16"/>
-      <c r="T59" s="16"/>
-      <c r="U59" s="16"/>
+      <c r="C59" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="D59" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="E59" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="F59" s="26" t="s">
+        <v>35</v>
+      </c>
+      <c r="G59" s="20" t="s">
+        <v>36</v>
+      </c>
+      <c r="H59" s="47" t="s">
+        <v>321</v>
+      </c>
+      <c r="I59" s="2" t="s">
+        <v>355</v>
+      </c>
+      <c r="J59" s="2" t="s">
+        <v>399</v>
+      </c>
+      <c r="K59" s="6" t="s">
+        <v>375</v>
+      </c>
+      <c r="L59" s="6" t="s">
+        <v>376</v>
+      </c>
+      <c r="M59" s="7" t="s">
+        <v>377</v>
+      </c>
+      <c r="N59" s="16" t="s">
+        <v>378</v>
+      </c>
+      <c r="O59" s="16" t="s">
+        <v>379</v>
+      </c>
+      <c r="P59" s="16" t="s">
+        <v>400</v>
+      </c>
+      <c r="Q59" s="7" t="s">
+        <v>381</v>
+      </c>
+      <c r="R59" s="7" t="s">
+        <v>382</v>
+      </c>
+      <c r="S59" s="7" t="s">
+        <v>383</v>
+      </c>
+      <c r="T59" s="7" t="s">
+        <v>384</v>
+      </c>
+      <c r="U59" s="16" t="s">
+        <v>394</v>
+      </c>
       <c r="V59" s="16"/>
       <c r="W59" s="16"/>
       <c r="X59" s="16"/>
@@ -7382,28 +7944,68 @@
       <c r="AB59" s="16"/>
       <c r="AC59" s="4"/>
     </row>
-    <row r="60" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A60" s="2"/>
+    <row r="60" spans="1:42" ht="180" x14ac:dyDescent="0.25">
+      <c r="A60" s="2" t="s">
+        <v>404</v>
+      </c>
       <c r="B60" s="2"/>
-      <c r="C60" s="2"/>
-      <c r="D60" s="2"/>
-      <c r="E60" s="2"/>
-      <c r="F60" s="2"/>
-      <c r="G60" s="2"/>
-      <c r="H60" s="2"/>
-      <c r="I60" s="2"/>
-      <c r="J60" s="2"/>
-      <c r="K60" s="2"/>
-      <c r="L60" s="2"/>
-      <c r="M60" s="16"/>
-      <c r="N60" s="16"/>
-      <c r="O60" s="16"/>
-      <c r="P60" s="16"/>
-      <c r="Q60" s="16"/>
-      <c r="R60" s="16"/>
-      <c r="S60" s="16"/>
-      <c r="T60" s="16"/>
-      <c r="U60" s="16"/>
+      <c r="C60" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="D60" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="E60" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="F60" s="26" t="s">
+        <v>35</v>
+      </c>
+      <c r="G60" s="20" t="s">
+        <v>36</v>
+      </c>
+      <c r="H60" s="47" t="s">
+        <v>321</v>
+      </c>
+      <c r="I60" s="2" t="s">
+        <v>402</v>
+      </c>
+      <c r="J60" s="2" t="s">
+        <v>403</v>
+      </c>
+      <c r="K60" s="6" t="s">
+        <v>375</v>
+      </c>
+      <c r="L60" s="6" t="s">
+        <v>376</v>
+      </c>
+      <c r="M60" s="7" t="s">
+        <v>377</v>
+      </c>
+      <c r="N60" s="16" t="s">
+        <v>388</v>
+      </c>
+      <c r="O60" s="16" t="s">
+        <v>379</v>
+      </c>
+      <c r="P60" s="16" t="s">
+        <v>380</v>
+      </c>
+      <c r="Q60" s="7" t="s">
+        <v>381</v>
+      </c>
+      <c r="R60" s="7" t="s">
+        <v>382</v>
+      </c>
+      <c r="S60" s="7" t="s">
+        <v>383</v>
+      </c>
+      <c r="T60" s="7" t="s">
+        <v>384</v>
+      </c>
+      <c r="U60" s="16" t="s">
+        <v>390</v>
+      </c>
       <c r="V60" s="16"/>
       <c r="W60" s="16"/>
       <c r="X60" s="16"/>
@@ -7413,28 +8015,68 @@
       <c r="AB60" s="16"/>
       <c r="AC60" s="4"/>
     </row>
-    <row r="61" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A61" s="2"/>
+    <row r="61" spans="1:42" ht="180" x14ac:dyDescent="0.25">
+      <c r="A61" s="2" t="s">
+        <v>405</v>
+      </c>
       <c r="B61" s="2"/>
-      <c r="C61" s="2"/>
-      <c r="D61" s="2"/>
-      <c r="E61" s="2"/>
-      <c r="F61" s="2"/>
-      <c r="G61" s="2"/>
-      <c r="H61" s="2"/>
-      <c r="I61" s="2"/>
-      <c r="J61" s="2"/>
-      <c r="K61" s="2"/>
-      <c r="L61" s="2"/>
-      <c r="M61" s="16"/>
-      <c r="N61" s="16"/>
-      <c r="O61" s="16"/>
-      <c r="P61" s="16"/>
-      <c r="Q61" s="16"/>
-      <c r="R61" s="16"/>
-      <c r="S61" s="16"/>
-      <c r="T61" s="16"/>
-      <c r="U61" s="16"/>
+      <c r="C61" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="D61" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="E61" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="F61" s="26" t="s">
+        <v>35</v>
+      </c>
+      <c r="G61" s="20" t="s">
+        <v>36</v>
+      </c>
+      <c r="H61" s="47" t="s">
+        <v>321</v>
+      </c>
+      <c r="I61" s="2" t="s">
+        <v>364</v>
+      </c>
+      <c r="J61" s="2" t="s">
+        <v>370</v>
+      </c>
+      <c r="K61" s="6" t="s">
+        <v>375</v>
+      </c>
+      <c r="L61" s="6" t="s">
+        <v>376</v>
+      </c>
+      <c r="M61" s="7" t="s">
+        <v>377</v>
+      </c>
+      <c r="N61" s="16" t="s">
+        <v>388</v>
+      </c>
+      <c r="O61" s="16" t="s">
+        <v>379</v>
+      </c>
+      <c r="P61" s="16" t="s">
+        <v>389</v>
+      </c>
+      <c r="Q61" s="7" t="s">
+        <v>381</v>
+      </c>
+      <c r="R61" s="7" t="s">
+        <v>382</v>
+      </c>
+      <c r="S61" s="7" t="s">
+        <v>383</v>
+      </c>
+      <c r="T61" s="7" t="s">
+        <v>384</v>
+      </c>
+      <c r="U61" s="16" t="s">
+        <v>394</v>
+      </c>
       <c r="V61" s="16"/>
       <c r="W61" s="16"/>
       <c r="X61" s="16"/>
@@ -7444,28 +8086,68 @@
       <c r="AB61" s="16"/>
       <c r="AC61" s="4"/>
     </row>
-    <row r="62" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A62" s="2"/>
+    <row r="62" spans="1:42" ht="180" x14ac:dyDescent="0.25">
+      <c r="A62" s="2" t="s">
+        <v>406</v>
+      </c>
       <c r="B62" s="2"/>
-      <c r="C62" s="2"/>
-      <c r="D62" s="2"/>
-      <c r="E62" s="2"/>
-      <c r="F62" s="2"/>
-      <c r="G62" s="2"/>
-      <c r="H62" s="2"/>
-      <c r="I62" s="2"/>
-      <c r="J62" s="2"/>
-      <c r="K62" s="2"/>
-      <c r="L62" s="2"/>
-      <c r="M62" s="16"/>
-      <c r="N62" s="16"/>
-      <c r="O62" s="16"/>
-      <c r="P62" s="16"/>
-      <c r="Q62" s="16"/>
-      <c r="R62" s="16"/>
-      <c r="S62" s="16"/>
-      <c r="T62" s="16"/>
-      <c r="U62" s="16"/>
+      <c r="C62" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="D62" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="E62" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="F62" s="26" t="s">
+        <v>35</v>
+      </c>
+      <c r="G62" s="20" t="s">
+        <v>36</v>
+      </c>
+      <c r="H62" s="47" t="s">
+        <v>321</v>
+      </c>
+      <c r="I62" s="2" t="s">
+        <v>368</v>
+      </c>
+      <c r="J62" s="2" t="s">
+        <v>369</v>
+      </c>
+      <c r="K62" s="6" t="s">
+        <v>375</v>
+      </c>
+      <c r="L62" s="6" t="s">
+        <v>376</v>
+      </c>
+      <c r="M62" s="7" t="s">
+        <v>377</v>
+      </c>
+      <c r="N62" s="16" t="s">
+        <v>388</v>
+      </c>
+      <c r="O62" s="16" t="s">
+        <v>379</v>
+      </c>
+      <c r="P62" s="16" t="s">
+        <v>393</v>
+      </c>
+      <c r="Q62" s="7" t="s">
+        <v>381</v>
+      </c>
+      <c r="R62" s="7" t="s">
+        <v>382</v>
+      </c>
+      <c r="S62" s="7" t="s">
+        <v>383</v>
+      </c>
+      <c r="T62" s="7" t="s">
+        <v>384</v>
+      </c>
+      <c r="U62" s="16" t="s">
+        <v>394</v>
+      </c>
       <c r="V62" s="16"/>
       <c r="W62" s="16"/>
       <c r="X62" s="16"/>
@@ -7475,58 +8157,189 @@
       <c r="AB62" s="16"/>
       <c r="AC62" s="4"/>
     </row>
-    <row r="63" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A63" s="2"/>
+    <row r="63" spans="1:42" ht="150" x14ac:dyDescent="0.25">
+      <c r="A63" s="50" t="s">
+        <v>407</v>
+      </c>
       <c r="B63" s="2"/>
-      <c r="C63" s="2"/>
-      <c r="D63" s="2"/>
-      <c r="E63" s="2"/>
-      <c r="F63" s="2"/>
-      <c r="G63" s="2"/>
-      <c r="H63" s="2"/>
-      <c r="I63" s="2"/>
-      <c r="J63" s="2"/>
-      <c r="K63" s="2"/>
-      <c r="L63" s="2"/>
-      <c r="M63" s="16"/>
-      <c r="N63" s="16"/>
-      <c r="O63" s="16"/>
-      <c r="P63" s="16"/>
-      <c r="Q63" s="16"/>
-      <c r="R63" s="16"/>
-      <c r="S63" s="16"/>
-      <c r="T63" s="16"/>
-      <c r="U63" s="16"/>
-      <c r="V63" s="16"/>
-      <c r="W63" s="16"/>
-      <c r="X63" s="16"/>
-      <c r="Y63" s="16"/>
-      <c r="Z63" s="16"/>
-      <c r="AA63" s="16"/>
-      <c r="AB63" s="16"/>
-      <c r="AC63" s="4"/>
-    </row>
-    <row r="64" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="C63" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="D63" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="E63" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="F63" s="26" t="s">
+        <v>35</v>
+      </c>
+      <c r="G63" s="20" t="s">
+        <v>36</v>
+      </c>
+      <c r="H63" s="47" t="s">
+        <v>321</v>
+      </c>
+      <c r="I63" s="2" t="s">
+        <v>322</v>
+      </c>
+      <c r="J63" s="2" t="s">
+        <v>323</v>
+      </c>
+      <c r="K63" s="2" t="s">
+        <v>324</v>
+      </c>
+      <c r="L63" s="2" t="s">
+        <v>408</v>
+      </c>
+      <c r="M63" s="16" t="s">
+        <v>409</v>
+      </c>
+      <c r="N63" s="16" t="s">
+        <v>410</v>
+      </c>
+      <c r="O63" s="16" t="s">
+        <v>411</v>
+      </c>
+      <c r="P63" s="16" t="s">
+        <v>412</v>
+      </c>
+      <c r="Q63" s="16" t="s">
+        <v>413</v>
+      </c>
+      <c r="R63" s="16" t="s">
+        <v>414</v>
+      </c>
+      <c r="S63" s="16" t="s">
+        <v>415</v>
+      </c>
+      <c r="T63" s="16" t="s">
+        <v>416</v>
+      </c>
+      <c r="U63" s="16" t="s">
+        <v>417</v>
+      </c>
+      <c r="V63" s="16" t="s">
+        <v>418</v>
+      </c>
+      <c r="W63" s="16" t="s">
+        <v>419</v>
+      </c>
+      <c r="X63" s="16" t="s">
+        <v>420</v>
+      </c>
+      <c r="Y63" s="16" t="s">
+        <v>421</v>
+      </c>
+      <c r="Z63" s="16" t="s">
+        <v>422</v>
+      </c>
+      <c r="AA63" s="16" t="s">
+        <v>423</v>
+      </c>
+      <c r="AB63" s="16" t="s">
+        <v>424</v>
+      </c>
+      <c r="AC63" s="3" t="s">
+        <v>325</v>
+      </c>
+      <c r="AD63" s="3" t="s">
+        <v>425</v>
+      </c>
+      <c r="AE63" s="3" t="s">
+        <v>426</v>
+      </c>
+      <c r="AF63" s="3" t="s">
+        <v>427</v>
+      </c>
+      <c r="AG63" s="3" t="s">
+        <v>428</v>
+      </c>
+      <c r="AH63" s="3" t="s">
+        <v>429</v>
+      </c>
+      <c r="AI63" s="3" t="s">
+        <v>430</v>
+      </c>
+      <c r="AJ63" s="3" t="s">
+        <v>431</v>
+      </c>
+      <c r="AK63" s="3" t="s">
+        <v>432</v>
+      </c>
+      <c r="AL63" s="3" t="s">
+        <v>325</v>
+      </c>
+      <c r="AM63" s="3" t="s">
+        <v>433</v>
+      </c>
+      <c r="AN63" s="3" t="s">
+        <v>434</v>
+      </c>
+      <c r="AO63" s="3" t="s">
+        <v>435</v>
+      </c>
+      <c r="AP63" s="3" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="64" spans="1:42" ht="150" x14ac:dyDescent="0.25">
       <c r="A64" s="2"/>
       <c r="B64" s="2"/>
-      <c r="C64" s="2"/>
-      <c r="D64" s="2"/>
-      <c r="E64" s="2"/>
-      <c r="F64" s="2"/>
-      <c r="G64" s="2"/>
-      <c r="H64" s="2"/>
-      <c r="I64" s="2"/>
-      <c r="J64" s="2"/>
-      <c r="K64" s="2"/>
-      <c r="L64" s="2"/>
-      <c r="M64" s="16"/>
-      <c r="N64" s="16"/>
-      <c r="O64" s="16"/>
-      <c r="P64" s="16"/>
-      <c r="Q64" s="16"/>
-      <c r="R64" s="16"/>
-      <c r="S64" s="16"/>
-      <c r="T64" s="16"/>
+      <c r="C64" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="D64" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="E64" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="F64" s="26" t="s">
+        <v>35</v>
+      </c>
+      <c r="G64" s="20" t="s">
+        <v>36</v>
+      </c>
+      <c r="H64" s="47" t="s">
+        <v>321</v>
+      </c>
+      <c r="I64" s="2" t="s">
+        <v>340</v>
+      </c>
+      <c r="J64" s="2" t="s">
+        <v>341</v>
+      </c>
+      <c r="K64" s="2" t="s">
+        <v>342</v>
+      </c>
+      <c r="L64" s="2" t="s">
+        <v>343</v>
+      </c>
+      <c r="M64" s="16" t="s">
+        <v>437</v>
+      </c>
+      <c r="N64" s="16" t="s">
+        <v>438</v>
+      </c>
+      <c r="O64" s="16" t="s">
+        <v>439</v>
+      </c>
+      <c r="P64" s="16" t="s">
+        <v>440</v>
+      </c>
+      <c r="Q64" s="16" t="s">
+        <v>441</v>
+      </c>
+      <c r="R64" s="16" t="s">
+        <v>442</v>
+      </c>
+      <c r="S64" s="16" t="s">
+        <v>443</v>
+      </c>
+      <c r="T64" s="16" t="s">
+        <v>444</v>
+      </c>
       <c r="U64" s="16"/>
       <c r="V64" s="16"/>
       <c r="W64" s="16"/>
@@ -7535,9 +8348,22 @@
       <c r="Z64" s="16"/>
       <c r="AA64" s="16"/>
       <c r="AB64" s="16"/>
-      <c r="AC64" s="4"/>
-    </row>
-    <row r="65" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="AC64" s="3"/>
+      <c r="AD64" s="3"/>
+      <c r="AE64" s="3"/>
+      <c r="AF64" s="3"/>
+      <c r="AG64" s="3"/>
+      <c r="AH64" s="3"/>
+      <c r="AI64" s="3"/>
+      <c r="AJ64" s="3"/>
+      <c r="AK64" s="3"/>
+      <c r="AL64" s="3"/>
+      <c r="AM64" s="3"/>
+      <c r="AN64" s="3"/>
+      <c r="AO64" s="3"/>
+      <c r="AP64" s="3"/>
+    </row>
+    <row r="65" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A65" s="2"/>
       <c r="B65" s="2"/>
       <c r="C65" s="2"/>
@@ -7566,9 +8392,22 @@
       <c r="Z65" s="16"/>
       <c r="AA65" s="16"/>
       <c r="AB65" s="16"/>
-      <c r="AC65" s="4"/>
-    </row>
-    <row r="66" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="AC65" s="3"/>
+      <c r="AD65" s="3"/>
+      <c r="AE65" s="3"/>
+      <c r="AF65" s="3"/>
+      <c r="AG65" s="3"/>
+      <c r="AH65" s="3"/>
+      <c r="AI65" s="3"/>
+      <c r="AJ65" s="3"/>
+      <c r="AK65" s="3"/>
+      <c r="AL65" s="3"/>
+      <c r="AM65" s="3"/>
+      <c r="AN65" s="3"/>
+      <c r="AO65" s="3"/>
+      <c r="AP65" s="3"/>
+    </row>
+    <row r="66" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A66" s="2"/>
       <c r="B66" s="2"/>
       <c r="C66" s="2"/>
@@ -7597,9 +8436,22 @@
       <c r="Z66" s="16"/>
       <c r="AA66" s="16"/>
       <c r="AB66" s="16"/>
-      <c r="AC66" s="4"/>
-    </row>
-    <row r="67" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="AC66" s="3"/>
+      <c r="AD66" s="3"/>
+      <c r="AE66" s="3"/>
+      <c r="AF66" s="3"/>
+      <c r="AG66" s="3"/>
+      <c r="AH66" s="3"/>
+      <c r="AI66" s="3"/>
+      <c r="AJ66" s="3"/>
+      <c r="AK66" s="3"/>
+      <c r="AL66" s="3"/>
+      <c r="AM66" s="3"/>
+      <c r="AN66" s="3"/>
+      <c r="AO66" s="3"/>
+      <c r="AP66" s="3"/>
+    </row>
+    <row r="67" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A67" s="2"/>
       <c r="B67" s="2"/>
       <c r="C67" s="2"/>
@@ -7628,9 +8480,22 @@
       <c r="Z67" s="16"/>
       <c r="AA67" s="16"/>
       <c r="AB67" s="16"/>
-      <c r="AC67" s="4"/>
-    </row>
-    <row r="68" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="AC67" s="3"/>
+      <c r="AD67" s="3"/>
+      <c r="AE67" s="3"/>
+      <c r="AF67" s="3"/>
+      <c r="AG67" s="3"/>
+      <c r="AH67" s="3"/>
+      <c r="AI67" s="3"/>
+      <c r="AJ67" s="3"/>
+      <c r="AK67" s="3"/>
+      <c r="AL67" s="3"/>
+      <c r="AM67" s="3"/>
+      <c r="AN67" s="3"/>
+      <c r="AO67" s="3"/>
+      <c r="AP67" s="3"/>
+    </row>
+    <row r="68" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A68" s="2"/>
       <c r="B68" s="2"/>
       <c r="C68" s="2"/>
@@ -7659,9 +8524,22 @@
       <c r="Z68" s="16"/>
       <c r="AA68" s="16"/>
       <c r="AB68" s="16"/>
-      <c r="AC68" s="4"/>
-    </row>
-    <row r="69" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="AC68" s="3"/>
+      <c r="AD68" s="3"/>
+      <c r="AE68" s="3"/>
+      <c r="AF68" s="3"/>
+      <c r="AG68" s="3"/>
+      <c r="AH68" s="3"/>
+      <c r="AI68" s="3"/>
+      <c r="AJ68" s="3"/>
+      <c r="AK68" s="3"/>
+      <c r="AL68" s="3"/>
+      <c r="AM68" s="3"/>
+      <c r="AN68" s="3"/>
+      <c r="AO68" s="3"/>
+      <c r="AP68" s="3"/>
+    </row>
+    <row r="69" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A69" s="2"/>
       <c r="B69" s="2"/>
       <c r="C69" s="2"/>
@@ -7690,9 +8568,22 @@
       <c r="Z69" s="16"/>
       <c r="AA69" s="16"/>
       <c r="AB69" s="16"/>
-      <c r="AC69" s="4"/>
-    </row>
-    <row r="70" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="AC69" s="3"/>
+      <c r="AD69" s="3"/>
+      <c r="AE69" s="3"/>
+      <c r="AF69" s="3"/>
+      <c r="AG69" s="3"/>
+      <c r="AH69" s="3"/>
+      <c r="AI69" s="3"/>
+      <c r="AJ69" s="3"/>
+      <c r="AK69" s="3"/>
+      <c r="AL69" s="3"/>
+      <c r="AM69" s="3"/>
+      <c r="AN69" s="3"/>
+      <c r="AO69" s="3"/>
+      <c r="AP69" s="3"/>
+    </row>
+    <row r="70" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A70" s="2"/>
       <c r="B70" s="2"/>
       <c r="C70" s="2"/>
@@ -7721,9 +8612,22 @@
       <c r="Z70" s="16"/>
       <c r="AA70" s="16"/>
       <c r="AB70" s="16"/>
-      <c r="AC70" s="4"/>
-    </row>
-    <row r="71" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="AC70" s="3"/>
+      <c r="AD70" s="3"/>
+      <c r="AE70" s="3"/>
+      <c r="AF70" s="3"/>
+      <c r="AG70" s="3"/>
+      <c r="AH70" s="3"/>
+      <c r="AI70" s="3"/>
+      <c r="AJ70" s="3"/>
+      <c r="AK70" s="3"/>
+      <c r="AL70" s="3"/>
+      <c r="AM70" s="3"/>
+      <c r="AN70" s="3"/>
+      <c r="AO70" s="3"/>
+      <c r="AP70" s="3"/>
+    </row>
+    <row r="71" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A71" s="2"/>
       <c r="B71" s="2"/>
       <c r="C71" s="2"/>
@@ -7752,9 +8656,22 @@
       <c r="Z71" s="16"/>
       <c r="AA71" s="16"/>
       <c r="AB71" s="16"/>
-      <c r="AC71" s="4"/>
-    </row>
-    <row r="72" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="AC71" s="3"/>
+      <c r="AD71" s="3"/>
+      <c r="AE71" s="3"/>
+      <c r="AF71" s="3"/>
+      <c r="AG71" s="3"/>
+      <c r="AH71" s="3"/>
+      <c r="AI71" s="3"/>
+      <c r="AJ71" s="3"/>
+      <c r="AK71" s="3"/>
+      <c r="AL71" s="3"/>
+      <c r="AM71" s="3"/>
+      <c r="AN71" s="3"/>
+      <c r="AO71" s="3"/>
+      <c r="AP71" s="3"/>
+    </row>
+    <row r="72" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A72" s="2"/>
       <c r="B72" s="2"/>
       <c r="C72" s="2"/>
@@ -7783,8 +8700,22 @@
       <c r="Z72" s="16"/>
       <c r="AA72" s="16"/>
       <c r="AB72" s="16"/>
-    </row>
-    <row r="73" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="AC72" s="5"/>
+      <c r="AD72" s="3"/>
+      <c r="AE72" s="3"/>
+      <c r="AF72" s="3"/>
+      <c r="AG72" s="3"/>
+      <c r="AH72" s="3"/>
+      <c r="AI72" s="3"/>
+      <c r="AJ72" s="3"/>
+      <c r="AK72" s="3"/>
+      <c r="AL72" s="3"/>
+      <c r="AM72" s="3"/>
+      <c r="AN72" s="3"/>
+      <c r="AO72" s="3"/>
+      <c r="AP72" s="3"/>
+    </row>
+    <row r="73" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A73" s="2"/>
       <c r="B73" s="2"/>
       <c r="C73" s="2"/>
@@ -7813,8 +8744,22 @@
       <c r="Z73" s="16"/>
       <c r="AA73" s="16"/>
       <c r="AB73" s="16"/>
-    </row>
-    <row r="74" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="AC73" s="5"/>
+      <c r="AD73" s="3"/>
+      <c r="AE73" s="3"/>
+      <c r="AF73" s="3"/>
+      <c r="AG73" s="3"/>
+      <c r="AH73" s="3"/>
+      <c r="AI73" s="3"/>
+      <c r="AJ73" s="3"/>
+      <c r="AK73" s="3"/>
+      <c r="AL73" s="3"/>
+      <c r="AM73" s="3"/>
+      <c r="AN73" s="3"/>
+      <c r="AO73" s="3"/>
+      <c r="AP73" s="3"/>
+    </row>
+    <row r="74" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A74" s="2"/>
       <c r="B74" s="2"/>
       <c r="C74" s="2"/>
@@ -7828,8 +8773,22 @@
       <c r="K74" s="2"/>
       <c r="L74" s="2"/>
       <c r="N74" s="5"/>
-    </row>
-    <row r="75" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="AC74" s="5"/>
+      <c r="AD74" s="3"/>
+      <c r="AE74" s="3"/>
+      <c r="AF74" s="3"/>
+      <c r="AG74" s="3"/>
+      <c r="AH74" s="3"/>
+      <c r="AI74" s="3"/>
+      <c r="AJ74" s="3"/>
+      <c r="AK74" s="3"/>
+      <c r="AL74" s="3"/>
+      <c r="AM74" s="3"/>
+      <c r="AN74" s="3"/>
+      <c r="AO74" s="3"/>
+      <c r="AP74" s="3"/>
+    </row>
+    <row r="75" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A75" s="2"/>
       <c r="B75" s="2"/>
       <c r="C75" s="2"/>
@@ -7843,8 +8802,22 @@
       <c r="K75" s="2"/>
       <c r="L75" s="2"/>
       <c r="N75" s="5"/>
-    </row>
-    <row r="76" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="AC75" s="5"/>
+      <c r="AD75" s="3"/>
+      <c r="AE75" s="3"/>
+      <c r="AF75" s="3"/>
+      <c r="AG75" s="3"/>
+      <c r="AH75" s="3"/>
+      <c r="AI75" s="3"/>
+      <c r="AJ75" s="3"/>
+      <c r="AK75" s="3"/>
+      <c r="AL75" s="3"/>
+      <c r="AM75" s="3"/>
+      <c r="AN75" s="3"/>
+      <c r="AO75" s="3"/>
+      <c r="AP75" s="3"/>
+    </row>
+    <row r="76" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A76" s="2"/>
       <c r="B76" s="2"/>
       <c r="C76" s="2"/>
@@ -7858,8 +8831,22 @@
       <c r="K76" s="2"/>
       <c r="L76" s="2"/>
       <c r="N76" s="5"/>
-    </row>
-    <row r="77" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="AC76" s="5"/>
+      <c r="AD76" s="3"/>
+      <c r="AE76" s="3"/>
+      <c r="AF76" s="3"/>
+      <c r="AG76" s="3"/>
+      <c r="AH76" s="3"/>
+      <c r="AI76" s="3"/>
+      <c r="AJ76" s="3"/>
+      <c r="AK76" s="3"/>
+      <c r="AL76" s="3"/>
+      <c r="AM76" s="3"/>
+      <c r="AN76" s="3"/>
+      <c r="AO76" s="3"/>
+      <c r="AP76" s="3"/>
+    </row>
+    <row r="77" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A77" s="2"/>
       <c r="B77" s="2"/>
       <c r="C77" s="2"/>
@@ -7873,8 +8860,22 @@
       <c r="K77" s="2"/>
       <c r="L77" s="2"/>
       <c r="N77" s="5"/>
-    </row>
-    <row r="78" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="AC77" s="5"/>
+      <c r="AD77" s="3"/>
+      <c r="AE77" s="3"/>
+      <c r="AF77" s="3"/>
+      <c r="AG77" s="3"/>
+      <c r="AH77" s="3"/>
+      <c r="AI77" s="3"/>
+      <c r="AJ77" s="3"/>
+      <c r="AK77" s="3"/>
+      <c r="AL77" s="3"/>
+      <c r="AM77" s="3"/>
+      <c r="AN77" s="3"/>
+      <c r="AO77" s="3"/>
+      <c r="AP77" s="3"/>
+    </row>
+    <row r="78" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A78" s="2"/>
       <c r="B78" s="2"/>
       <c r="C78" s="2"/>
@@ -7888,8 +8889,22 @@
       <c r="K78" s="2"/>
       <c r="L78" s="2"/>
       <c r="N78" s="5"/>
-    </row>
-    <row r="79" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="AC78" s="5"/>
+      <c r="AD78" s="3"/>
+      <c r="AE78" s="3"/>
+      <c r="AF78" s="3"/>
+      <c r="AG78" s="3"/>
+      <c r="AH78" s="3"/>
+      <c r="AI78" s="3"/>
+      <c r="AJ78" s="3"/>
+      <c r="AK78" s="3"/>
+      <c r="AL78" s="3"/>
+      <c r="AM78" s="3"/>
+      <c r="AN78" s="3"/>
+      <c r="AO78" s="3"/>
+      <c r="AP78" s="3"/>
+    </row>
+    <row r="79" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A79" s="2"/>
       <c r="B79" s="2"/>
       <c r="C79" s="2"/>
@@ -7902,8 +8917,22 @@
       <c r="J79" s="2"/>
       <c r="K79" s="2"/>
       <c r="L79" s="2"/>
-    </row>
-    <row r="80" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="AC79" s="5"/>
+      <c r="AD79" s="3"/>
+      <c r="AE79" s="3"/>
+      <c r="AF79" s="3"/>
+      <c r="AG79" s="3"/>
+      <c r="AH79" s="3"/>
+      <c r="AI79" s="3"/>
+      <c r="AJ79" s="3"/>
+      <c r="AK79" s="3"/>
+      <c r="AL79" s="3"/>
+      <c r="AM79" s="3"/>
+      <c r="AN79" s="3"/>
+      <c r="AO79" s="3"/>
+      <c r="AP79" s="3"/>
+    </row>
+    <row r="80" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A80" s="2"/>
       <c r="B80" s="2"/>
       <c r="C80" s="2"/>
@@ -7916,8 +8945,22 @@
       <c r="J80" s="2"/>
       <c r="K80" s="2"/>
       <c r="L80" s="2"/>
-    </row>
-    <row r="81" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="AC80" s="5"/>
+      <c r="AD80" s="3"/>
+      <c r="AE80" s="3"/>
+      <c r="AF80" s="3"/>
+      <c r="AG80" s="3"/>
+      <c r="AH80" s="3"/>
+      <c r="AI80" s="3"/>
+      <c r="AJ80" s="3"/>
+      <c r="AK80" s="3"/>
+      <c r="AL80" s="3"/>
+      <c r="AM80" s="3"/>
+      <c r="AN80" s="3"/>
+      <c r="AO80" s="3"/>
+      <c r="AP80" s="3"/>
+    </row>
+    <row r="81" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A81" s="2"/>
       <c r="B81" s="2"/>
       <c r="C81" s="2"/>
@@ -7930,8 +8973,21 @@
       <c r="J81" s="2"/>
       <c r="K81" s="2"/>
       <c r="L81" s="2"/>
-    </row>
-    <row r="82" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="AD81" s="4"/>
+      <c r="AE81" s="4"/>
+      <c r="AF81" s="4"/>
+      <c r="AG81" s="4"/>
+      <c r="AH81" s="4"/>
+      <c r="AI81" s="4"/>
+      <c r="AJ81" s="4"/>
+      <c r="AK81" s="4"/>
+      <c r="AL81" s="4"/>
+      <c r="AM81" s="4"/>
+      <c r="AN81" s="4"/>
+      <c r="AO81" s="3"/>
+      <c r="AP81" s="3"/>
+    </row>
+    <row r="82" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A82" s="2"/>
       <c r="B82" s="2"/>
       <c r="C82" s="2"/>
@@ -7944,8 +9000,10 @@
       <c r="J82" s="2"/>
       <c r="K82" s="2"/>
       <c r="L82" s="2"/>
-    </row>
-    <row r="83" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="AO82" s="3"/>
+      <c r="AP82" s="3"/>
+    </row>
+    <row r="83" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A83" s="2"/>
       <c r="B83" s="2"/>
       <c r="C83" s="2"/>
@@ -7958,8 +9016,10 @@
       <c r="J83" s="2"/>
       <c r="K83" s="2"/>
       <c r="L83" s="2"/>
-    </row>
-    <row r="84" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="AO83" s="3"/>
+      <c r="AP83" s="3"/>
+    </row>
+    <row r="84" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A84" s="2"/>
       <c r="B84" s="2"/>
       <c r="C84" s="2"/>
@@ -7972,8 +9032,10 @@
       <c r="J84" s="2"/>
       <c r="K84" s="2"/>
       <c r="L84" s="2"/>
-    </row>
-    <row r="85" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="AO84" s="3"/>
+      <c r="AP84" s="3"/>
+    </row>
+    <row r="85" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A85" s="2"/>
       <c r="B85" s="2"/>
       <c r="C85" s="2"/>
@@ -7986,8 +9048,10 @@
       <c r="J85" s="2"/>
       <c r="K85" s="2"/>
       <c r="L85" s="2"/>
-    </row>
-    <row r="86" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="AO85" s="3"/>
+      <c r="AP85" s="3"/>
+    </row>
+    <row r="86" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A86" s="2"/>
       <c r="B86" s="2"/>
       <c r="C86" s="2"/>
@@ -8000,8 +9064,10 @@
       <c r="J86" s="2"/>
       <c r="K86" s="2"/>
       <c r="L86" s="2"/>
-    </row>
-    <row r="87" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="AO86" s="3"/>
+      <c r="AP86" s="3"/>
+    </row>
+    <row r="87" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A87" s="2"/>
       <c r="B87" s="2"/>
       <c r="C87" s="2"/>
@@ -8014,8 +9080,10 @@
       <c r="J87" s="2"/>
       <c r="K87" s="2"/>
       <c r="L87" s="2"/>
-    </row>
-    <row r="88" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="AO87" s="3"/>
+      <c r="AP87" s="3"/>
+    </row>
+    <row r="88" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A88" s="2"/>
       <c r="B88" s="2"/>
       <c r="C88" s="2"/>
@@ -8028,8 +9096,10 @@
       <c r="J88" s="2"/>
       <c r="K88" s="2"/>
       <c r="L88" s="2"/>
-    </row>
-    <row r="89" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="AO88" s="3"/>
+      <c r="AP88" s="3"/>
+    </row>
+    <row r="89" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A89" s="2"/>
       <c r="B89" s="2"/>
       <c r="C89" s="2"/>
@@ -8042,8 +9112,10 @@
       <c r="J89" s="2"/>
       <c r="K89" s="2"/>
       <c r="L89" s="2"/>
-    </row>
-    <row r="90" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="AO89" s="3"/>
+      <c r="AP89" s="3"/>
+    </row>
+    <row r="90" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A90" s="2"/>
       <c r="B90" s="2"/>
       <c r="C90" s="2"/>
@@ -8056,8 +9128,10 @@
       <c r="J90" s="2"/>
       <c r="K90" s="2"/>
       <c r="L90" s="2"/>
-    </row>
-    <row r="91" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="AO90" s="3"/>
+      <c r="AP90" s="3"/>
+    </row>
+    <row r="91" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A91" s="2"/>
       <c r="B91" s="2"/>
       <c r="C91" s="2"/>
@@ -8070,8 +9144,10 @@
       <c r="J91" s="2"/>
       <c r="K91" s="2"/>
       <c r="L91" s="2"/>
-    </row>
-    <row r="92" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="AO91" s="3"/>
+      <c r="AP91" s="3"/>
+    </row>
+    <row r="92" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A92" s="2"/>
       <c r="B92" s="2"/>
       <c r="C92" s="2"/>
@@ -8084,8 +9160,10 @@
       <c r="J92" s="2"/>
       <c r="K92" s="2"/>
       <c r="L92" s="2"/>
-    </row>
-    <row r="93" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="AO92" s="3"/>
+      <c r="AP92" s="3"/>
+    </row>
+    <row r="93" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A93" s="2"/>
       <c r="B93" s="2"/>
       <c r="C93" s="2"/>
@@ -8098,8 +9176,10 @@
       <c r="J93" s="2"/>
       <c r="K93" s="2"/>
       <c r="L93" s="2"/>
-    </row>
-    <row r="94" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="AO93" s="3"/>
+      <c r="AP93" s="3"/>
+    </row>
+    <row r="94" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A94" s="2"/>
       <c r="B94" s="2"/>
       <c r="C94" s="2"/>
@@ -8112,8 +9192,10 @@
       <c r="J94" s="2"/>
       <c r="K94" s="2"/>
       <c r="L94" s="2"/>
-    </row>
-    <row r="95" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="AO94" s="3"/>
+      <c r="AP94" s="3"/>
+    </row>
+    <row r="95" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A95" s="2"/>
       <c r="B95" s="2"/>
       <c r="C95" s="2"/>
@@ -8126,8 +9208,10 @@
       <c r="J95" s="2"/>
       <c r="K95" s="2"/>
       <c r="L95" s="2"/>
-    </row>
-    <row r="96" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="AO95" s="3"/>
+      <c r="AP95" s="3"/>
+    </row>
+    <row r="96" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A96" s="2"/>
       <c r="B96" s="2"/>
       <c r="C96" s="2"/>
@@ -8140,8 +9224,10 @@
       <c r="J96" s="2"/>
       <c r="K96" s="2"/>
       <c r="L96" s="2"/>
-    </row>
-    <row r="97" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="AO96" s="3"/>
+      <c r="AP96" s="3"/>
+    </row>
+    <row r="97" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A97" s="2"/>
       <c r="B97" s="2"/>
       <c r="C97" s="2"/>
@@ -8154,8 +9240,10 @@
       <c r="J97" s="2"/>
       <c r="K97" s="2"/>
       <c r="L97" s="2"/>
-    </row>
-    <row r="98" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="AO97" s="3"/>
+      <c r="AP97" s="3"/>
+    </row>
+    <row r="98" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A98" s="2"/>
       <c r="B98" s="2"/>
       <c r="C98" s="2"/>
@@ -8168,8 +9256,10 @@
       <c r="J98" s="2"/>
       <c r="K98" s="2"/>
       <c r="L98" s="2"/>
-    </row>
-    <row r="99" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="AO98" s="3"/>
+      <c r="AP98" s="3"/>
+    </row>
+    <row r="99" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A99" s="2"/>
       <c r="B99" s="2"/>
       <c r="C99" s="2"/>
@@ -8182,8 +9272,10 @@
       <c r="J99" s="2"/>
       <c r="K99" s="2"/>
       <c r="L99" s="2"/>
-    </row>
-    <row r="100" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="AO99" s="3"/>
+      <c r="AP99" s="3"/>
+    </row>
+    <row r="100" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A100" s="2"/>
       <c r="B100" s="2"/>
       <c r="C100" s="2"/>
@@ -8196,8 +9288,10 @@
       <c r="J100" s="2"/>
       <c r="K100" s="2"/>
       <c r="L100" s="2"/>
-    </row>
-    <row r="101" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="AO100" s="3"/>
+      <c r="AP100" s="3"/>
+    </row>
+    <row r="101" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A101" s="2"/>
       <c r="B101" s="2"/>
       <c r="C101" s="2"/>
@@ -8210,8 +9304,10 @@
       <c r="J101" s="2"/>
       <c r="K101" s="2"/>
       <c r="L101" s="2"/>
-    </row>
-    <row r="102" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="AO101" s="3"/>
+      <c r="AP101" s="3"/>
+    </row>
+    <row r="102" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A102" s="2"/>
       <c r="B102" s="2"/>
       <c r="C102" s="2"/>
@@ -8224,8 +9320,10 @@
       <c r="J102" s="2"/>
       <c r="K102" s="2"/>
       <c r="L102" s="2"/>
-    </row>
-    <row r="103" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="AO102" s="3"/>
+      <c r="AP102" s="3"/>
+    </row>
+    <row r="103" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A103" s="2"/>
       <c r="B103" s="2"/>
       <c r="C103" s="2"/>
@@ -8239,7 +9337,7 @@
       <c r="K103" s="2"/>
       <c r="L103" s="2"/>
     </row>
-    <row r="104" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A104" s="2"/>
       <c r="B104" s="2"/>
       <c r="C104" s="2"/>
@@ -8253,7 +9351,7 @@
       <c r="K104" s="2"/>
       <c r="L104" s="2"/>
     </row>
-    <row r="105" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A105" s="2"/>
       <c r="B105" s="2"/>
       <c r="C105" s="2"/>
@@ -8267,7 +9365,7 @@
       <c r="K105" s="2"/>
       <c r="L105" s="2"/>
     </row>
-    <row r="106" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A106" s="2"/>
       <c r="B106" s="2"/>
       <c r="C106" s="2"/>
@@ -8281,7 +9379,7 @@
       <c r="K106" s="2"/>
       <c r="L106" s="2"/>
     </row>
-    <row r="107" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A107" s="2"/>
       <c r="B107" s="2"/>
       <c r="C107" s="2"/>
@@ -8295,7 +9393,7 @@
       <c r="K107" s="2"/>
       <c r="L107" s="2"/>
     </row>
-    <row r="108" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A108" s="2"/>
       <c r="B108" s="2"/>
       <c r="C108" s="2"/>
@@ -8309,7 +9407,7 @@
       <c r="K108" s="2"/>
       <c r="L108" s="2"/>
     </row>
-    <row r="109" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A109" s="2"/>
       <c r="B109" s="2"/>
       <c r="C109" s="2"/>
@@ -8323,7 +9421,7 @@
       <c r="K109" s="2"/>
       <c r="L109" s="2"/>
     </row>
-    <row r="110" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A110" s="2"/>
       <c r="B110" s="2"/>
       <c r="C110" s="2"/>
@@ -8337,7 +9435,7 @@
       <c r="K110" s="2"/>
       <c r="L110" s="2"/>
     </row>
-    <row r="111" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A111" s="2"/>
       <c r="B111" s="2"/>
       <c r="C111" s="2"/>
@@ -8351,7 +9449,7 @@
       <c r="K111" s="2"/>
       <c r="L111" s="2"/>
     </row>
-    <row r="112" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A112" s="2"/>
       <c r="B112" s="2"/>
       <c r="C112" s="2"/>
@@ -9025,19 +10123,19 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="H10:O11 U10:U11 Q10:R11">
-    <cfRule type="duplicateValues" dxfId="5" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="4" priority="5"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H13:O14">
-    <cfRule type="duplicateValues" dxfId="4" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="3" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H18:O19">
-    <cfRule type="duplicateValues" dxfId="3" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="2" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H20:S21">
-    <cfRule type="duplicateValues" dxfId="2" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="1" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H24:AA24 H22:AA22">
-    <cfRule type="duplicateValues" dxfId="1" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
modificacion de CashMagmente del 49
</commit_message>
<xml_diff>
--- a/src/test/resources/Descriptions/DC_AUT_002_CashManagmentTest.xlsx
+++ b/src/test/resources/Descriptions/DC_AUT_002_CashManagmentTest.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20394"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20395"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AFB2C0C-162D-494C-A560-D5A09E5F3073}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FEEB48A-069C-4FB7-85D6-E45DA1978238}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1496" uniqueCount="445">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1655" uniqueCount="526">
   <si>
     <t>Escenario</t>
   </si>
@@ -2251,9 +2251,6 @@
     <t>TC_002_61_administradorConsultaCuentasChequeMXNTXT</t>
   </si>
   <si>
-    <t>TC_002_62_administradorConsultaCuentasLineaOperativa</t>
-  </si>
-  <si>
     <t>El usuario valida que se muestre el campo "País".||El sistema muestra el campo "País" de forma correcta.</t>
   </si>
   <si>
@@ -2409,12 +2406,420 @@
   <si>
     <t>El usuario valida el campo "Tasa".||El sistema muestra la tasa de forma correcta.</t>
   </si>
+  <si>
+    <t>TC_002_62_administradorConsultaCuentasLineaOperativaPDF</t>
+  </si>
+  <si>
+    <t>El usuario valida el campo "Descripción del préstamo".||El sistema muestra la descripción del préstamo de forma correcta.</t>
+  </si>
+  <si>
+    <t>El usuario valida el campo "Pagos vencidos".||El sistema muestra los pagos vencidos de forma correcta.</t>
+  </si>
+  <si>
+    <t>El usuario valida el campo "Estado del crédito".||El sistema muestra el estado del crédito de forma correcta.</t>
+  </si>
+  <si>
+    <t>El usuario valida el campo "Total del saldo".||El sistema muestra el campo "Total del saldo " del movimiento con el siguiente formato:
+Signo $
+Separación de miles y millones con separador de coma (,)
+Signo de punto para decimales (.)
+2 decimales</t>
+  </si>
+  <si>
+    <t>El usuario valida el campo "Adeudo Vencido Capital".||El sistema muestra el campo "Adeudo Vencido Capital" del movimiento con el siguiente formato:
+Signo $
+Separación de miles y millones con separador de coma (,)
+Signo de punto para decimales (.)
+2 decimales</t>
+  </si>
+  <si>
+    <t>El usuario valida el campo "Adeudo Vencido Intereses".||El sistema muestra el campo "Adeudo Vencido Intereses" del movimiento con el siguiente formato:
+Signo $
+Separación de miles y millones con separador de coma (,)
+Signo de punto para decimales (.)
+2 decimales</t>
+  </si>
+  <si>
+    <t>El usuario valida el campo "Adeudo Vencido Seguro".||El sistema muestra el campo "Adeudo Vencido Seguro" del movimiento con el siguiente formato:
+Signo $
+Separación de miles y millones con separador de coma (,)
+Signo de punto para decimales (.)
+2 decimales</t>
+  </si>
+  <si>
+    <t>El usuario valida el campo "Adeudo Vencido Comisiones".||El sistema muestra el campo "Adeudo Vencido Comisiones" del movimiento con el siguiente formato:
+Signo $
+Separación de miles y millones con separador de coma (,)
+Signo de punto para decimales (.)
+2 decimales</t>
+  </si>
+  <si>
+    <t>El usuario valida el campo "Adeudo Vencido Gastos de cobranza".||El sistema muestra el campo "Adeudo Vencido Gastos de cobranza" del movimiento con el siguiente formato:
+Signo $
+Separación de miles y millones con separador de coma (,)
+Signo de punto para decimales (.)
+2 decimales</t>
+  </si>
+  <si>
+    <t>El usuario valida el campo "Adeudo Vencido Moratorios".||
+El sistema muestra el campo "Adeudo Vencido Moratorios" del movimiento con el siguiente formato:
+Signo $
+Separación de miles y millones con separador de coma (,)
+Signo de punto para decimales (.)
+2 decimales</t>
+  </si>
+  <si>
+    <t>El usuario valida el campo "Adeudo Vencido IVA".||El sistema muestra el campo "Adeudo Vencido IVA" del movimiento con el siguiente formato:
+Signo $
+Separación de miles y millones con separador de coma (,)
+Signo de punto para decimales (.)
+2 decimales</t>
+  </si>
+  <si>
+    <t>El usuario valida el campo "Adeudo Vencido Total vencido".||El sistema muestra el campo "Adeudo Vencido Total vencido" del movimiento con el siguiente formato:
+Signo $
+Separación de miles y millones con separador de coma (,)
+Signo de punto para decimales (.)
+2 decimales</t>
+  </si>
+  <si>
+    <t>El usuario valida el campo "Mensualidad Vigente: Capital".||El sistema muestra el campo "Mensualidad Vigente: Capital" del movimiento con el siguiente formato:
+Signo $
+Separación de miles y millones con separador de coma (,)
+Signo de punto para decimales (.)
+2 decimales</t>
+  </si>
+  <si>
+    <t>El usuario valida el campo "Mensualidad Vigente: Intereses".||El sistema muestra el campo "Total del saldo " del movimiento con el siguiente formato:
+Signo $
+Separación de miles y millones con separador de coma (,)
+Signo de punto para decimales (.)
+2 decimales</t>
+  </si>
+  <si>
+    <t>El usuario valida el campo "Mensualidad Vigente:IVA Intereses".||El sistema muestra el campo "Mensualidad Vigente:IVA Intereses" del movimiento con el siguiente formato:
+Signo $
+Separación de miles y millones con separador de coma (,)
+Signo de punto para decimales (.)
+2 decimales</t>
+  </si>
+  <si>
+    <t>El usuario valida el campo "Mensualidad Vigente: Seguros".||El sistema muestra el campo "Mensualidad Vigente: Seguros" del movimiento con el siguiente formato:
+Signo $
+Separación de miles y millones con separador de coma (,)
+Signo de punto para decimales (.)
+2 decimales</t>
+  </si>
+  <si>
+    <t>El usuario valida el campo "Mensualidad Vigente: IVA Seguros".||
+El sistema muestra el campo "Mensualidad Vigente: IVA Seguros"" del movimiento con el siguiente formato:
+Signo $
+Separación de miles y millones con separador de coma (,)
+Signo de punto para decimales (.)
+2 decimales</t>
+  </si>
+  <si>
+    <t>El usuario valida el campo "Mensualidad Vigente: Comisiones".||El sistema muestra el campo "Mensualidad Vigente: Comisiones" del movimiento con el siguiente formato:
+Signo $
+Separación de miles y millones con separador de coma (,)
+Signo de punto para decimales (.)
+2 decimales</t>
+  </si>
+  <si>
+    <t>El usuario valida el campo "Mensualidad Vigente: IVA Comisiones".||El sistema muestra el campo "Mensualidad Vigente: IVA Comisiones" del movimiento con el siguiente formato:
+Signo $
+Separación de miles y millones con separador de coma (,)
+Signo de punto para decimales (.)
+2 decimales</t>
+  </si>
+  <si>
+    <t>El usuario valida el campo "Mensualidad Vigente: Total".||El sistema muestra el campo "Mensualidad Vigente: Total" del movimiento con el siguiente formato:
+Signo $
+Separación de miles y millones con separador de coma (,)
+Signo de punto para decimales (.)
+2 decimales</t>
+  </si>
+  <si>
+    <t>El usuario valida que se muestre la columna "Tipo operación".||El sistema muestra la columna "Tipo de operación" con los valores "Cargo" o "Abono".</t>
+  </si>
+  <si>
+    <t>El usuario valida que se muestre la columna "Descripción del movimiento".||El sistema muestra la columna "Descripción del movimiento" con la descripción del movimiento.</t>
+  </si>
+  <si>
+    <t>El usuario indica una fecha fin en el campo de búsqueda "Seleccione fecha fin".||El sistema muestra la fecha fin de forma correcta y el resultado de la búsqueda de movimientos en la siguiente tabla:
+Columna "Fecha del movimiento"
+Columna "Referencia"
+Columna "Importe operación"
+Columna "Tipo operación"
+Columna "Descripción del movimiento"</t>
+  </si>
+  <si>
+    <t>El usuario valida el campo "Fondo".||El sistema muestra el fondo de forma correcta.</t>
+  </si>
+  <si>
+    <t>El usuario valida el campo "Número de títulos".||El sistema muestra el número de títulos de forma correcta.</t>
+  </si>
+  <si>
+    <t>El usuario da clic en la opción "Mostrar detalles".||El sistema permite mostrar la sección de Saldos con los siguientes campos:
+Precio de títulos
+Valuación
+Estado
+Opción "Ocutar detalles"</t>
+  </si>
+  <si>
+    <t>El usuario valida que se muestre el campo "Precio de títulos".||El sistema muestra la columna "Precio de títulos" de forma correcta con formato de moneda:
+Signo $
+Separación de miles y millones con separador de coma (,)
+Signo de punto para decimales (.)
+2 decimales</t>
+  </si>
+  <si>
+    <t>El usuario valida el campo "Valuación".||El sistema muestra la columna "Precio de títulos" de forma correcta con formato de moneda:
+Signo $
+Separación de miles y millones con separador de coma (,)
+Signo de punto para decimales (.)
+2 decimales</t>
+  </si>
+  <si>
+    <t>El usuario valida el campo "Estado".||El sistema muestra el estado de forma correcta.</t>
+  </si>
+  <si>
+    <t>El usuario valida que se muestre la columna "Fecha".||El sistema muestra la columna "Fecha" en formato DD/MMM/AAAA".</t>
+  </si>
+  <si>
+    <t>El usuario valida que se muestre la columna "Referencia Numérica".||El sistema muestra la columna "Referencia Numérica" de forma correcta.</t>
+  </si>
+  <si>
+    <t>El usuario valida que se muestre la columna "Importe de operación".||El sistema muestra la columna "Importe de operación" del movimiento con el siguiente formato:
+Signo $
+Separación de miles y millones con separador de coma (,)
+Signo de punto para decimales (.)
+2 decimales</t>
+  </si>
+  <si>
+    <t>El usuario valida que se muestre la columna "Tipo de operación".||El sistema muestra la columna "Tipo de operación" con los valores "Cargo" o "Abono".</t>
+  </si>
+  <si>
+    <t>El usuario valida que se muestre la columna "Transacción".||El sistema muestra la columna "Transacción" con la descripción del movimiento.</t>
+  </si>
+  <si>
+    <t>El usuario valida que se muestre la columna opciones (…).||El sistema muestra el comprobante del movimiento.</t>
+  </si>
+  <si>
+    <t>El usuario indica una fecha fin en el campo de búsqueda "Seleccione fecha fin".||El sistema muestra la fecha fin de forma correcta y el resultado de la búsqueda de movimientos en la siguiente tabla:
+Columna "Fecha"
+Columna "Referencia Numérica"
+Columna "Importe de operación"
+Columna "Tipo de operación"
+Columna "Transacción"</t>
+  </si>
+  <si>
+    <t>TC_002_65_administradorConsulta CresitosHipotecarios</t>
+  </si>
+  <si>
+    <t>El usuario valida el campo "País".||El sistema muestra el país de forma correcta.</t>
+  </si>
+  <si>
+    <t>El usuario valida el campo "Ciudad".||El sistema muestra el país de forma correcta.</t>
+  </si>
+  <si>
+    <t>El usuario valida que se muestre el campo "Valor Crédito Original".||El sistema muestra el campo "Valor Crédito Original" de forma correcta con formato de moneda:
+Signo $
+Separación de miles y millones con separador de coma (,)
+Signo de punto para decimales (.)
+2 decimales</t>
+  </si>
+  <si>
+    <t>El usuario da clic en la opción "Mostrar detalles".||El sistema permite mostrar la sección de Saldos con los siguientes campos:
+Saldo vigente
+Saldo vencido
+Valor del UDI
+Sucursal de Asignación
+Fecha de Otorgamiento
+Pagos vencidos
+Opción "Ocutar detalles"</t>
+  </si>
+  <si>
+    <t>El usuario valida que se muestre el campo "Saldo vigente"||El sistema muestra la columna "Saldo vigente" de forma correcta con formato de moneda:
+Signo $
+Separación de miles y millones con separador de coma (,)
+Signo de punto para decimales (.)
+2 decimales</t>
+  </si>
+  <si>
+    <t>El usuario valida que se muestre el campo "Saldo vencido"||El sistema muestra la columna "Saldo vencido" de forma correcta con formato de moneda:
+Signo $
+Separación de miles y millones con separador de coma (,)
+Signo de punto para decimales (.)
+2 decimales</t>
+  </si>
+  <si>
+    <t>El usuario valida el campo "Valor del UDI".||El sistema muestra el valor del UDI de forma correcta.</t>
+  </si>
+  <si>
+    <t>El usuario valida el campo "Sucursal de Asignación".||El sistema muestra la sucursal de asignación de forma correcta.</t>
+  </si>
+  <si>
+    <t>El usuario valida el campo "Fecha de Otorgamiento".||El sistema muestra la fecha de otorgamiento de forma correcta en formato DD/MMM/AAAA.</t>
+  </si>
+  <si>
+    <t>El usuario valida que se muestre la columna "Importe operación".||El sistema muestra la columna "Importe operación" del movimiento con el siguiente formato:
+Signo $
+Separación de miles y millones con separador de coma (,)
+Signo de punto para decimales (.)
+2 decimales
+Se muestra el valor positivo si se trata de un Abono.
+Se muestra el valor negativo si se trata de un Cargo.</t>
+  </si>
+  <si>
+    <t>El usuario valida que se muestre la columna "Tipo de operación".||El sistema muestra la columna "Tipo de operación".</t>
+  </si>
+  <si>
+    <t>El usuario indica una fecha fin en el campo de búsqueda "Seleccione fecha fin".||El sistema muestra la fecha fin de forma correcta y el resultado de la búsqueda de movimientos en la siguiente tabla:
+Columna "Fecha del movimiento"
+Columna "Importe operación"
+Columna "Referencia"
+Columna "Descripción del movimiento"
+Columna "Tipo de operación"</t>
+  </si>
+  <si>
+    <t>TC_002_66_administradorConsulta Contar con permisos para consultar cuentas de Inversión</t>
+  </si>
+  <si>
+    <t>El usuario valida que se muestre el campo "Número de Cuenta eje"||El sistema muestra el campo "Número de Cuenta eje" de forma correcta.</t>
+  </si>
+  <si>
+    <t>El usuario valida que se muestre el campo "Importe de Capital".||El sistema muestra el campo "Importe de Capital" de forma correcta con formato de moneda:
+Signo $
+Separación de miles y millones con separador de coma (,)
+Signo de punto para decimales (.)
+2 decimales</t>
+  </si>
+  <si>
+    <t>El usuario selecciona un número de inversión.||El sistema muestra el detalle del número de inversión seleccionado.</t>
+  </si>
+  <si>
+    <t>El usuario valida que se muestre el campo "Sucursal de asignación".||El sistema muestra la columna "Sucursal de asignación" de forma correcta con formato de moneda:
+Signo $
+Separación de miles y millones con separador de coma (,)
+Signo de punto para decimales (.)
+2 decimales</t>
+  </si>
+  <si>
+    <t>El usuario valida que se muestre el campo "Nombre del cliente".||El sistema muestra el campo "Nombre del cliente" de forma correcta.</t>
+  </si>
+  <si>
+    <t>El usuario valida que se muestre el campo "Fecha de apertura".||El sistema muestra el campo "Fecha de apertura" de forma correcta.</t>
+  </si>
+  <si>
+    <t>El usuario valida que se muestre el campo "Fecha de vencimiento".||El sistema muestra el campo "Fecha de vencimiento" de forma correcta.</t>
+  </si>
+  <si>
+    <t>El usuario valida que se muestre el campo "Clave renovación".||El sistema muestra el campo "Clave renovación" de forma correcta.</t>
+  </si>
+  <si>
+    <t>El usuario valida que se muestre el campo "Sobretasa".||El sistema muestra el campo "Sobretasa" de forma correcta.</t>
+  </si>
+  <si>
+    <t>El usuario valida que se muestre el campo "Tasa".||El sistema muestra el campo "Tasa" de forma correcta.</t>
+  </si>
+  <si>
+    <t>El usuario valida que se muestre el campo "Intereses".||El sistema muestra el campo "Intereses" de forma correcta con formato de moneda:
+Signo $
+Separación de miles y millones con separador de coma (,)
+Signo de punto para decimales (.)
+2 decimales</t>
+  </si>
+  <si>
+    <t>El usuario valida que se muestre el campo "Plazo".||El sistema muestra el campo "Plazo" de forma correcta.</t>
+  </si>
+  <si>
+    <t>El usuario indica una fecha fin en el campo de búsqueda "Seleccione fecha fin".||El sistema muestra la fecha fin de forma correcta y el resultado de la búsqueda de movimientos en la siguiente tabla:
+Columna "Fecha "
+Columna "Tipo de operación"
+Columna "Descripción"
+Columna "Importe"
+Columna "Saldo final importe de capital"</t>
+  </si>
+  <si>
+    <t>TC_002_63_administradorConsultaCuentasPrestamosPersonalesPDF</t>
+  </si>
+  <si>
+    <t>TC_002_64_administradorConsultaCuentasFondosInversionPDF</t>
+  </si>
+  <si>
+    <t>TC_002_67_administradorConsultaCuentasTDCMXNPDF</t>
+  </si>
+  <si>
+    <t>El usuario valida que se muestre el campo "Número de la tarjeta"||El sistema muestra el campo "Número de la tarjeta" de forma correcta.</t>
+  </si>
+  <si>
+    <t>El usuario valida que se muestre el campo "Nombre de cliente".||El sistema muestra el nombre del cliente de forma correcta.</t>
+  </si>
+  <si>
+    <t>El usuario valida que se muestre el campo "País".||El sistema muestra el país de forma correcta.</t>
+  </si>
+  <si>
+    <t>El usuario valida que se muestre el campo "Moneda".||El sistema muestra la moneda de forma correcta.</t>
+  </si>
+  <si>
+    <t>El usuario da clic en "Ver detalles".||El sistema muestra los campos:
+Saldo disponible
+Límite de Crédito
+Estado de la cuenta
+Fecha Límite de pago
+Pago mínimo
+Fecha de corte
+Pagos vencidos</t>
+  </si>
+  <si>
+    <t>El usuario valida que se muestre el campo "Saldo disponible".||El sistema muestra el campo "Saldo disponible" de forma correcta con formato de moneda:
+Signo $
+Separación de miles y millones con separador de coma (,)
+Signo de punto para decimales (.)
+2 decimales</t>
+  </si>
+  <si>
+    <t>El usuario valida que se muestre el campo "Límite de crédito"||El sistema muestra el campo "Límite de crédito" de forma correcta con formato de moneda:
+Signo $
+Separación de miles y millones con separador de coma (,)
+Signo de punto para decimales (.)
+2 decimales</t>
+  </si>
+  <si>
+    <t>El usuario valida que se muestre el campo "Estado de la cuenta"||El sistema muestra el estado de la cuenta como "ACTIVA".</t>
+  </si>
+  <si>
+    <t>El usuario valida que se muestre el campo "Fecha Límite de pago"||El sistema muestra la fecha límite de pago de forma correcta.</t>
+  </si>
+  <si>
+    <t>El usuario valida que se muestre el campo "Pago mínimo"||El sistema muestra el campo "Pago mínimo" de forma correcta con formato de moneda:
+Signo $
+Separación de miles y millones con separador de coma (,)
+Signo de punto para decimales (.)
+2 decimales</t>
+  </si>
+  <si>
+    <t>El usuario valida que se muestre el campo "Fecha de corte"||El sistema muestra la fecha de corte de forma correcta.</t>
+  </si>
+  <si>
+    <t>El usuario valida que se muestre el campo "Pagos vencidos"||El sistema muestra el número de Pagos vencidos de forma correcta.</t>
+  </si>
+  <si>
+    <t>El usuario valida que se muestre la opción del cuadro de Búsqueda.||El sistema muestra la opción del cuadro de "Búsqueda" de forma correcta.</t>
+  </si>
+  <si>
+    <t>El usuario valida que se muestre la opción "Ver consolidado"||El sistema muestra la opción "Ver consolidado" de forma correcta como hipervínculo.</t>
+  </si>
+  <si>
+    <t>El usuario valida que se muestre el botón de Descarga.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2429,8 +2834,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2465,6 +2877,11 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
       </patternFill>
     </fill>
   </fills>
@@ -2640,10 +3057,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -2793,8 +3211,12 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Incorrecto" xfId="1" builtinId="27"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="5">
@@ -3166,10 +3588,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AR159"/>
+  <dimension ref="A1:BC159"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+    <sheetView tabSelected="1" topLeftCell="V66" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="Y68" sqref="Y68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3218,6 +3640,17 @@
     <col min="42" max="42" width="62" customWidth="1"/>
     <col min="43" max="43" width="58.28515625" customWidth="1"/>
     <col min="44" max="44" width="49.28515625" customWidth="1"/>
+    <col min="45" max="45" width="46.42578125" customWidth="1"/>
+    <col min="46" max="46" width="42.42578125" customWidth="1"/>
+    <col min="47" max="47" width="42.140625" customWidth="1"/>
+    <col min="48" max="48" width="40.42578125" customWidth="1"/>
+    <col min="49" max="49" width="47" customWidth="1"/>
+    <col min="50" max="50" width="43.42578125" customWidth="1"/>
+    <col min="51" max="51" width="43" customWidth="1"/>
+    <col min="52" max="52" width="45.85546875" customWidth="1"/>
+    <col min="53" max="53" width="46.140625" customWidth="1"/>
+    <col min="54" max="54" width="50.7109375" customWidth="1"/>
+    <col min="55" max="55" width="51.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:44" x14ac:dyDescent="0.25">
@@ -7058,7 +7491,7 @@
       <c r="AM48" s="3"/>
       <c r="AN48" s="3"/>
     </row>
-    <row r="49" spans="1:42" ht="105" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:55" ht="105" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
         <v>358</v>
       </c>
@@ -7140,7 +7573,7 @@
       <c r="AM49" s="3"/>
       <c r="AN49" s="3"/>
     </row>
-    <row r="50" spans="1:42" ht="105" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:55" ht="105" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
         <v>359</v>
       </c>
@@ -7224,7 +7657,7 @@
       <c r="AM50" s="3"/>
       <c r="AN50" s="3"/>
     </row>
-    <row r="51" spans="1:42" ht="105" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:55" ht="105" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
         <v>366</v>
       </c>
@@ -7306,7 +7739,7 @@
       <c r="AM51" s="3"/>
       <c r="AN51" s="3"/>
     </row>
-    <row r="52" spans="1:42" ht="105" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:55" ht="105" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
         <v>367</v>
       </c>
@@ -7390,7 +7823,7 @@
       <c r="AM52" s="3"/>
       <c r="AN52" s="3"/>
     </row>
-    <row r="53" spans="1:42" ht="105" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:55" ht="105" x14ac:dyDescent="0.25">
       <c r="A53" s="2" t="s">
         <v>372</v>
       </c>
@@ -7472,7 +7905,7 @@
       <c r="AM53" s="3"/>
       <c r="AN53" s="3"/>
     </row>
-    <row r="54" spans="1:42" ht="105" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:55" ht="105" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
         <v>373</v>
       </c>
@@ -7556,7 +7989,7 @@
       <c r="AM54" s="3"/>
       <c r="AN54" s="3"/>
     </row>
-    <row r="55" spans="1:42" ht="180" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:55" ht="180" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
         <v>386</v>
       </c>
@@ -7638,7 +8071,7 @@
       <c r="AM55" s="3"/>
       <c r="AN55" s="3"/>
     </row>
-    <row r="56" spans="1:42" ht="180" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:55" ht="180" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
         <v>391</v>
       </c>
@@ -7720,7 +8153,7 @@
       <c r="AM56" s="3"/>
       <c r="AN56" s="3"/>
     </row>
-    <row r="57" spans="1:42" ht="180" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:55" ht="180" x14ac:dyDescent="0.25">
       <c r="A57" s="2" t="s">
         <v>395</v>
       </c>
@@ -7802,7 +8235,7 @@
       <c r="AM57" s="3"/>
       <c r="AN57" s="3"/>
     </row>
-    <row r="58" spans="1:42" ht="180" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:55" ht="180" x14ac:dyDescent="0.25">
       <c r="A58" s="2" t="s">
         <v>398</v>
       </c>
@@ -7873,7 +8306,7 @@
       <c r="AB58" s="16"/>
       <c r="AC58" s="4"/>
     </row>
-    <row r="59" spans="1:42" ht="180" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:55" ht="180" x14ac:dyDescent="0.25">
       <c r="A59" s="2" t="s">
         <v>401</v>
       </c>
@@ -7944,7 +8377,7 @@
       <c r="AB59" s="16"/>
       <c r="AC59" s="4"/>
     </row>
-    <row r="60" spans="1:42" ht="180" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:55" ht="180" x14ac:dyDescent="0.25">
       <c r="A60" s="2" t="s">
         <v>404</v>
       </c>
@@ -8015,7 +8448,7 @@
       <c r="AB60" s="16"/>
       <c r="AC60" s="4"/>
     </row>
-    <row r="61" spans="1:42" ht="180" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:55" ht="180" x14ac:dyDescent="0.25">
       <c r="A61" s="2" t="s">
         <v>405</v>
       </c>
@@ -8086,7 +8519,7 @@
       <c r="AB61" s="16"/>
       <c r="AC61" s="4"/>
     </row>
-    <row r="62" spans="1:42" ht="180" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:55" ht="180" x14ac:dyDescent="0.25">
       <c r="A62" s="2" t="s">
         <v>406</v>
       </c>
@@ -8157,9 +8590,9 @@
       <c r="AB62" s="16"/>
       <c r="AC62" s="4"/>
     </row>
-    <row r="63" spans="1:42" ht="150" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:55" ht="150" x14ac:dyDescent="0.25">
       <c r="A63" s="50" t="s">
-        <v>407</v>
+        <v>444</v>
       </c>
       <c r="B63" s="2"/>
       <c r="C63" s="6" t="s">
@@ -8190,101 +8623,103 @@
         <v>324</v>
       </c>
       <c r="L63" s="2" t="s">
+        <v>407</v>
+      </c>
+      <c r="M63" s="16" t="s">
         <v>408</v>
       </c>
-      <c r="M63" s="16" t="s">
+      <c r="N63" s="16" t="s">
         <v>409</v>
       </c>
-      <c r="N63" s="16" t="s">
+      <c r="O63" s="16" t="s">
         <v>410</v>
       </c>
-      <c r="O63" s="16" t="s">
+      <c r="P63" s="16" t="s">
         <v>411</v>
       </c>
-      <c r="P63" s="16" t="s">
+      <c r="Q63" s="16" t="s">
         <v>412</v>
       </c>
-      <c r="Q63" s="16" t="s">
+      <c r="R63" s="16" t="s">
         <v>413</v>
       </c>
-      <c r="R63" s="16" t="s">
+      <c r="S63" s="16" t="s">
         <v>414</v>
       </c>
-      <c r="S63" s="16" t="s">
+      <c r="T63" s="16" t="s">
         <v>415</v>
       </c>
-      <c r="T63" s="16" t="s">
+      <c r="U63" s="16" t="s">
         <v>416</v>
       </c>
-      <c r="U63" s="16" t="s">
+      <c r="V63" s="16" t="s">
         <v>417</v>
       </c>
-      <c r="V63" s="16" t="s">
+      <c r="W63" s="16" t="s">
         <v>418</v>
       </c>
-      <c r="W63" s="16" t="s">
+      <c r="X63" s="16" t="s">
         <v>419</v>
       </c>
-      <c r="X63" s="16" t="s">
+      <c r="Y63" s="16" t="s">
         <v>420</v>
       </c>
-      <c r="Y63" s="16" t="s">
+      <c r="Z63" s="16" t="s">
         <v>421</v>
       </c>
-      <c r="Z63" s="16" t="s">
+      <c r="AA63" s="16" t="s">
         <v>422</v>
       </c>
-      <c r="AA63" s="16" t="s">
+      <c r="AB63" s="16" t="s">
         <v>423</v>
-      </c>
-      <c r="AB63" s="16" t="s">
-        <v>424</v>
       </c>
       <c r="AC63" s="3" t="s">
         <v>325</v>
       </c>
       <c r="AD63" s="3" t="s">
+        <v>424</v>
+      </c>
+      <c r="AE63" s="3" t="s">
         <v>425</v>
       </c>
-      <c r="AE63" s="3" t="s">
+      <c r="AF63" s="3" t="s">
         <v>426</v>
       </c>
-      <c r="AF63" s="3" t="s">
+      <c r="AG63" s="3" t="s">
         <v>427</v>
       </c>
-      <c r="AG63" s="3" t="s">
+      <c r="AH63" s="3" t="s">
         <v>428</v>
       </c>
-      <c r="AH63" s="3" t="s">
+      <c r="AI63" s="3" t="s">
         <v>429</v>
       </c>
-      <c r="AI63" s="3" t="s">
+      <c r="AJ63" s="3" t="s">
         <v>430</v>
       </c>
-      <c r="AJ63" s="3" t="s">
+      <c r="AK63" s="3" t="s">
         <v>431</v>
-      </c>
-      <c r="AK63" s="3" t="s">
-        <v>432</v>
       </c>
       <c r="AL63" s="3" t="s">
         <v>325</v>
       </c>
       <c r="AM63" s="3" t="s">
+        <v>432</v>
+      </c>
+      <c r="AN63" s="3" t="s">
         <v>433</v>
       </c>
-      <c r="AN63" s="3" t="s">
+      <c r="AO63" s="3" t="s">
         <v>434</v>
       </c>
-      <c r="AO63" s="3" t="s">
+      <c r="AP63" s="3" t="s">
         <v>435</v>
       </c>
-      <c r="AP63" s="3" t="s">
-        <v>436</v>
-      </c>
-    </row>
-    <row r="64" spans="1:42" ht="150" x14ac:dyDescent="0.25">
-      <c r="A64" s="2"/>
+    </row>
+    <row r="64" spans="1:55" ht="164.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A64" s="2" t="s">
+        <v>508</v>
+      </c>
       <c r="B64" s="2"/>
       <c r="C64" s="6" t="s">
         <v>32</v>
@@ -8317,88 +8752,239 @@
         <v>343</v>
       </c>
       <c r="M64" s="16" t="s">
+        <v>436</v>
+      </c>
+      <c r="N64" s="16" t="s">
         <v>437</v>
       </c>
-      <c r="N64" s="16" t="s">
+      <c r="O64" s="16" t="s">
         <v>438</v>
       </c>
-      <c r="O64" s="16" t="s">
+      <c r="P64" s="16" t="s">
         <v>439</v>
       </c>
-      <c r="P64" s="16" t="s">
+      <c r="Q64" s="16" t="s">
         <v>440</v>
       </c>
-      <c r="Q64" s="16" t="s">
+      <c r="R64" s="16" t="s">
         <v>441</v>
       </c>
-      <c r="R64" s="16" t="s">
+      <c r="S64" s="16" t="s">
         <v>442</v>
       </c>
-      <c r="S64" s="16" t="s">
+      <c r="T64" s="16" t="s">
         <v>443</v>
       </c>
-      <c r="T64" s="16" t="s">
-        <v>444</v>
-      </c>
-      <c r="U64" s="16"/>
-      <c r="V64" s="16"/>
-      <c r="W64" s="16"/>
-      <c r="X64" s="16"/>
-      <c r="Y64" s="16"/>
-      <c r="Z64" s="16"/>
-      <c r="AA64" s="16"/>
-      <c r="AB64" s="16"/>
-      <c r="AC64" s="3"/>
-      <c r="AD64" s="3"/>
-      <c r="AE64" s="3"/>
-      <c r="AF64" s="3"/>
-      <c r="AG64" s="3"/>
-      <c r="AH64" s="3"/>
-      <c r="AI64" s="3"/>
-      <c r="AJ64" s="3"/>
-      <c r="AK64" s="3"/>
-      <c r="AL64" s="3"/>
-      <c r="AM64" s="3"/>
-      <c r="AN64" s="3"/>
-      <c r="AO64" s="3"/>
-      <c r="AP64" s="3"/>
-    </row>
-    <row r="65" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A65" s="2"/>
+      <c r="U64" s="16" t="s">
+        <v>445</v>
+      </c>
+      <c r="V64" s="16" t="s">
+        <v>446</v>
+      </c>
+      <c r="W64" s="16" t="s">
+        <v>447</v>
+      </c>
+      <c r="X64" s="16" t="s">
+        <v>448</v>
+      </c>
+      <c r="Y64" s="16" t="s">
+        <v>449</v>
+      </c>
+      <c r="Z64" s="16" t="s">
+        <v>450</v>
+      </c>
+      <c r="AA64" s="16" t="s">
+        <v>451</v>
+      </c>
+      <c r="AB64" s="16" t="s">
+        <v>452</v>
+      </c>
+      <c r="AC64" s="3" t="s">
+        <v>453</v>
+      </c>
+      <c r="AD64" s="3" t="s">
+        <v>454</v>
+      </c>
+      <c r="AE64" s="3" t="s">
+        <v>455</v>
+      </c>
+      <c r="AF64" s="3" t="s">
+        <v>456</v>
+      </c>
+      <c r="AG64" s="3" t="s">
+        <v>457</v>
+      </c>
+      <c r="AH64" s="3" t="s">
+        <v>458</v>
+      </c>
+      <c r="AI64" s="3" t="s">
+        <v>459</v>
+      </c>
+      <c r="AJ64" s="3" t="s">
+        <v>460</v>
+      </c>
+      <c r="AK64" s="3" t="s">
+        <v>461</v>
+      </c>
+      <c r="AL64" s="3" t="s">
+        <v>462</v>
+      </c>
+      <c r="AM64" s="3" t="s">
+        <v>463</v>
+      </c>
+      <c r="AN64" s="3" t="s">
+        <v>464</v>
+      </c>
+      <c r="AO64" s="3" t="s">
+        <v>423</v>
+      </c>
+      <c r="AP64" s="3" t="s">
+        <v>325</v>
+      </c>
+      <c r="AQ64" s="3" t="s">
+        <v>424</v>
+      </c>
+      <c r="AR64" s="3" t="s">
+        <v>425</v>
+      </c>
+      <c r="AS64" s="3" t="s">
+        <v>426</v>
+      </c>
+      <c r="AT64" s="3" t="s">
+        <v>427</v>
+      </c>
+      <c r="AU64" s="3" t="s">
+        <v>428</v>
+      </c>
+      <c r="AV64" s="3" t="s">
+        <v>429</v>
+      </c>
+      <c r="AW64" s="3" t="s">
+        <v>465</v>
+      </c>
+      <c r="AX64" s="3" t="s">
+        <v>466</v>
+      </c>
+      <c r="AY64" s="3" t="s">
+        <v>325</v>
+      </c>
+      <c r="AZ64" s="3" t="s">
+        <v>432</v>
+      </c>
+      <c r="BA64" s="3" t="s">
+        <v>467</v>
+      </c>
+      <c r="BB64" s="3" t="s">
+        <v>434</v>
+      </c>
+      <c r="BC64" s="3" t="s">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="65" spans="1:42" ht="190.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A65" s="2" t="s">
+        <v>509</v>
+      </c>
       <c r="B65" s="2"/>
-      <c r="C65" s="2"/>
-      <c r="D65" s="2"/>
-      <c r="E65" s="2"/>
-      <c r="F65" s="2"/>
-      <c r="G65" s="2"/>
-      <c r="H65" s="2"/>
-      <c r="I65" s="2"/>
-      <c r="J65" s="2"/>
-      <c r="K65" s="2"/>
-      <c r="L65" s="2"/>
-      <c r="M65" s="16"/>
-      <c r="N65" s="16"/>
-      <c r="O65" s="16"/>
-      <c r="P65" s="16"/>
-      <c r="Q65" s="16"/>
-      <c r="R65" s="16"/>
-      <c r="S65" s="16"/>
-      <c r="T65" s="16"/>
-      <c r="U65" s="16"/>
-      <c r="V65" s="16"/>
-      <c r="W65" s="16"/>
-      <c r="X65" s="16"/>
-      <c r="Y65" s="16"/>
-      <c r="Z65" s="16"/>
-      <c r="AA65" s="16"/>
-      <c r="AB65" s="16"/>
-      <c r="AC65" s="3"/>
-      <c r="AD65" s="3"/>
-      <c r="AE65" s="3"/>
-      <c r="AF65" s="3"/>
-      <c r="AG65" s="3"/>
-      <c r="AH65" s="3"/>
-      <c r="AI65" s="3"/>
+      <c r="C65" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="D65" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="E65" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="F65" s="26" t="s">
+        <v>35</v>
+      </c>
+      <c r="G65" s="20" t="s">
+        <v>36</v>
+      </c>
+      <c r="H65" s="47" t="s">
+        <v>321</v>
+      </c>
+      <c r="I65" s="2" t="s">
+        <v>345</v>
+      </c>
+      <c r="J65" s="2" t="s">
+        <v>346</v>
+      </c>
+      <c r="K65" s="2" t="s">
+        <v>347</v>
+      </c>
+      <c r="L65" s="2" t="s">
+        <v>442</v>
+      </c>
+      <c r="M65" s="43" t="s">
+        <v>436</v>
+      </c>
+      <c r="N65" s="16" t="s">
+        <v>468</v>
+      </c>
+      <c r="O65" s="43" t="s">
+        <v>469</v>
+      </c>
+      <c r="P65" s="43" t="s">
+        <v>470</v>
+      </c>
+      <c r="Q65" s="43" t="s">
+        <v>471</v>
+      </c>
+      <c r="R65" s="43" t="s">
+        <v>472</v>
+      </c>
+      <c r="S65" s="43" t="s">
+        <v>473</v>
+      </c>
+      <c r="T65" s="43" t="s">
+        <v>423</v>
+      </c>
+      <c r="U65" s="43" t="s">
+        <v>325</v>
+      </c>
+      <c r="V65" s="43" t="s">
+        <v>424</v>
+      </c>
+      <c r="W65" s="43" t="s">
+        <v>425</v>
+      </c>
+      <c r="X65" s="43" t="s">
+        <v>426</v>
+      </c>
+      <c r="Y65" s="43" t="s">
+        <v>474</v>
+      </c>
+      <c r="Z65" s="43" t="s">
+        <v>475</v>
+      </c>
+      <c r="AA65" s="43" t="s">
+        <v>476</v>
+      </c>
+      <c r="AB65" s="43" t="s">
+        <v>477</v>
+      </c>
+      <c r="AC65" s="2" t="s">
+        <v>478</v>
+      </c>
+      <c r="AD65" s="2" t="s">
+        <v>479</v>
+      </c>
+      <c r="AE65" s="3" t="s">
+        <v>325</v>
+      </c>
+      <c r="AF65" s="2" t="s">
+        <v>432</v>
+      </c>
+      <c r="AG65" s="2" t="s">
+        <v>480</v>
+      </c>
+      <c r="AH65" s="2" t="s">
+        <v>434</v>
+      </c>
+      <c r="AI65" s="2" t="s">
+        <v>435</v>
+      </c>
       <c r="AJ65" s="3"/>
       <c r="AK65" s="3"/>
       <c r="AL65" s="3"/>
@@ -8407,81 +8993,211 @@
       <c r="AO65" s="3"/>
       <c r="AP65" s="3"/>
     </row>
-    <row r="66" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A66" s="2"/>
+    <row r="66" spans="1:42" ht="190.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A66" s="51" t="s">
+        <v>481</v>
+      </c>
       <c r="B66" s="2"/>
-      <c r="C66" s="2"/>
-      <c r="D66" s="2"/>
-      <c r="E66" s="2"/>
-      <c r="F66" s="2"/>
-      <c r="G66" s="2"/>
-      <c r="H66" s="2"/>
-      <c r="I66" s="2"/>
-      <c r="J66" s="2"/>
-      <c r="K66" s="2"/>
-      <c r="L66" s="2"/>
-      <c r="M66" s="16"/>
-      <c r="N66" s="16"/>
-      <c r="O66" s="16"/>
-      <c r="P66" s="16"/>
-      <c r="Q66" s="16"/>
-      <c r="R66" s="16"/>
-      <c r="S66" s="16"/>
-      <c r="T66" s="16"/>
-      <c r="U66" s="16"/>
-      <c r="V66" s="16"/>
-      <c r="W66" s="16"/>
-      <c r="X66" s="16"/>
-      <c r="Y66" s="16"/>
-      <c r="Z66" s="16"/>
-      <c r="AA66" s="16"/>
-      <c r="AB66" s="16"/>
-      <c r="AC66" s="3"/>
-      <c r="AD66" s="3"/>
-      <c r="AE66" s="3"/>
-      <c r="AF66" s="3"/>
-      <c r="AG66" s="3"/>
-      <c r="AH66" s="3"/>
-      <c r="AI66" s="3"/>
-      <c r="AJ66" s="3"/>
-      <c r="AK66" s="3"/>
+      <c r="C66" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="D66" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="E66" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="F66" s="26" t="s">
+        <v>35</v>
+      </c>
+      <c r="G66" s="20" t="s">
+        <v>36</v>
+      </c>
+      <c r="H66" s="47" t="s">
+        <v>321</v>
+      </c>
+      <c r="I66" s="2" t="s">
+        <v>350</v>
+      </c>
+      <c r="J66" s="2" t="s">
+        <v>351</v>
+      </c>
+      <c r="K66" s="2" t="s">
+        <v>352</v>
+      </c>
+      <c r="L66" s="2" t="s">
+        <v>442</v>
+      </c>
+      <c r="M66" s="43" t="s">
+        <v>482</v>
+      </c>
+      <c r="N66" s="43" t="s">
+        <v>483</v>
+      </c>
+      <c r="O66" s="43" t="s">
+        <v>484</v>
+      </c>
+      <c r="P66" s="43" t="s">
+        <v>485</v>
+      </c>
+      <c r="Q66" s="43" t="s">
+        <v>486</v>
+      </c>
+      <c r="R66" s="43" t="s">
+        <v>487</v>
+      </c>
+      <c r="S66" s="16" t="s">
+        <v>488</v>
+      </c>
+      <c r="T66" s="43" t="s">
+        <v>489</v>
+      </c>
+      <c r="U66" s="43" t="s">
+        <v>490</v>
+      </c>
+      <c r="V66" s="16" t="s">
+        <v>446</v>
+      </c>
+      <c r="W66" s="16" t="s">
+        <v>423</v>
+      </c>
+      <c r="X66" s="16" t="s">
+        <v>325</v>
+      </c>
+      <c r="Y66" s="43" t="s">
+        <v>424</v>
+      </c>
+      <c r="Z66" s="16" t="s">
+        <v>425</v>
+      </c>
+      <c r="AA66" s="43" t="s">
+        <v>426</v>
+      </c>
+      <c r="AB66" s="43" t="s">
+        <v>427</v>
+      </c>
+      <c r="AC66" s="2" t="s">
+        <v>491</v>
+      </c>
+      <c r="AD66" s="2" t="s">
+        <v>428</v>
+      </c>
+      <c r="AE66" s="2" t="s">
+        <v>466</v>
+      </c>
+      <c r="AF66" s="2" t="s">
+        <v>492</v>
+      </c>
+      <c r="AG66" s="2" t="s">
+        <v>325</v>
+      </c>
+      <c r="AH66" s="2" t="s">
+        <v>432</v>
+      </c>
+      <c r="AI66" s="2" t="s">
+        <v>493</v>
+      </c>
+      <c r="AJ66" s="2" t="s">
+        <v>434</v>
+      </c>
+      <c r="AK66" s="2" t="s">
+        <v>435</v>
+      </c>
       <c r="AL66" s="3"/>
       <c r="AM66" s="3"/>
       <c r="AN66" s="3"/>
       <c r="AO66" s="3"/>
       <c r="AP66" s="3"/>
     </row>
-    <row r="67" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A67" s="2"/>
+    <row r="67" spans="1:42" ht="197.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A67" s="51" t="s">
+        <v>494</v>
+      </c>
       <c r="B67" s="2"/>
-      <c r="C67" s="2"/>
-      <c r="D67" s="2"/>
-      <c r="E67" s="2"/>
-      <c r="F67" s="2"/>
-      <c r="G67" s="2"/>
-      <c r="H67" s="2"/>
-      <c r="I67" s="2"/>
-      <c r="J67" s="2"/>
-      <c r="K67" s="2"/>
-      <c r="L67" s="2"/>
-      <c r="M67" s="16"/>
-      <c r="N67" s="16"/>
-      <c r="O67" s="16"/>
-      <c r="P67" s="16"/>
-      <c r="Q67" s="16"/>
-      <c r="R67" s="16"/>
-      <c r="S67" s="16"/>
-      <c r="T67" s="16"/>
-      <c r="U67" s="16"/>
-      <c r="V67" s="16"/>
-      <c r="W67" s="16"/>
-      <c r="X67" s="16"/>
-      <c r="Y67" s="16"/>
-      <c r="Z67" s="16"/>
-      <c r="AA67" s="16"/>
-      <c r="AB67" s="16"/>
-      <c r="AC67" s="3"/>
-      <c r="AD67" s="3"/>
+      <c r="C67" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="D67" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="E67" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="F67" s="26" t="s">
+        <v>35</v>
+      </c>
+      <c r="G67" s="20" t="s">
+        <v>36</v>
+      </c>
+      <c r="H67" s="47" t="s">
+        <v>321</v>
+      </c>
+      <c r="I67" s="2" t="s">
+        <v>355</v>
+      </c>
+      <c r="J67" s="2" t="s">
+        <v>356</v>
+      </c>
+      <c r="K67" s="2" t="s">
+        <v>357</v>
+      </c>
+      <c r="L67" s="2" t="s">
+        <v>495</v>
+      </c>
+      <c r="M67" s="43" t="s">
+        <v>496</v>
+      </c>
+      <c r="N67" s="43" t="s">
+        <v>497</v>
+      </c>
+      <c r="O67" s="43" t="s">
+        <v>407</v>
+      </c>
+      <c r="P67" s="43" t="s">
+        <v>408</v>
+      </c>
+      <c r="Q67" s="43" t="s">
+        <v>498</v>
+      </c>
+      <c r="R67" s="43" t="s">
+        <v>499</v>
+      </c>
+      <c r="S67" s="16" t="s">
+        <v>500</v>
+      </c>
+      <c r="T67" s="43" t="s">
+        <v>501</v>
+      </c>
+      <c r="U67" s="43" t="s">
+        <v>502</v>
+      </c>
+      <c r="V67" s="43" t="s">
+        <v>503</v>
+      </c>
+      <c r="W67" s="43" t="s">
+        <v>504</v>
+      </c>
+      <c r="X67" s="43" t="s">
+        <v>505</v>
+      </c>
+      <c r="Y67" s="16" t="s">
+        <v>506</v>
+      </c>
+      <c r="Z67" s="43" t="s">
+        <v>325</v>
+      </c>
+      <c r="AA67" s="43" t="s">
+        <v>432</v>
+      </c>
+      <c r="AB67" s="43" t="s">
+        <v>507</v>
+      </c>
+      <c r="AC67" s="2" t="s">
+        <v>434</v>
+      </c>
+      <c r="AD67" s="2" t="s">
+        <v>435</v>
+      </c>
       <c r="AE67" s="3"/>
       <c r="AF67" s="3"/>
       <c r="AG67" s="3"/>
@@ -8495,32 +9211,80 @@
       <c r="AO67" s="3"/>
       <c r="AP67" s="3"/>
     </row>
-    <row r="68" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A68" s="2"/>
+    <row r="68" spans="1:42" ht="195" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A68" s="2" t="s">
+        <v>510</v>
+      </c>
       <c r="B68" s="2"/>
-      <c r="C68" s="2"/>
-      <c r="D68" s="2"/>
-      <c r="E68" s="2"/>
-      <c r="F68" s="2"/>
-      <c r="G68" s="2"/>
-      <c r="H68" s="2"/>
-      <c r="I68" s="2"/>
-      <c r="J68" s="2"/>
-      <c r="K68" s="2"/>
-      <c r="L68" s="2"/>
-      <c r="M68" s="16"/>
-      <c r="N68" s="16"/>
-      <c r="O68" s="16"/>
-      <c r="P68" s="16"/>
-      <c r="Q68" s="16"/>
-      <c r="R68" s="16"/>
-      <c r="S68" s="16"/>
-      <c r="T68" s="16"/>
-      <c r="U68" s="16"/>
-      <c r="V68" s="16"/>
-      <c r="W68" s="16"/>
-      <c r="X68" s="16"/>
-      <c r="Y68" s="16"/>
+      <c r="C68" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="D68" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="E68" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="F68" s="26" t="s">
+        <v>35</v>
+      </c>
+      <c r="G68" s="20" t="s">
+        <v>36</v>
+      </c>
+      <c r="H68" s="47" t="s">
+        <v>321</v>
+      </c>
+      <c r="I68" s="2" t="s">
+        <v>402</v>
+      </c>
+      <c r="J68" s="2" t="s">
+        <v>403</v>
+      </c>
+      <c r="K68" s="2" t="s">
+        <v>511</v>
+      </c>
+      <c r="L68" s="2" t="s">
+        <v>512</v>
+      </c>
+      <c r="M68" s="16" t="s">
+        <v>513</v>
+      </c>
+      <c r="N68" s="43" t="s">
+        <v>514</v>
+      </c>
+      <c r="O68" s="43" t="s">
+        <v>515</v>
+      </c>
+      <c r="P68" s="43" t="s">
+        <v>516</v>
+      </c>
+      <c r="Q68" s="43" t="s">
+        <v>517</v>
+      </c>
+      <c r="R68" s="43" t="s">
+        <v>518</v>
+      </c>
+      <c r="S68" s="43" t="s">
+        <v>519</v>
+      </c>
+      <c r="T68" s="43" t="s">
+        <v>520</v>
+      </c>
+      <c r="U68" s="43" t="s">
+        <v>521</v>
+      </c>
+      <c r="V68" s="43" t="s">
+        <v>522</v>
+      </c>
+      <c r="W68" s="43" t="s">
+        <v>523</v>
+      </c>
+      <c r="X68" s="43" t="s">
+        <v>524</v>
+      </c>
+      <c r="Y68" s="16" t="s">
+        <v>525</v>
+      </c>
       <c r="Z68" s="16"/>
       <c r="AA68" s="16"/>
       <c r="AB68" s="16"/>

</xml_diff>

<commit_message>
modificacion de nombres y estructuracion de excel 002
</commit_message>
<xml_diff>
--- a/src/test/resources/Descriptions/DC_AUT_002_CashManagmentTest.xlsx
+++ b/src/test/resources/Descriptions/DC_AUT_002_CashManagmentTest.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20395"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FEEB48A-069C-4FB7-85D6-E45DA1978238}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BDCFD34-2EAF-4CFC-8232-E3E0B649EA96}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1655" uniqueCount="526">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1760" uniqueCount="557">
   <si>
     <t>Escenario</t>
   </si>
@@ -2812,7 +2812,148 @@
     <t>El usuario valida que se muestre la opción "Ver consolidado"||El sistema muestra la opción "Ver consolidado" de forma correcta como hipervínculo.</t>
   </si>
   <si>
-    <t>El usuario valida que se muestre el botón de Descarga.</t>
+    <t>El usuario valida que se muestre el botón de Descarga.||El sistema muestra el botón de "Descarga" de forma correcta.</t>
+  </si>
+  <si>
+    <t>El usuario valida que se muestre la columna "Número de autorización".||El sistema muestra la columna "Número de autorización" de forma correcta.</t>
+  </si>
+  <si>
+    <t>El usuario valida que se muestre la columna "Transacción".||El sistema muestra la columna "Transacción" de forma correcta.</t>
+  </si>
+  <si>
+    <t>El usuario valida que se muestre la columna "Monto".||El sistema muestra la columna "Monto" del movimiento con el siguiente formato:
+Signo $
+Separación de miles y millones con separador de coma (,)
+Signo de punto para decimales (.)
+2 decimales
+Se muestra el valor positivo si se trata de un Abono.
+Se muestra el valor negativo si se trata de un Cargo.</t>
+  </si>
+  <si>
+    <t>El usuario valida que se muestre la columna opciones (…).||El sistema la columna opciones (…) de forma correcta.</t>
+  </si>
+  <si>
+    <t>El usuario indica una fecha fin en el campo de búsqueda "Seleccione fecha fin".||El sistema muestra la fecha fin de forma correcta y el resultado de la búsqueda de movimientos en la siguiente tabla:
+Columna "Fecha"
+Columna "Número de autorización"
+Columna "Transacción"
+Columna "Monto"
+Columna "Tipo de operación"</t>
+  </si>
+  <si>
+    <t>TC_002_68_administradorConsulta</t>
+  </si>
+  <si>
+    <t>El usuario valida el campo "Identificación cliente".||El sistema muestra la identificación del cliente de forma correcta.</t>
+  </si>
+  <si>
+    <t>El usuario valida el Nombre de cliente.||El sistema muestra el nombre del cliente de forma correcta.</t>
+  </si>
+  <si>
+    <t>El usuario valida el estado de la cuenta.||El sistema muestra el estado de la cuenta en la parte superior derecha como "ACTIVA".</t>
+  </si>
+  <si>
+    <t>El usuario valida que se muestre la columna "Saldo total".||El sistema muestra la columna "Saldo total" de forma correcta con formato de moneda:
+Signo $
+Separación de miles y millones con separador de coma (,)
+Signo de punto para decimales (.)
+2 decimales</t>
+  </si>
+  <si>
+    <t>El usuario valida que se muestre la columna "Saldo disponible"||El sistema muestra la columna "Saldo disponible" de forma correcta con formato de moneda:
+Signo $
+Separación de miles y millones con separador de coma (,)
+Signo de punto para decimales (.)
+2 decimales</t>
+  </si>
+  <si>
+    <t>El usuario valida que se muestre la columna "Saldo salvo buen cobro"||El sistema muestra la columna "Saldo salvo buen cobro" de forma correcta con formato de moneda:
+Signo $
+Separación de miles y millones con separador de coma (,)
+Signo de punto para decimales (.)
+2 decimales</t>
+  </si>
+  <si>
+    <t>El usuario valida que se muestre la columna "Saldo límite de sobregiro"||El sistema muestra la columna "Saldo límite de sobregiro" de forma correcta con formato de moneda:
+Signo $
+Separación de miles y millones con separador de coma (,)
+Signo de punto para decimales (.)
+2 decimales</t>
+  </si>
+  <si>
+    <t>El usuario valida que se muestre el campo "Alias".||El sistema muestra el campo Alias de forma correcta.</t>
+  </si>
+  <si>
+    <t>El usuario valida que se muestre la columna "Descripción".||El sistema muestra la columna "Descripción" con la descripción del movimiento.</t>
+  </si>
+  <si>
+    <t>El usuario valida que se muestre la columna "Saldo final".||El sistema muestra la columna "Monto" del movimiento con el siguiente formato:
+Signo $
+Separación de miles y millones con separador de coma (,)
+Signo de punto para decimales (.)
+2 decimales</t>
+  </si>
+  <si>
+    <t>El usuario indica una fecha fin en el campo de búsqueda "Seleccione fecha fin".||El sistema muestra la fecha fin de forma correcta y el resultado de la búsqueda de movimientos en la siguiente tabla:
+Columna "Fecha del movimiento"
+Columna "Tipo de operación"
+Columna "Descripción"
+Columna "Monto"
+Columna "Saldo final"</t>
+  </si>
+  <si>
+    <t>TC_002_69_administradorConsulta</t>
+  </si>
+  <si>
+    <t>TC_002_70_administradorConsulta</t>
+  </si>
+  <si>
+    <t>El usuario valida el total de cuentas mostradas entre paréntesis en la sección "LÍNEA OPERATIVA CONSOLIDADOS".||El sistema muestra el total de créditos de Línea Operativa de forma correcta.</t>
+  </si>
+  <si>
+    <t>El usuario da clic en el menú "Linea operativa"||El sistema muestra la lista de créditos de Línea Operativa y debe coincidir con el total de cuentas mostradas en el Dashboard en la sección "LÍNEA OPERATIVA CONSOLIDADOS".</t>
+  </si>
+  <si>
+    <t>El usuario da clic en la opción "Ver consolidado"||El sistema muestra la sección "LÍNEA OPERATIVA CONSOLIDADOS" con el número total de cuentas indicadas entre paréntesis y debe coincidir con el total de cuentas mostradas en el Dashboard en la sección "LÍNEA OPERATIVA CONSOLIDADOS".</t>
+  </si>
+  <si>
+    <t>El usuario valida el monto mostrado en el campo "Saldo total del crédito".||El sistema debe mostrar el mismo monto que el mostrado en el Dashboard en la sección "LÍNEA OPERATIVA CONSOLIDADOS"</t>
+  </si>
+  <si>
+    <t>El usuario valida el formato mostrado en el campo "Saldo total del crédito".||El sistema muestra el campo "Saldo total del crédito" de forma correcta con el siguiente formato:
+Formato de moneda con signo $
+Separación de miles y millones con separador de coma (,)
+Signo de punto para decimales (.)
+2 decimales</t>
+  </si>
+  <si>
+    <t>El usuario valida el monto mostrado en el campo "Saldo total del crédito".||El sistema debe mostrar el mismo monto que la suma de las cuentas de la columna "Saldo total del crédito".</t>
+  </si>
+  <si>
+    <t>El usuario valida el monto mostrado en el campo "Capital disponible".||El sistema debe mostrar el mismo monto que el mostrado en el Dashboard en la sección "LÍNEA OPERATIVA CONSOLIDADOS"</t>
+  </si>
+  <si>
+    <t>El usuario valida el formato mostrado en el campo "Capital disponible".||El sistema muestra el campo "Capital disponible" de forma correcta con el siguiente formato:
+Formato de moneda con signo $
+Separación de miles y millones con separador de coma (,)
+Signo de punto para decimales (.)
+2 decimales</t>
+  </si>
+  <si>
+    <t>El usuario valida el monto mostrado en el campo "Capital disponible".||El sistema debe mostrar el mismo monto que la suma de las cuentas de la columna "Capital disponible".</t>
+  </si>
+  <si>
+    <t>El usuario valida el monto mostrado en el campo "Importe autorizado".||El sistema debe mostrar el mismo monto que el mostrado en el Dashboard en la sección "LÍNEA OPERATIVA CONSOLIDADOS"</t>
+  </si>
+  <si>
+    <t>El usuario valida el formato mostrado en el campo "Importe autorizado"||El sistema muestra el campo "Importe autorizado" de forma correcta con el siguiente formato:
+Formato de moneda con signo $
+Separación de miles y millones con separador de coma (,)
+Signo de punto para decimales (.)
+2 decimales</t>
+  </si>
+  <si>
+    <t>El usuario valida el monto mostrado en el campo "Importe autorizado".||El sistema debe mostrar el mismo monto que la suma de las cuentas de la columna "Importe autorizado".</t>
   </si>
 </sst>
 </file>
@@ -3590,8 +3731,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BC159"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="V66" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="Y68" sqref="Y68"/>
+    <sheetView tabSelected="1" topLeftCell="A51" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A54" sqref="A54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9285,61 +9426,161 @@
       <c r="Y68" s="16" t="s">
         <v>525</v>
       </c>
-      <c r="Z68" s="16"/>
-      <c r="AA68" s="16"/>
-      <c r="AB68" s="16"/>
-      <c r="AC68" s="3"/>
-      <c r="AD68" s="3"/>
-      <c r="AE68" s="3"/>
-      <c r="AF68" s="3"/>
-      <c r="AG68" s="3"/>
-      <c r="AH68" s="3"/>
-      <c r="AI68" s="3"/>
-      <c r="AJ68" s="3"/>
-      <c r="AK68" s="3"/>
-      <c r="AL68" s="3"/>
-      <c r="AM68" s="3"/>
-      <c r="AN68" s="3"/>
+      <c r="Z68" s="43" t="s">
+        <v>325</v>
+      </c>
+      <c r="AA68" s="43" t="s">
+        <v>424</v>
+      </c>
+      <c r="AB68" s="43" t="s">
+        <v>425</v>
+      </c>
+      <c r="AC68" s="3" t="s">
+        <v>525</v>
+      </c>
+      <c r="AD68" s="3" t="s">
+        <v>474</v>
+      </c>
+      <c r="AE68" s="2" t="s">
+        <v>526</v>
+      </c>
+      <c r="AF68" s="3" t="s">
+        <v>527</v>
+      </c>
+      <c r="AG68" s="3" t="s">
+        <v>528</v>
+      </c>
+      <c r="AH68" s="2" t="s">
+        <v>477</v>
+      </c>
+      <c r="AI68" s="3" t="s">
+        <v>529</v>
+      </c>
+      <c r="AJ68" s="2" t="s">
+        <v>325</v>
+      </c>
+      <c r="AK68" s="3" t="s">
+        <v>432</v>
+      </c>
+      <c r="AL68" s="2" t="s">
+        <v>530</v>
+      </c>
+      <c r="AM68" s="2" t="s">
+        <v>434</v>
+      </c>
+      <c r="AN68" s="2" t="s">
+        <v>435</v>
+      </c>
       <c r="AO68" s="3"/>
       <c r="AP68" s="3"/>
     </row>
-    <row r="69" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A69" s="2"/>
+    <row r="69" spans="1:42" ht="200.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A69" s="51" t="s">
+        <v>531</v>
+      </c>
       <c r="B69" s="2"/>
-      <c r="C69" s="2"/>
-      <c r="D69" s="2"/>
-      <c r="E69" s="2"/>
-      <c r="F69" s="2"/>
-      <c r="G69" s="2"/>
-      <c r="H69" s="2"/>
-      <c r="I69" s="2"/>
-      <c r="J69" s="2"/>
-      <c r="K69" s="2"/>
-      <c r="L69" s="2"/>
-      <c r="M69" s="16"/>
-      <c r="N69" s="16"/>
-      <c r="O69" s="16"/>
-      <c r="P69" s="16"/>
-      <c r="Q69" s="16"/>
-      <c r="R69" s="16"/>
-      <c r="S69" s="16"/>
-      <c r="T69" s="16"/>
-      <c r="U69" s="16"/>
-      <c r="V69" s="16"/>
-      <c r="W69" s="16"/>
-      <c r="X69" s="16"/>
-      <c r="Y69" s="16"/>
-      <c r="Z69" s="16"/>
-      <c r="AA69" s="16"/>
-      <c r="AB69" s="16"/>
-      <c r="AC69" s="3"/>
-      <c r="AD69" s="3"/>
-      <c r="AE69" s="3"/>
-      <c r="AF69" s="3"/>
-      <c r="AG69" s="3"/>
-      <c r="AH69" s="3"/>
-      <c r="AI69" s="3"/>
-      <c r="AJ69" s="3"/>
+      <c r="C69" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="D69" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="E69" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="F69" s="26" t="s">
+        <v>35</v>
+      </c>
+      <c r="G69" s="20" t="s">
+        <v>36</v>
+      </c>
+      <c r="H69" s="47" t="s">
+        <v>321</v>
+      </c>
+      <c r="I69" s="2" t="s">
+        <v>364</v>
+      </c>
+      <c r="J69" s="2" t="s">
+        <v>370</v>
+      </c>
+      <c r="K69" s="2" t="s">
+        <v>365</v>
+      </c>
+      <c r="L69" s="2" t="s">
+        <v>532</v>
+      </c>
+      <c r="M69" s="43" t="s">
+        <v>436</v>
+      </c>
+      <c r="N69" s="43" t="s">
+        <v>533</v>
+      </c>
+      <c r="O69" s="43" t="s">
+        <v>534</v>
+      </c>
+      <c r="P69" s="43" t="s">
+        <v>535</v>
+      </c>
+      <c r="Q69" s="43" t="s">
+        <v>536</v>
+      </c>
+      <c r="R69" s="43" t="s">
+        <v>537</v>
+      </c>
+      <c r="S69" s="43" t="s">
+        <v>538</v>
+      </c>
+      <c r="T69" s="43" t="s">
+        <v>539</v>
+      </c>
+      <c r="U69" s="43" t="s">
+        <v>423</v>
+      </c>
+      <c r="V69" s="43" t="s">
+        <v>325</v>
+      </c>
+      <c r="W69" s="16" t="s">
+        <v>424</v>
+      </c>
+      <c r="X69" s="43" t="s">
+        <v>425</v>
+      </c>
+      <c r="Y69" s="16" t="s">
+        <v>426</v>
+      </c>
+      <c r="Z69" s="43" t="s">
+        <v>427</v>
+      </c>
+      <c r="AA69" s="43" t="s">
+        <v>477</v>
+      </c>
+      <c r="AB69" s="43" t="s">
+        <v>540</v>
+      </c>
+      <c r="AC69" s="2" t="s">
+        <v>528</v>
+      </c>
+      <c r="AD69" s="3" t="s">
+        <v>541</v>
+      </c>
+      <c r="AE69" s="2" t="s">
+        <v>529</v>
+      </c>
+      <c r="AF69" s="3" t="s">
+        <v>325</v>
+      </c>
+      <c r="AG69" s="2" t="s">
+        <v>432</v>
+      </c>
+      <c r="AH69" s="2" t="s">
+        <v>542</v>
+      </c>
+      <c r="AI69" s="3" t="s">
+        <v>434</v>
+      </c>
+      <c r="AJ69" s="3" t="s">
+        <v>435</v>
+      </c>
       <c r="AK69" s="3"/>
       <c r="AL69" s="3"/>
       <c r="AM69" s="3"/>
@@ -9347,43 +9588,113 @@
       <c r="AO69" s="3"/>
       <c r="AP69" s="3"/>
     </row>
-    <row r="70" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A70" s="2"/>
+    <row r="70" spans="1:42" ht="203.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A70" s="51" t="s">
+        <v>543</v>
+      </c>
       <c r="B70" s="2"/>
-      <c r="C70" s="2"/>
-      <c r="D70" s="2"/>
-      <c r="E70" s="2"/>
-      <c r="F70" s="2"/>
-      <c r="G70" s="2"/>
-      <c r="H70" s="2"/>
-      <c r="I70" s="2"/>
-      <c r="J70" s="2"/>
-      <c r="K70" s="2"/>
-      <c r="L70" s="2"/>
-      <c r="M70" s="16"/>
-      <c r="N70" s="16"/>
-      <c r="O70" s="16"/>
-      <c r="P70" s="16"/>
-      <c r="Q70" s="16"/>
-      <c r="R70" s="16"/>
-      <c r="S70" s="16"/>
-      <c r="T70" s="16"/>
-      <c r="U70" s="16"/>
-      <c r="V70" s="16"/>
-      <c r="W70" s="16"/>
-      <c r="X70" s="16"/>
-      <c r="Y70" s="16"/>
-      <c r="Z70" s="16"/>
-      <c r="AA70" s="16"/>
-      <c r="AB70" s="16"/>
-      <c r="AC70" s="3"/>
-      <c r="AD70" s="3"/>
-      <c r="AE70" s="3"/>
-      <c r="AF70" s="3"/>
-      <c r="AG70" s="3"/>
-      <c r="AH70" s="3"/>
-      <c r="AI70" s="3"/>
-      <c r="AJ70" s="3"/>
+      <c r="C70" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="D70" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="E70" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="F70" s="26" t="s">
+        <v>35</v>
+      </c>
+      <c r="G70" s="20" t="s">
+        <v>36</v>
+      </c>
+      <c r="H70" s="47" t="s">
+        <v>321</v>
+      </c>
+      <c r="I70" s="2" t="s">
+        <v>368</v>
+      </c>
+      <c r="J70" s="2" t="s">
+        <v>369</v>
+      </c>
+      <c r="K70" s="2" t="s">
+        <v>371</v>
+      </c>
+      <c r="L70" s="2" t="s">
+        <v>532</v>
+      </c>
+      <c r="M70" s="43" t="s">
+        <v>436</v>
+      </c>
+      <c r="N70" s="43" t="s">
+        <v>533</v>
+      </c>
+      <c r="O70" s="43" t="s">
+        <v>534</v>
+      </c>
+      <c r="P70" s="43" t="s">
+        <v>535</v>
+      </c>
+      <c r="Q70" s="43" t="s">
+        <v>536</v>
+      </c>
+      <c r="R70" s="43" t="s">
+        <v>537</v>
+      </c>
+      <c r="S70" s="43" t="s">
+        <v>538</v>
+      </c>
+      <c r="T70" s="43" t="s">
+        <v>539</v>
+      </c>
+      <c r="U70" s="43" t="s">
+        <v>423</v>
+      </c>
+      <c r="V70" s="43" t="s">
+        <v>325</v>
+      </c>
+      <c r="W70" s="16" t="s">
+        <v>424</v>
+      </c>
+      <c r="X70" s="43" t="s">
+        <v>425</v>
+      </c>
+      <c r="Y70" s="43" t="s">
+        <v>525</v>
+      </c>
+      <c r="Z70" s="43" t="s">
+        <v>427</v>
+      </c>
+      <c r="AA70" s="43" t="s">
+        <v>477</v>
+      </c>
+      <c r="AB70" s="43" t="s">
+        <v>540</v>
+      </c>
+      <c r="AC70" s="2" t="s">
+        <v>528</v>
+      </c>
+      <c r="AD70" s="3" t="s">
+        <v>541</v>
+      </c>
+      <c r="AE70" s="2" t="s">
+        <v>529</v>
+      </c>
+      <c r="AF70" s="3" t="s">
+        <v>325</v>
+      </c>
+      <c r="AG70" s="2" t="s">
+        <v>432</v>
+      </c>
+      <c r="AH70" s="2" t="s">
+        <v>542</v>
+      </c>
+      <c r="AI70" s="3" t="s">
+        <v>434</v>
+      </c>
+      <c r="AJ70" s="3" t="s">
+        <v>435</v>
+      </c>
       <c r="AK70" s="3"/>
       <c r="AL70" s="3"/>
       <c r="AM70" s="3"/>
@@ -9391,28 +9702,68 @@
       <c r="AO70" s="3"/>
       <c r="AP70" s="3"/>
     </row>
-    <row r="71" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A71" s="2"/>
+    <row r="71" spans="1:42" ht="205.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A71" s="51" t="s">
+        <v>544</v>
+      </c>
       <c r="B71" s="2"/>
-      <c r="C71" s="2"/>
-      <c r="D71" s="2"/>
-      <c r="E71" s="2"/>
-      <c r="F71" s="2"/>
-      <c r="G71" s="2"/>
-      <c r="H71" s="2"/>
-      <c r="I71" s="2"/>
-      <c r="J71" s="2"/>
-      <c r="K71" s="2"/>
-      <c r="L71" s="2"/>
-      <c r="M71" s="16"/>
-      <c r="N71" s="16"/>
-      <c r="O71" s="16"/>
-      <c r="P71" s="16"/>
-      <c r="Q71" s="16"/>
-      <c r="R71" s="16"/>
-      <c r="S71" s="16"/>
-      <c r="T71" s="16"/>
-      <c r="U71" s="16"/>
+      <c r="C71" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="D71" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="E71" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="F71" s="26" t="s">
+        <v>35</v>
+      </c>
+      <c r="G71" s="20" t="s">
+        <v>36</v>
+      </c>
+      <c r="H71" s="2" t="s">
+        <v>545</v>
+      </c>
+      <c r="I71" s="2" t="s">
+        <v>321</v>
+      </c>
+      <c r="J71" s="2" t="s">
+        <v>546</v>
+      </c>
+      <c r="K71" s="2" t="s">
+        <v>524</v>
+      </c>
+      <c r="L71" s="2" t="s">
+        <v>547</v>
+      </c>
+      <c r="M71" s="16" t="s">
+        <v>548</v>
+      </c>
+      <c r="N71" s="43" t="s">
+        <v>549</v>
+      </c>
+      <c r="O71" s="16" t="s">
+        <v>550</v>
+      </c>
+      <c r="P71" s="43" t="s">
+        <v>551</v>
+      </c>
+      <c r="Q71" s="43" t="s">
+        <v>552</v>
+      </c>
+      <c r="R71" s="43" t="s">
+        <v>553</v>
+      </c>
+      <c r="S71" s="43" t="s">
+        <v>554</v>
+      </c>
+      <c r="T71" s="16" t="s">
+        <v>555</v>
+      </c>
+      <c r="U71" s="43" t="s">
+        <v>556</v>
+      </c>
       <c r="V71" s="16"/>
       <c r="W71" s="16"/>
       <c r="X71" s="16"/>
@@ -9435,7 +9786,7 @@
       <c r="AO71" s="3"/>
       <c r="AP71" s="3"/>
     </row>
-    <row r="72" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:42" ht="204.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" s="2"/>
       <c r="B72" s="2"/>
       <c r="C72" s="2"/>

</xml_diff>

<commit_message>
se agrego del 86 al 93 casos en excel002
</commit_message>
<xml_diff>
--- a/src/test/resources/Descriptions/DC_AUT_002_CashManagmentTest.xlsx
+++ b/src/test/resources/Descriptions/DC_AUT_002_CashManagmentTest.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20395"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BDCFD34-2EAF-4CFC-8232-E3E0B649EA96}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{655B4969-4AFA-4449-8FA4-A7E257196385}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1760" uniqueCount="557">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1912" uniqueCount="574">
   <si>
     <t>Escenario</t>
   </si>
@@ -2955,12 +2955,63 @@
   <si>
     <t>El usuario valida el monto mostrado en el campo "Importe autorizado".||El sistema debe mostrar el mismo monto que la suma de las cuentas de la columna "Importe autorizado".</t>
   </si>
+  <si>
+    <t>TC_002_86_administradorConsultaCuentasLineaOperativaCSV</t>
+  </si>
+  <si>
+    <t>El usuario da clic en la opción "Descarga".||El sistema muestra la página "Opciones de descarga" con las opciones "Manual" y "Plantilla".</t>
+  </si>
+  <si>
+    <t>TC_002_87_administradorConsultaCuentasPrestamosPersonalesTXT</t>
+  </si>
+  <si>
+    <t>El usuario habilita la opción "Archivo con encabezado"||El sistema permite habilitar el radio botton de forma correcta.</t>
+  </si>
+  <si>
+    <t>TC_002_88_administradorConsultaCuentasFondosInversionCSV</t>
+  </si>
+  <si>
+    <t>TC_002_89_administradorConsultaCreditosHipotecarioTXT</t>
+  </si>
+  <si>
+    <t>TC_002_90_administradorConsultaCuentasInversionCSV</t>
+  </si>
+  <si>
+    <t>TC_002_91_administradorConsultaCuentasTDCMXNTXT</t>
+  </si>
+  <si>
+    <t>TC_002_92_administradorConsultaCuentasChequeUSDCSV</t>
+  </si>
+  <si>
+    <t>El usuario da clic en la pestaña "Cuentas Cheque USD"||El sistema muestra la lista de Cuentas Cheque USD.</t>
+  </si>
+  <si>
+    <t>El usuario da clic en el botón "Descargar".||El sistema permite descargar el reporte de Créditos Hipotecarios en formato TXT de forma correcta.</t>
+  </si>
+  <si>
+    <t>El usuario da clic en el botón "Descargar".||El sistema permite descargar el reporte de cuentas de Inversión en formato CSV de forma correcta .</t>
+  </si>
+  <si>
+    <t>El usuario da clic en el botón "Descargar".||El sistema permite descargar el reporte de cuentas de Tarjetas de Crédito en formato TXT de forma correcta.</t>
+  </si>
+  <si>
+    <t>El usuario da clic en el botón "Descargar".||El sistema permite descargar el reporte de Cuentas Cheque USD de forma correcta en formato CSV .</t>
+  </si>
+  <si>
+    <t>TC_002_93_administradorConsultaCuentasChequeMXNTXT</t>
+  </si>
+  <si>
+    <t>El usuario valida las cuentas de cheques de la pestaña "Cuentas Cheque MXN"||El sistema muestra la lista de Cuentas Cheque MXN.</t>
+  </si>
+  <si>
+    <t>El usuario da clic en el botón "Descargar".||El sistema permite descargar el reporte de Cuenta Cheque MXN de forma correcta en formato TXT .</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2978,6 +3029,13 @@
     <font>
       <sz val="11"/>
       <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -3026,7 +3084,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="14">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -3197,12 +3255,23 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFDFE1E6"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -3354,6 +3423,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -3731,8 +3803,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BC159"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A51" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A54" sqref="A54"/>
+    <sheetView tabSelected="1" topLeftCell="N40" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="T94" sqref="T94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10182,131 +10254,499 @@
       <c r="AO86" s="3"/>
       <c r="AP86" s="3"/>
     </row>
-    <row r="87" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A87" s="2"/>
+    <row r="87" spans="1:42" ht="212.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A87" s="2" t="s">
+        <v>557</v>
+      </c>
       <c r="B87" s="2"/>
-      <c r="C87" s="2"/>
-      <c r="D87" s="2"/>
-      <c r="E87" s="2"/>
-      <c r="F87" s="2"/>
-      <c r="G87" s="2"/>
-      <c r="H87" s="2"/>
-      <c r="I87" s="2"/>
-      <c r="J87" s="2"/>
-      <c r="K87" s="2"/>
-      <c r="L87" s="2"/>
+      <c r="C87" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="D87" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="E87" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="F87" s="26" t="s">
+        <v>35</v>
+      </c>
+      <c r="G87" s="20" t="s">
+        <v>36</v>
+      </c>
+      <c r="H87" s="2" t="s">
+        <v>321</v>
+      </c>
+      <c r="I87" s="2" t="s">
+        <v>322</v>
+      </c>
+      <c r="J87" s="2" t="s">
+        <v>558</v>
+      </c>
+      <c r="K87" s="2" t="s">
+        <v>376</v>
+      </c>
+      <c r="L87" s="2" t="s">
+        <v>377</v>
+      </c>
+      <c r="M87" s="2" t="s">
+        <v>378</v>
+      </c>
+      <c r="N87" s="2" t="s">
+        <v>379</v>
+      </c>
+      <c r="O87" s="2" t="s">
+        <v>380</v>
+      </c>
+      <c r="P87" s="2" t="s">
+        <v>381</v>
+      </c>
+      <c r="Q87" s="2" t="s">
+        <v>382</v>
+      </c>
+      <c r="R87" s="2" t="s">
+        <v>383</v>
+      </c>
+      <c r="S87" s="2" t="s">
+        <v>384</v>
+      </c>
+      <c r="T87" s="2" t="s">
+        <v>385</v>
+      </c>
       <c r="AO87" s="3"/>
       <c r="AP87" s="3"/>
     </row>
-    <row r="88" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A88" s="2"/>
+    <row r="88" spans="1:42" ht="214.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A88" s="2" t="s">
+        <v>559</v>
+      </c>
       <c r="B88" s="2"/>
-      <c r="C88" s="2"/>
-      <c r="D88" s="2"/>
-      <c r="E88" s="2"/>
-      <c r="F88" s="2"/>
-      <c r="G88" s="2"/>
-      <c r="H88" s="2"/>
-      <c r="I88" s="2"/>
-      <c r="J88" s="2"/>
-      <c r="K88" s="2"/>
-      <c r="L88" s="2"/>
+      <c r="C88" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="D88" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="E88" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="F88" s="26" t="s">
+        <v>35</v>
+      </c>
+      <c r="G88" s="20" t="s">
+        <v>36</v>
+      </c>
+      <c r="H88" s="2" t="s">
+        <v>321</v>
+      </c>
+      <c r="I88" s="2" t="s">
+        <v>340</v>
+      </c>
+      <c r="J88" s="52" t="s">
+        <v>558</v>
+      </c>
+      <c r="K88" s="2" t="s">
+        <v>376</v>
+      </c>
+      <c r="L88" s="2" t="s">
+        <v>377</v>
+      </c>
+      <c r="M88" s="2" t="s">
+        <v>388</v>
+      </c>
+      <c r="N88" s="2" t="s">
+        <v>379</v>
+      </c>
+      <c r="O88" s="2" t="s">
+        <v>389</v>
+      </c>
+      <c r="P88" s="2" t="s">
+        <v>381</v>
+      </c>
+      <c r="Q88" s="2" t="s">
+        <v>560</v>
+      </c>
+      <c r="R88" s="2" t="s">
+        <v>383</v>
+      </c>
+      <c r="S88" s="2" t="s">
+        <v>384</v>
+      </c>
+      <c r="T88" s="2" t="s">
+        <v>390</v>
+      </c>
       <c r="AO88" s="3"/>
       <c r="AP88" s="3"/>
     </row>
-    <row r="89" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A89" s="2"/>
+    <row r="89" spans="1:42" ht="210" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A89" s="2" t="s">
+        <v>561</v>
+      </c>
       <c r="B89" s="2"/>
-      <c r="C89" s="2"/>
-      <c r="D89" s="2"/>
-      <c r="E89" s="2"/>
-      <c r="F89" s="2"/>
-      <c r="G89" s="2"/>
-      <c r="H89" s="2"/>
-      <c r="I89" s="2"/>
-      <c r="J89" s="2"/>
-      <c r="K89" s="2"/>
-      <c r="L89" s="2"/>
+      <c r="C89" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="D89" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="E89" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="F89" s="26" t="s">
+        <v>35</v>
+      </c>
+      <c r="G89" s="20" t="s">
+        <v>36</v>
+      </c>
+      <c r="H89" s="2" t="s">
+        <v>321</v>
+      </c>
+      <c r="I89" s="2" t="s">
+        <v>345</v>
+      </c>
+      <c r="J89" s="52" t="s">
+        <v>558</v>
+      </c>
+      <c r="K89" s="2" t="s">
+        <v>376</v>
+      </c>
+      <c r="L89" s="2" t="s">
+        <v>377</v>
+      </c>
+      <c r="M89" s="2" t="s">
+        <v>378</v>
+      </c>
+      <c r="N89" s="2" t="s">
+        <v>379</v>
+      </c>
+      <c r="O89" s="2" t="s">
+        <v>393</v>
+      </c>
+      <c r="P89" s="2" t="s">
+        <v>381</v>
+      </c>
+      <c r="Q89" s="2" t="s">
+        <v>560</v>
+      </c>
+      <c r="R89" s="2" t="s">
+        <v>383</v>
+      </c>
+      <c r="S89" s="2" t="s">
+        <v>384</v>
+      </c>
+      <c r="T89" s="2" t="s">
+        <v>394</v>
+      </c>
       <c r="AO89" s="3"/>
       <c r="AP89" s="3"/>
     </row>
-    <row r="90" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A90" s="2"/>
+    <row r="90" spans="1:42" ht="213" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A90" s="2" t="s">
+        <v>562</v>
+      </c>
       <c r="B90" s="2"/>
-      <c r="C90" s="2"/>
-      <c r="D90" s="2"/>
-      <c r="E90" s="2"/>
-      <c r="F90" s="2"/>
-      <c r="G90" s="2"/>
-      <c r="H90" s="2"/>
-      <c r="I90" s="2"/>
-      <c r="J90" s="2"/>
-      <c r="K90" s="2"/>
-      <c r="L90" s="2"/>
+      <c r="C90" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="D90" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="E90" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="F90" s="26" t="s">
+        <v>35</v>
+      </c>
+      <c r="G90" s="20" t="s">
+        <v>36</v>
+      </c>
+      <c r="H90" s="2" t="s">
+        <v>321</v>
+      </c>
+      <c r="I90" s="2" t="s">
+        <v>350</v>
+      </c>
+      <c r="J90" s="52" t="s">
+        <v>558</v>
+      </c>
+      <c r="K90" s="2" t="s">
+        <v>376</v>
+      </c>
+      <c r="L90" s="2" t="s">
+        <v>377</v>
+      </c>
+      <c r="M90" s="2" t="s">
+        <v>388</v>
+      </c>
+      <c r="N90" s="2" t="s">
+        <v>379</v>
+      </c>
+      <c r="O90" s="2" t="s">
+        <v>397</v>
+      </c>
+      <c r="P90" s="2" t="s">
+        <v>381</v>
+      </c>
+      <c r="Q90" s="2" t="s">
+        <v>560</v>
+      </c>
+      <c r="R90" s="2" t="s">
+        <v>383</v>
+      </c>
+      <c r="S90" s="2" t="s">
+        <v>384</v>
+      </c>
+      <c r="T90" s="2" t="s">
+        <v>567</v>
+      </c>
       <c r="AO90" s="3"/>
       <c r="AP90" s="3"/>
     </row>
-    <row r="91" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A91" s="2"/>
+    <row r="91" spans="1:42" ht="212.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A91" s="2" t="s">
+        <v>563</v>
+      </c>
       <c r="B91" s="2"/>
-      <c r="C91" s="2"/>
-      <c r="D91" s="2"/>
-      <c r="E91" s="2"/>
-      <c r="F91" s="2"/>
-      <c r="G91" s="2"/>
-      <c r="H91" s="2"/>
-      <c r="I91" s="2"/>
-      <c r="J91" s="2"/>
-      <c r="K91" s="2"/>
-      <c r="L91" s="2"/>
+      <c r="C91" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="D91" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="E91" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="F91" s="26" t="s">
+        <v>35</v>
+      </c>
+      <c r="G91" s="20" t="s">
+        <v>36</v>
+      </c>
+      <c r="H91" s="2" t="s">
+        <v>321</v>
+      </c>
+      <c r="I91" s="2" t="s">
+        <v>355</v>
+      </c>
+      <c r="J91" s="52" t="s">
+        <v>558</v>
+      </c>
+      <c r="K91" s="2" t="s">
+        <v>376</v>
+      </c>
+      <c r="L91" s="2" t="s">
+        <v>377</v>
+      </c>
+      <c r="M91" s="2" t="s">
+        <v>378</v>
+      </c>
+      <c r="N91" s="2" t="s">
+        <v>379</v>
+      </c>
+      <c r="O91" s="2" t="s">
+        <v>400</v>
+      </c>
+      <c r="P91" s="2" t="s">
+        <v>381</v>
+      </c>
+      <c r="Q91" s="2" t="s">
+        <v>560</v>
+      </c>
+      <c r="R91" s="2" t="s">
+        <v>383</v>
+      </c>
+      <c r="S91" s="2" t="s">
+        <v>384</v>
+      </c>
+      <c r="T91" s="2" t="s">
+        <v>568</v>
+      </c>
       <c r="AO91" s="3"/>
       <c r="AP91" s="3"/>
     </row>
-    <row r="92" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A92" s="2"/>
+    <row r="92" spans="1:42" ht="210.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A92" s="2" t="s">
+        <v>564</v>
+      </c>
       <c r="B92" s="2"/>
-      <c r="C92" s="2"/>
-      <c r="D92" s="2"/>
-      <c r="E92" s="2"/>
-      <c r="F92" s="2"/>
-      <c r="G92" s="2"/>
-      <c r="H92" s="2"/>
-      <c r="I92" s="2"/>
-      <c r="J92" s="2"/>
-      <c r="K92" s="2"/>
-      <c r="L92" s="2"/>
+      <c r="C92" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="D92" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="E92" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="F92" s="26" t="s">
+        <v>35</v>
+      </c>
+      <c r="G92" s="20" t="s">
+        <v>36</v>
+      </c>
+      <c r="H92" s="2" t="s">
+        <v>321</v>
+      </c>
+      <c r="I92" s="2" t="s">
+        <v>402</v>
+      </c>
+      <c r="J92" s="52" t="s">
+        <v>558</v>
+      </c>
+      <c r="K92" s="2" t="s">
+        <v>376</v>
+      </c>
+      <c r="L92" s="2" t="s">
+        <v>377</v>
+      </c>
+      <c r="M92" s="2" t="s">
+        <v>388</v>
+      </c>
+      <c r="N92" s="2" t="s">
+        <v>379</v>
+      </c>
+      <c r="O92" s="2" t="s">
+        <v>380</v>
+      </c>
+      <c r="P92" s="2" t="s">
+        <v>381</v>
+      </c>
+      <c r="Q92" s="2" t="s">
+        <v>560</v>
+      </c>
+      <c r="R92" s="2" t="s">
+        <v>383</v>
+      </c>
+      <c r="S92" s="2" t="s">
+        <v>384</v>
+      </c>
+      <c r="T92" s="2" t="s">
+        <v>569</v>
+      </c>
       <c r="AO92" s="3"/>
       <c r="AP92" s="3"/>
     </row>
-    <row r="93" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A93" s="2"/>
+    <row r="93" spans="1:42" ht="213" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A93" s="2" t="s">
+        <v>565</v>
+      </c>
       <c r="B93" s="2"/>
-      <c r="C93" s="2"/>
-      <c r="D93" s="2"/>
-      <c r="E93" s="2"/>
-      <c r="F93" s="2"/>
-      <c r="G93" s="2"/>
-      <c r="H93" s="2"/>
-      <c r="I93" s="2"/>
-      <c r="J93" s="2"/>
-      <c r="K93" s="2"/>
-      <c r="L93" s="2"/>
+      <c r="C93" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="D93" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="E93" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="F93" s="26" t="s">
+        <v>35</v>
+      </c>
+      <c r="G93" s="20" t="s">
+        <v>36</v>
+      </c>
+      <c r="H93" s="2" t="s">
+        <v>321</v>
+      </c>
+      <c r="I93" s="2" t="s">
+        <v>566</v>
+      </c>
+      <c r="J93" s="52" t="s">
+        <v>558</v>
+      </c>
+      <c r="K93" s="2" t="s">
+        <v>376</v>
+      </c>
+      <c r="L93" s="2" t="s">
+        <v>377</v>
+      </c>
+      <c r="M93" s="2" t="s">
+        <v>378</v>
+      </c>
+      <c r="N93" s="2" t="s">
+        <v>379</v>
+      </c>
+      <c r="O93" s="2" t="s">
+        <v>389</v>
+      </c>
+      <c r="P93" s="2" t="s">
+        <v>381</v>
+      </c>
+      <c r="Q93" s="2" t="s">
+        <v>560</v>
+      </c>
+      <c r="R93" s="2" t="s">
+        <v>383</v>
+      </c>
+      <c r="S93" s="2" t="s">
+        <v>384</v>
+      </c>
+      <c r="T93" s="2" t="s">
+        <v>570</v>
+      </c>
       <c r="AO93" s="3"/>
       <c r="AP93" s="3"/>
     </row>
-    <row r="94" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A94" s="2"/>
+    <row r="94" spans="1:42" ht="215.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A94" s="2" t="s">
+        <v>571</v>
+      </c>
       <c r="B94" s="2"/>
-      <c r="C94" s="2"/>
-      <c r="D94" s="2"/>
-      <c r="E94" s="2"/>
-      <c r="F94" s="2"/>
-      <c r="G94" s="2"/>
-      <c r="H94" s="2"/>
-      <c r="I94" s="2"/>
-      <c r="J94" s="2"/>
-      <c r="K94" s="2"/>
-      <c r="L94" s="2"/>
+      <c r="C94" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="D94" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="E94" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="F94" s="26" t="s">
+        <v>35</v>
+      </c>
+      <c r="G94" s="20" t="s">
+        <v>36</v>
+      </c>
+      <c r="H94" s="2" t="s">
+        <v>321</v>
+      </c>
+      <c r="I94" s="2" t="s">
+        <v>572</v>
+      </c>
+      <c r="J94" s="52" t="s">
+        <v>558</v>
+      </c>
+      <c r="K94" s="2" t="s">
+        <v>376</v>
+      </c>
+      <c r="L94" s="2" t="s">
+        <v>377</v>
+      </c>
+      <c r="M94" s="2" t="s">
+        <v>388</v>
+      </c>
+      <c r="N94" s="2" t="s">
+        <v>379</v>
+      </c>
+      <c r="O94" s="2" t="s">
+        <v>393</v>
+      </c>
+      <c r="P94" s="2" t="s">
+        <v>381</v>
+      </c>
+      <c r="Q94" s="2" t="s">
+        <v>560</v>
+      </c>
+      <c r="R94" s="2" t="s">
+        <v>383</v>
+      </c>
+      <c r="S94" s="2" t="s">
+        <v>384</v>
+      </c>
+      <c r="T94" s="2" t="s">
+        <v>573</v>
+      </c>
       <c r="AO94" s="3"/>
       <c r="AP94" s="3"/>
     </row>

</xml_diff>

<commit_message>
refactorización y validaciones de "CashManagment"
</commit_message>
<xml_diff>
--- a/src/test/resources/Descriptions/DC_AUT_002_CashManagmentTest.xlsx
+++ b/src/test/resources/Descriptions/DC_AUT_002_CashManagmentTest.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20395"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{655B4969-4AFA-4449-8FA4-A7E257196385}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96ED278F-C8E3-4663-93CD-22B9A9F42264}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1912" uniqueCount="574">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2264" uniqueCount="744">
   <si>
     <t>Escenario</t>
   </si>
@@ -3005,6 +3005,733 @@
   </si>
   <si>
     <t>El usuario da clic en el botón "Descargar".||El sistema permite descargar el reporte de Cuenta Cheque MXN de forma correcta en formato TXT .</t>
+  </si>
+  <si>
+    <t>TC_002_78_administradorConsultaCuentasLineaOperativaBD</t>
+  </si>
+  <si>
+    <t>El usuario ingresa el siguiente dato:
+Nombre de usuario.||El sistema permite ingresar el nombre de usuario de forma correcta.</t>
+  </si>
+  <si>
+    <t>El usuario ingresa el siguiente dato:
+Contraseña.||El sistema permite ingresar la contraseña de forma correcta.</t>
+  </si>
+  <si>
+    <t>El usuario ingresa el siguiente dato:
+Token.||El sistema permite ingresar el token de forma correcta.</t>
+  </si>
+  <si>
+    <t>El usuario da clic en el botón "Ingresar".||El sistema muestra la página principal de CCOP "Resumen consolidado de productos".</t>
+  </si>
+  <si>
+    <t>El usuario da clic en la pestaña "Productos y servicios".||El sistema muestra la página "Cuentas".</t>
+  </si>
+  <si>
+    <t>El usuario da clic en el menú "Linea Operativa".||El sistema muestra la lista de cuentas de Línea Operativa.</t>
+  </si>
+  <si>
+    <t>El usuario valida que se muestre la columna "Número de crédito".||El sistema muestra la columna "Número de crédito" de forma correcta.</t>
+  </si>
+  <si>
+    <t>El usuario valida que se muestre la columna "Saldo total del crédito".||El sistema muestra la columna "Saldo total del crédito" de forma correcta con formato de moneda:
+-Signo $
+-Separación de miles y millones con separador de coma (,)
+-Signo de punto para decimales (.)
+-2 decimales</t>
+  </si>
+  <si>
+    <t>El usuario valida que se muestre la columna "Capital disponible".||El sistema muestra la columna "Capital disponible" de forma correcta con formato de moneda:
+-Signo $
+-Separación de miles y millones con separador de coma (,)
+-Signo de punto para decimales (.)
+-2 decimales</t>
+  </si>
+  <si>
+    <t>El usuario valida que se muestre la columna "Importe autorizado".||El sistema muestra la columna "Importe autorizado" de forma correcta con formato de moneda:
+-Signo $
+-Separación de miles y millones con separador de coma (,)
+-Signo de punto para decimales (.)
+-2 decimales</t>
+  </si>
+  <si>
+    <t>El usuario valida que se muestre la opción "Ver consolidado".||El sistema muestra la opción "Ver consolidado" de forma correcta como hipervínculo.</t>
+  </si>
+  <si>
+    <t>El usuario valida que se muestre el botón de Descarga.||El sistema muestra el botón de "Descarga" de forma correcta.
+Nota: Puede presentarse con el icono de impresora o flecha hacia abajo en lugar del botón de Descarga.</t>
+  </si>
+  <si>
+    <t>TC_002_79_administradorConsultaCuentasPrestamosPersonalesBD</t>
+  </si>
+  <si>
+    <t>El usuario da clic en el menú "Prestamos Personales".||El sistema muestra la lista de créditos de Préstamos Personales .</t>
+  </si>
+  <si>
+    <t>El usuario valida que se muestre la columna "Pago vigente".||El sistema muestra la columna "Pago vigente" de forma correcta con formato de moneda:
+-Signo $
+-Separación de miles y millones con separador de coma (,)
+-Signo de punto para decimales (.)
+-2 decimales</t>
+  </si>
+  <si>
+    <t>El usuario valida que se muestre la columna "Pago vencido".||El sistema muestra la columna "Pago vencido" de forma correcta con formato de moneda:
+-Signo $
+-Separación de miles y millones con separador de coma (,)
+-Signo de punto para decimales (.)
+-2 decimales</t>
+  </si>
+  <si>
+    <t>TC_002_80_administradorConsultaCuentasFondosInversionBD</t>
+  </si>
+  <si>
+    <t>El usuario da clic en el menú "Fondos".||El sistema muestra la lista de contratos de Fondos de Inversión.</t>
+  </si>
+  <si>
+    <t>El usuario valida que se muestre la columna "Número de contrato".||El sistema muestra la columna "Número de contrato" de forma correcta.</t>
+  </si>
+  <si>
+    <t>El usuario valida que se muestre la columna "Saldo total".||El sistema muestra la columna "Saldo total" de forma correcta con formato de moneda:
+-Signo $
+-Separación de miles y millones con separador de coma (,)
+-Signo de punto para decimales (.)
+-2 decimales</t>
+  </si>
+  <si>
+    <t>TC_002_81_administradorConsultaCreditosHipotecariosBD</t>
+  </si>
+  <si>
+    <t>El usuario da clic en el menú "Hipotecarios".||El sistema muestra la lista de Créditos Hipotecarios.</t>
+  </si>
+  <si>
+    <t>El usuario valida que se muestre la columna "N° Crédito".||El sistema muestra la columna "N° Crédito" de forma correcta.</t>
+  </si>
+  <si>
+    <t>El usuario valida que se muestre la columna "Valor Crédito Original".||El sistema muestra la columna "Valor Crédito Original" de forma correcta con formato de moneda:
+-Signo $
+-Separación de miles y millones con separador de coma (,)
+-Signo de punto para decimales (.)
+-2 decimales</t>
+  </si>
+  <si>
+    <t>El usuario valida que se muestre la columna "Saldo vigente".||El sistema muestra la columna "Saldo vigente" de forma correcta con formato de moneda:
+-Signo $
+-Separación de miles y millones con separador de coma (,)
+-Signo de punto para decimales (.)
+-2 decimales</t>
+  </si>
+  <si>
+    <t>El usuario valida que se muestre la columna "Saldo vencido".||El sistema muestra la columna "Saldo vencido" de forma correcta con formato de moneda:
+-Signo $
+-Separación de miles y millones con separador de coma (,)
+-Signo de punto para decimales (.)
+-2 decimales</t>
+  </si>
+  <si>
+    <t>TC_002_82_administradorConsulta CuentasInversionBD</t>
+  </si>
+  <si>
+    <t>El usuario da clic en el menú "Inversiones".||El sistema muestra la lista de Cuentas de Inversión .</t>
+  </si>
+  <si>
+    <t>El usuario valida que se muestre la columna "Importe de Capital".||El sistema muestra la columna "Importe de Capital" de forma correcta con formato de moneda:
+-Signo $
+-Separación de miles y millones con separador de coma (,)
+-Signo de punto para decimales (.)
+-2 decimales</t>
+  </si>
+  <si>
+    <t>TC_002_83_administradorConsultaCuentasTDCMXNBD</t>
+  </si>
+  <si>
+    <t>El usuario da clic en el menú "Tarjetas de Crédito".||El sistema muestra la lista de Tarjetas de Crédito .</t>
+  </si>
+  <si>
+    <t>El usuario valida que se muestre la columna "Número de tarjeta".||El sistema muestra la columna "Número de tarjeta" de forma correcta.</t>
+  </si>
+  <si>
+    <t>El usuario valida que se muestre la columna "Saldo disponible".||El sistema muestra la columna "Saldo disponible" de forma correcta con formato de moneda:
+-Signo $
+-Separación de miles y millones con separador de coma (,)
+-Signo de punto para decimales (.)
+-2 decimales</t>
+  </si>
+  <si>
+    <t>El usuario valida que se muestre la columna "Saldo utilizado".||El sistema muestra la columna "Saldo utilizado" de forma correcta con formato de moneda:
+-Signo $
+-Separación de miles y millones con separador de coma (,)
+-Signo de punto para decimales (.)
+-2 decimales</t>
+  </si>
+  <si>
+    <t>El usuario valida que se muestre la columna "Límite de crédito".||El sistema muestra la columna "Límite de crédito de forma correcta con formato de moneda:
+-Signo $
+-Separación de miles y millones con separador de coma (,)
+-Signo de punto para decimales (.)
+-2 decimales</t>
+  </si>
+  <si>
+    <t>TC_002_84_administradorConsultaCuentasChequesUSDBD</t>
+  </si>
+  <si>
+    <t>El usuario da clic en la pestaña "Cuentas Cheque USD".||El sistema muestra la lista de cuentas de cheques USD.</t>
+  </si>
+  <si>
+    <t>El usuario valida que se muestre la columna "No de cuenta".||El sistema muestra la columna "No de cuenta" de forma correcta.</t>
+  </si>
+  <si>
+    <t>El usuario valida que se muestre la columna "Saldo total".||El sistema muestra la columna "Saldo total" de forma correcta con formato de moneda:
+-Signo $
+-Separación de miles y millones con separador de coma (,)
+-Signo de punto para decimales (.)
+-2 decim</t>
+  </si>
+  <si>
+    <t>El usuario valida que se muestre la columna "Saldo disponible".||El sistema muestra la columna "Saldo disponible" de forma correcta con formato de moneda:
+-Signo $
+-Separación de miles y millones con separador de coma (,)
+-Signo de punto para decimales (.)
+-2 decim</t>
+  </si>
+  <si>
+    <t>El usuario valida que se muestre la columna "Saldo salvo buen cobro".||El sistema muestra la columna "Saldo salvo buen cobro" de forma correcta con formato de moneda:
+-Signo $
+-Separación de miles y millones con separador de coma (,)
+-Signo de punto para decimales (.)
+-2 decim</t>
+  </si>
+  <si>
+    <t>El usuario valida que se muestre la columna "Saldo límite de sobregiro".||El sistema muestra la columna "Saldo límite de sobregiro" de forma correcta con formato de moneda:
+-Signo $
+-Separación de miles y millones con separador de coma (,)
+-Signo de punto para decimales (.)
+-2 decim</t>
+  </si>
+  <si>
+    <t>TC_002_85_administradorConsultaCuentasChequeMXNBD</t>
+  </si>
+  <si>
+    <t>El usuario valida las cuentas de cheques de la pestaña "Cuentas Cheque MXN".||El sistema muestra la lista de cuentas de cheques MXN.</t>
+  </si>
+  <si>
+    <t>El usuario valida que se muestre la columna "Saldo disponible".||El sistema muestra la columna "Saldo disponible" de forma correcta con formato de moneda:
+-Signo $
+-Separación de miles y millones con separador de coma (,)
+-Signo de punto para decimales (.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El usuario valida que se muestre la columna "Saldo salvo buen cobro".||El sistema muestra la columna "Saldo salvo buen cobro" de forma correcta con formato de moneda:
+-Signo $
+-Separación de miles y millones con separador de coma (,)
+-Signo de punto para </t>
+  </si>
+  <si>
+    <t>El usuario valida que se muestre la columna "Saldo límite de sobregiro".||El sistema muestra la columna "Saldo límite de sobregiro" de forma correcta con formato de moneda:
+-Signo $
+-Separación de miles y millones con separador de coma (,)
+-Signo de punto</t>
+  </si>
+  <si>
+    <t>TC_002_94_administradorConsultaCuentasLineaOperativaFM</t>
+  </si>
+  <si>
+    <t>El usuario valida que se muestre la sección LÍNEA OPERATIVA CONSOLIDADOS.||El sistema muestra de forma correcta la sección LÍNEA OPERATIVA CONSOLIDADOS.</t>
+  </si>
+  <si>
+    <t>El usuario valida que se muestre el link "Ver créditos&gt;" en la sección LÍNEA OPERATIVA CONSOLIDADOS.||El sistema muestra de forma correcta el link "Ver créditos&gt;".</t>
+  </si>
+  <si>
+    <t>El usuario valida que se muestre el campo "Saldo total del crédito".||El sistema muestra el campo "Saldo total del crédito" de forma correcta con formato de moneda:
+-Signo $
+-Separación de miles y millones con separador de coma (,)
+-Signo de punto para decimales (.)
+-2 decim</t>
+  </si>
+  <si>
+    <t>El usuario valida que se muestre el campo "Capital disponible".||El sistema muestra el campo "Capital disponible" de forma correcta con formato de moneda:
+-Signo $
+-Separación de miles y millones con separador de coma (,)
+-Signo de punto para decimales (.)
+-2 decim</t>
+  </si>
+  <si>
+    <t>El usuario valida que se muestre el campo "Importe autorizado".||El sistema muestra el campo "Importe autorizado" de forma correcta con formato de moneda:
+-Signo $
+-Separación de miles y millones con separador de coma (,)
+-Signo de punto para decimales (.)
+-2 decim</t>
+  </si>
+  <si>
+    <t>TC_002_95_administradorConsultaCuentasPrestamosPersonalesFM</t>
+  </si>
+  <si>
+    <t>El usuario valida que se muestre la sección PRÉSTAMOS PERSONALES CONSOLIDADOS.||El sistema muestra de forma correcta la sección PRÉSTAMOS PERSONALES CONSOLIDADOS.</t>
+  </si>
+  <si>
+    <t>El usuario valida que se muestre el link "Ver préstamos&gt;" en la sección PRÉSTAMOS PERSONALES CONSOLIDADOS.||El sistema muestra de forma correcta el link "Ver préstamos&gt;".</t>
+  </si>
+  <si>
+    <t>El usuario valida que se muestre el campo "Saldo total".||El sistema muestra el campo "Saldo total" de forma correcta con formato de moneda:
+-Signo $
+-Separación de miles y millones con separador de coma (,)
+-Signo de punto para decimales (.)
+-2 decim</t>
+  </si>
+  <si>
+    <t>El usuario valida que se muestre el campo "Pagos vigentes".||El sistema muestra el campo "Pagos vigentes" de forma correcta con formato de moneda:
+-Signo $
+-Separación de miles y millones con separador de coma (,)
+-Signo de punto para decimales (.)
+-2 decim</t>
+  </si>
+  <si>
+    <t>El usuario valida que se muestre el campo "Pagos vencidos".||El sistema muestra el campo "Pagos vencidos" de forma correcta con formato de moneda:
+-Signo $
+-Separación de miles y millones con separador de coma (,)
+-Signo de punto para decimales (.)
+-2 decim</t>
+  </si>
+  <si>
+    <t>TC_002_96_administradorConsultaCuentasFondosInversonFM</t>
+  </si>
+  <si>
+    <t>El usuario valida que se muestre la sección FONDOS DE INVERSIÓN CONSOLIDADOS.||El sistema muestra de forma correcta la sección FONDOS DE INVERSIÓN CONSOLIDADOS.</t>
+  </si>
+  <si>
+    <t>El usuario valida que se muestre el link "Ver fondos&gt;" en la sección FONDOS DE INVERSIÓN CONSOLIDADOS.||El sistema muestra de forma correcta el link "Ver fondos&gt;".</t>
+  </si>
+  <si>
+    <t>El usuario valida que se muestre el campo "Saldo total".|El sistema muestra el campo "Saldo total" de forma correcta con formato de moneda:
+-Signo $
+-Separación de miles y millones con separador de coma (,)
+-Signo de punto para decimales (.)
+-2 decim</t>
+  </si>
+  <si>
+    <t>TC_002_97_administradorConsultaCreditoHipotecarioFM</t>
+  </si>
+  <si>
+    <t>El usuario valida que se muestre la sección CRÉDITOS HIPOTECARIOS CONSOLIDADOS.||El sistema muestra de forma correcta la sección CRÉDITOS HIPOTECARIOS CONSOLIDADOS.</t>
+  </si>
+  <si>
+    <t>El usuario valida que se muestre el link "Ver créditos&gt;" en la sección CRÉDITOS HIPOTECARIOS CONSOLIDADOS.||El sistema muestra de forma correcta el link "Ver créditos&gt;".</t>
+  </si>
+  <si>
+    <t>El usuario valida que se muestre el campo "Valor Crédito Original".||El sistema muestra el campo "Valor Crédito Original" de forma correcta con formato de moneda:
+-Signo $
+-Separación de miles y millones con separador de coma (,)
+-Signo de punto para decimales (.)
+-2 decim</t>
+  </si>
+  <si>
+    <t>El usuario valida que se muestre el campo "Saldo vigente".||El sistema muestra el campo "Saldo vigente" de forma correcta con formato de moneda:
+-Signo $
+-Separación de miles y millones con separador de coma (,)
+-Signo de punto para decimales (.)
+-2 decim</t>
+  </si>
+  <si>
+    <t>El usuario valida que se muestre el campo "Saldo vencido".||El sistema muestra el campo "Saldo vencido" de forma correcta con formato de moneda:
+-Signo $
+-Separación de miles y millones con separador de coma (,)
+-Signo de punto para decimales (.)
+-2 decim</t>
+  </si>
+  <si>
+    <t>TC_002_98_administradorConsultaCuentasInversionFM</t>
+  </si>
+  <si>
+    <t>El usuario valida que se muestre la sección CONTRATOS DE INVERSIÓN CONSOLIDADOS.||El sistema muestra de forma correcta la sección CONTRATOS DE INVERSIÓN CONSOLIDADOS.</t>
+  </si>
+  <si>
+    <t>El usuario valida que se muestre el link "Ver contratos&gt;" en la sección CONTRATOS DE INVERSIÓN CONSOLIDADOS.||El sistema muestra de forma correcta el link "Ver contratos&gt;".</t>
+  </si>
+  <si>
+    <t>El usuario valida que se muestre la columna "Importe de Capital".||El sistema muestra la columna "Importe de Capital" de forma correcta con formato de moneda:
+-Signo $
+-Separación de miles y millones con separador de coma (,)
+-Signo de punto para decimales (.)
+-2 decim</t>
+  </si>
+  <si>
+    <t>TC_002_99_administradorConsultaCuentasTDCMXNFM</t>
+  </si>
+  <si>
+    <t>El usuario valida que se muestre la sección TARJETAS DE CRÉDITO CONSOLIDADAS.||El sistema muestra de forma correcta la sección TARJETAS DE CRÉDITO CONSOLIDADAS.</t>
+  </si>
+  <si>
+    <t>El usuario valida que se muestre el link "Ver tarjetas&gt;" en la sección TARJETAS DE CRÉDITO CONSOLIDADAS.||El sistema muestra de forma correcta el link "Ver tarjetas&gt;".</t>
+  </si>
+  <si>
+    <t>El usuario valida que se muestre el campo "Saldo disponible".||El sistema muestra el campo "Saldo disponible" de forma correcta con formato de moneda:
+-Signo $
+-Separación de miles y millones con separador de coma (,)
+-Signo de punto para decimales (.)
+-2 decim</t>
+  </si>
+  <si>
+    <t>El usuario valida que se muestre el campo "Saldo utilizado".||El sistema muestra el campo "Saldo utilizado" de forma correcta con formato de moneda:
+-Signo $
+-Separación de miles y millones con separador de coma (,)
+-Signo de punto para decimales (.)
+-2 decim</t>
+  </si>
+  <si>
+    <t>El usuario valida que se muestre el campo "Límite de crédito".||El sistema muestra el campo "Límite de crédito" de forma correcta con formato de moneda:
+-Signo $
+-Separación de miles y millones con separador de coma (,)
+-Signo de punto para decimales (.)
+-2 decim</t>
+  </si>
+  <si>
+    <t>TC_002_100_administradorConsultaCuentasChequesUSDFM</t>
+  </si>
+  <si>
+    <t>El usuario valida que se muestre la sección CUENTAS CHEQUE USD CONSOLIDADAS.||El sistema muestra de forma correcta la sección CUENTAS CHEQUE USD CONSOLIDADAS.</t>
+  </si>
+  <si>
+    <t>El usuario valida que se muestre el link "Ver cuentas&gt;" en la sección CUENTAS CHEQUE USD CONSOLIDADAS.||El sistema muestra de forma correcta el link "Ver cuentas&gt;".</t>
+  </si>
+  <si>
+    <t>El usuario valida que se muestre el campo "Saldo salvo buen cobro".||El sistema muestra el campo "Saldo salvo buen cobro" de forma correcta con formato de moneda:
+-Signo $
+-Separación de miles y millones con separador de coma (,)
+-Signo de punto para decimales (.)
+-2 decim</t>
+  </si>
+  <si>
+    <t>El usuario valida que se muestre el campo "Saldo límite de sobregiro".||El sistema muestra el campo "Saldo límite de sobregiro" de forma correcta con formato de moneda:
+-Signo $
+-Separación de miles y millones con separador de coma (,)
+-Signo de punto para decimales (.)
+-2 decim</t>
+  </si>
+  <si>
+    <t>TC_002_101_administradorConsultaCuentasChequesMXNFM</t>
+  </si>
+  <si>
+    <t>El usuario valida que se muestre la sección CUENTAS CHEQUE MXN CONSOLIDADAS.||El sistema muestra de forma correcta la sección CUENTAS CHEQUE MXN CONSOLIDADAS.</t>
+  </si>
+  <si>
+    <t>El usuario valida que se muestre el link "Ver cuentas&gt;".||El sistema muestra de forma correcta el link "Ver cuentas&gt;".</t>
+  </si>
+  <si>
+    <t>El usuario valida que se muestre el campo "Saldo disponible".||El sistema muestra el campo "Saldo disponible" de forma correcta con formato de moneda:
+-Signo $
+-Separación de miles y millones con separador de coma (,)
+-Signo de punto para decimales (.)
+-2</t>
+  </si>
+  <si>
+    <t>El usuario valida que se muestre el campo "Saldo salvo buen cobro".||El sistema muestra el campo "Saldo salvo buen cobro" de forma correcta con formato de moneda:
+-Signo $
+-Separación de miles y millones con separador de coma (,)
+-Signo de punto para deci</t>
+  </si>
+  <si>
+    <t>El usuario valida que se muestre el campo "Saldo límite de sobregiro".||El sistema muestra el campo "Saldo límite de sobregiro" de forma correcta con formato de moneda:
+-Signo $
+-Separación de miles y millones con separador de coma (,)
+-Signo de punto para decimales (.)
+-2 decimales</t>
+  </si>
+  <si>
+    <t>TC_002_102_administradorConsulta</t>
+  </si>
+  <si>
+    <t>El usuario da clic en el botón " V " ubicado en el lado superior derecho posterior al nombre de usuario.||El sistema muestra la opción "Cerrar sesión".</t>
+  </si>
+  <si>
+    <t>El usuario da clic en la opción "Cerrar sesión".||El sistema muestra la página de inicio de CCOP.</t>
+  </si>
+  <si>
+    <t>TC_002_103_administradorConsulta</t>
+  </si>
+  <si>
+    <t>El usuario valida el total de cuentas mostradas entre paréntesis en la sección "PRÉSTAMOS PERSONALES CONSOLIDADOS".||El sistema muestra el total de créditos de Préstamos Personales de forma correcta.</t>
+  </si>
+  <si>
+    <t>El usuario da clic en el menú "Prestamos personales".||El sistema muestra la lista de créditos de Préstamos Personales y debe coincidir con el total de cuentas mostradas en el Dashboard en la sección "PRÉSTAMOS PERSONALES CONSOLIDADOS".</t>
+  </si>
+  <si>
+    <t>El usuario da clic en la opción "Ver consolidado".||El sistema muestra la sección "PRÉSTAMOS PERSONALES CONSOLIDADOS" con el número total de créditos indicado entre paréntesis y debe coincidir con el total de cuentas mostradas en el Dashboard en la sección "PRÉSTAMOS PERSONALES CONSOLIDADOS".</t>
+  </si>
+  <si>
+    <t>El usuario valida el monto mostrado en el campo "Saldo total".||El sistema debe mostrar el mismo monto que el mostrado en el Dashboard en la sección "PRÉSTAMOS PERSONALES CONSOLIDADOS"</t>
+  </si>
+  <si>
+    <t>El usuario valida el formato mostrado en el campo "Saldo total".||El sistema muestra el campo "Saldo total" de forma correcta con el siguiente formato:
+Formato de moneda con signo $
+Separación de miles y millones con separador de coma (,)
+Signo de punto para decimales (.)
+2 decimales</t>
+  </si>
+  <si>
+    <t>El usuario valida el monto mostrado en el campo "Saldo total".||El sistema debe mostrar el mismo monto que la suma de las cuentas de la columna "Saldo total".</t>
+  </si>
+  <si>
+    <t>El usuario valida el monto mostrado en el campo "Pagos vigentes".||El sistema debe mostrar el mismo monto que el mostrado en el Dashboard en la sección "PRÉSTAMOS PERSONALES CONSOLIDADOS"</t>
+  </si>
+  <si>
+    <t>El usuario valida el formato mostrado en el campo "Pagos vigentes".||El sistema muestra el campo "Pagos vigentes" de forma correcta con el siguiente formato:
+Formato de moneda con signo $
+Separación de miles y millones con separador de coma (,)
+Signo de punto para decimales (.)
+2 decimales</t>
+  </si>
+  <si>
+    <t>El usuario valida el monto mostrado en el campo "Pagos vigentes.||El sistema debe mostrar el mismo monto que la suma de las cuentas de la columna "Pagos vigentes".</t>
+  </si>
+  <si>
+    <t>El usuario valida el monto mostrado en el campo "Pagos vencidos".||El sistema debe mostrar el mismo monto que el mostrado en el Dashboard en la sección "PRÉSTAMOS PERSONALES CONSOLIDADOS"</t>
+  </si>
+  <si>
+    <t>El usuario valida el formato mostrado en el campo "Pagos vencidos".||El sistema muestra el campo "Pagos vencidos" de forma correcta con el siguiente formato:
+Formato de moneda con signo $
+Separación de miles y millones con separador de coma (,)
+Signo de punto para decimales (.)
+2 decimales</t>
+  </si>
+  <si>
+    <t>El usuario valida el monto mostrado en el campo "Pagos vencidos".||El sistema debe mostrar el mismo monto que la suma de las cuentas de la columna "Pagos vencidos".</t>
+  </si>
+  <si>
+    <t>SC_002_71_administradorConsultaCuentasPrestamosPersonalesConsolidado</t>
+  </si>
+  <si>
+    <t>SC_002_72_administradorConsultaCuentasFondosInversionConsolidado</t>
+  </si>
+  <si>
+    <t>El usuario valida el total de cuentas mostradas entre paréntesis en la sección "FONDOS DE INVERSIÓN CONSOLIDADOS".||El sistema muestra el total de contratos de Fondos de Inversión de forma correcta.</t>
+  </si>
+  <si>
+    <t>El usuario da clic en el menú "Fondos".||El sistema muestra la lista de contratos de Fondos de Inversión y debe coincidir con el total de cuentas mostradas en el Dashboard en la sección "FONDOS DE INVERSIÓN CONSOLIDADOS".</t>
+  </si>
+  <si>
+    <t>El usuario da clic en la opción "Ver consolidado".||El sistema muestra la sección "FONDOS DE INVERSIÓN CONSOLIDADOS" con el número total de contratos indicado entre paréntesis y debe coincidir con el total de cuentas mostradas en el Dashboard en la sección "FONDOS DE INVERSIÓN CONSOLIDADOS".</t>
+  </si>
+  <si>
+    <t>El usuario valida el monto mostrado en el campo "Saldo total".||El sistema debe mostrar el mismo monto que el mostrado en el Dashboard en la sección "FONDOS DE INVERSIÓN CONSOLIDADOS"</t>
+  </si>
+  <si>
+    <t>El usuario valida el formato mostrado en el campo "Saldo total".||El sistema muestra el campo "Saldo total" de forma correcta con el siguiente formato:
+-Formato de moneda con signo $
+-Separación de miles y millones con separador de coma (,)
+-Signo de punto para decimales (.)
+-2 decimales</t>
+  </si>
+  <si>
+    <t>SC_002_73_administradorConsultaCreditosHipotecariosConsolidado</t>
+  </si>
+  <si>
+    <t>El usuario valida el total de cuentas mostradas entre paréntesis en la sección "CRÉDITOS HIPOTECARIOS CONSOLIDADOS".||El sistema muestra el total de Créditos Hipotecarios de forma correcta.</t>
+  </si>
+  <si>
+    <t>El usuario da clic en el menú "Hipotecarios".||El sistema muestra la lista de Créditos Hipotecarios y debe coincidir con el total de cuentas mostradas en el Dashboard en la sección "CRÉDITOS HIPOTECARIOS CONSOLIDADOS".</t>
+  </si>
+  <si>
+    <t>El usuario da clic en la opción "Ver consolidado".||El sistema muestra la sección "CRÉDITOS HIPOTECARIOS CONSOLIDADOS" con el número total de créditos indicados entre paréntesis y debe coincidir con el total de cuentas mostradas en el Dashboard en la sección "CRÉDITOS HIPOTECARIOS CONSOLIDADOS".</t>
+  </si>
+  <si>
+    <t>El usuario valida el monto mostrado en el campo "Valor Crédito Original".||El sistema debe mostrar el mismo monto que el mostrado en el Dashboard en la sección "CRÉDITOS HIPOTECARIOS CONSOLIDADOS"</t>
+  </si>
+  <si>
+    <t>El usuario valida el formato mostrado en el campo "Valor Crédito Original".||El sistema muestra el campo "Valor Crédito Original" de forma correcta con el siguiente formato:
+-Formato de moneda con signo $
+-Separación de miles y millones con separador de coma (,)
+-Signo de punto para decimales (.)
+-2 decimales</t>
+  </si>
+  <si>
+    <t>El usuario valida el monto mostrado en el campo "Valor Crédito Original".||El sistema debe mostrar el mismo monto que la suma de las cuentas de la columna "Valor Crédito Original".</t>
+  </si>
+  <si>
+    <t>El usuario valida el monto mostrado en el campo "Saldo vigente".||El sistema debe mostrar el mismo monto que el mostrado en el Dashboard en la sección "CRÉDITOS HIPOTECARIOS CONSOLIDADOS"</t>
+  </si>
+  <si>
+    <t>El usuario valida el formato mostrado en el campo "Saldo vigente".||El sistema muestra el campo "Saldo vigente" de forma correcta con el siguiente formato:
+-Formato de moneda con signo $
+-Separación de miles y millones con separador de coma (,)
+-Signo de punto para decimales (.)
+-2 decimales</t>
+  </si>
+  <si>
+    <t>El usuario valida el monto mostrado en el campo "Saldo vigente".||El sistema debe mostrar el mismo monto que la suma de las cuentas de la columna "Saldo vigente".</t>
+  </si>
+  <si>
+    <t>El usuario valida el monto mostrado en el campo "Saldo vencido".||El sistema debe mostrar el mismo monto que el mostrado en el Dashboard en la sección "CRÉDITOS HIPOTECARIOS CONSOLIDADOS"</t>
+  </si>
+  <si>
+    <t>El usuario valida el formato mostrado en el campo "Saldo vencido".||El sistema muestra el campo "Saldo vencido" de forma correcta con el siguiente formato:
+-Formato de moneda con signo $
+-Separación de miles y millones con separador de coma (,)
+-Signo de punto para decimales (.)
+-2 decimales</t>
+  </si>
+  <si>
+    <t>El usuario valida el monto mostrado en el campo "Saldo vencido".||El sistema debe mostrar el mismo monto que la suma de las cuentas de la columna "Saldo vencido".</t>
+  </si>
+  <si>
+    <t>SC_002_74_administradorConsultaCuentasInversionesConsolidado</t>
+  </si>
+  <si>
+    <t>El usuario valida el total de cuentas mostradas entre paréntesis en la sección "CONTRATOS DE INVERSIÓN CONSOLIDADOS".||El sistema muestra el total de créditos de inversiones de forma correcta.</t>
+  </si>
+  <si>
+    <t>El usuario da clic en el menú "Inversiones".||El sistema muestra la lista de créditos de inversiones y debe coincidir con el total de cuentas mostradas en el Dashboard en la sección "CONTRATOS DE INVERSIÓN CONSOLIDADOS".</t>
+  </si>
+  <si>
+    <t>El usuario da clic en la opción "Ver consolidado".||El sistema muestra la sección "CONTRATOS DE INVERSIÓN CONSOLIDADOS" con el número total de contratos indicado entre paréntesis y debe coincidir con el total de cuentas mostradas en el Dashboard en la sección "CONTRATOS DE INVERSIÓN CONSOLIDADOS".</t>
+  </si>
+  <si>
+    <t>El usuario valida el monto mostrado en el campo "Importe de Capital".||El sistema debe mostrar el mismo monto que el mostrado en el Dashboard en la sección "CONTRATOS DE INVERSIÓN CONSOLIDADOS"</t>
+  </si>
+  <si>
+    <t>El usuario valida el formato mostrado en el campo "Importe de Capital".||El sistema muestra el campo "Importe de Capital" de forma correcta con el siguiente formato:
+-Formato de moneda con signo $
+-Separación de miles y millones con separador de coma (,)
+-Signo de punto para decimales (.)
+-2 decimales</t>
+  </si>
+  <si>
+    <t>El usuario valida el monto mostrado en el campo "Importe de Capital".||El sistema debe mostrar el mismo monto que la suma de las cuentas de la columna "Importe de Capital".</t>
+  </si>
+  <si>
+    <t>SC_002_75_administradorConsultaCuentasTDCMXNConsolidado</t>
+  </si>
+  <si>
+    <t>El usuario valida el total de cuentas mostradas entre paréntesis en la sección "TARJETAS DE CRÉDITO CONSOLIDADAS".||El sistema muestra el total de cuentas de tarjetas de crédito de forma correcta.</t>
+  </si>
+  <si>
+    <t>El usuario da clic en el menú "Tarjetas de Crédito".||El sistema muestra la lista de cuentas de tarjetas de crédito y debe coincidir con el total de cuentas mostradas en el Dashboard en la sección "TARJETAS DE CRÉDITO CONSOLIDADAS".</t>
+  </si>
+  <si>
+    <t>El usuario da clic en la opción "Ver consolidado".||El sistema muestra la sección "TARJETAS DE CRÉDITO CONSOLIDADAS" con el número total de cuentas indicadas entre paréntesis y debe coincidir con el total de cuentas mostradas en el Dashboard en la sección "TARJETAS DE CRÉDITO CONSOLIDADAS".</t>
+  </si>
+  <si>
+    <t>El usuario valida el monto mostrado en el campo "Saldo disponible".||El sistema debe mostrar el mismo monto que el mostrado en el Dashboard en la sección "TARJETAS DE CRÉDITO CONSOLIDADAS"</t>
+  </si>
+  <si>
+    <t>El usuario valida el formato mostrado en el campo "Saldo disponible".||El sistema muestra el campo "Saldo disponible" de forma correcta con el siguiente formato:
+-Formato de moneda con signo $
+-Separación de miles y millones con separador de coma (,)
+-Signo de punto para decimales (.)
+-2 decimales</t>
+  </si>
+  <si>
+    <t>El usuario valida el monto mostrado en el campo "Saldo disponible".||El sistema debe mostrar el mismo monto que la suma de las cuentas de la columna "Saldo disponible".</t>
+  </si>
+  <si>
+    <t>El usuario valida el monto mostrado en el campo "Saldo utilizado".||El sistema debe mostrar el mismo monto que el mostrado en el Dashboard en la sección "TARJETAS DE CRÉDITO CONSOLIDADAS"</t>
+  </si>
+  <si>
+    <t>El usuario valida el formato mostrado en el campo "Saldo utilizado".||El sistema muestra el campo "Saldo utilizado" de forma correcta con el siguiente formato:
+-Formato de moneda con signo $
+-Separación de miles y millones con separador de coma (,)
+-Signo de punto para decimales (.)
+-2 decimales</t>
+  </si>
+  <si>
+    <t>El usuario valida el monto mostrado en el campo "Saldo utilizado".||El sistema debe mostrar el mismo monto que la suma de las cuentas de la columna "Saldo utilizado".</t>
+  </si>
+  <si>
+    <t>El usuario valida el monto mostrado en el campo "Límite de crédito".||El sistema debe mostrar el mismo monto que el mostrado en el Dashboard en la sección "TARJETAS DE CRÉDITO CONSOLIDADAS"</t>
+  </si>
+  <si>
+    <t>El usuario valida el formato mostrado en el campo "Límite de crédito".||El sistema muestra el campo "Límite de crédito" de forma correcta con el siguiente formato:
+-Formato de moneda con signo $
+-Separación de miles y millones con separador de coma (,)
+-Signo de punto para decimales (.)
+-2 decimales</t>
+  </si>
+  <si>
+    <t>El usuario valida el monto mostrado en el campo "Límite de crédito".||El sistema debe mostrar el mismo monto que la suma de las cuentas de la columna "Límite de crédito".</t>
+  </si>
+  <si>
+    <t>SC_002_76_administradorConsultacuentasChequesUSDConsolidado</t>
+  </si>
+  <si>
+    <t>El usuario valida el total de cuentas mostradas entre paréntesis en la sección "CUENTAS CHEQUE USD CONSOLIDADAS".||El sistema muestra el total de Cuentas Cheque USD de forma correcta.</t>
+  </si>
+  <si>
+    <t>El usuario da clic en la pestaña "Cuentas Cheque USD".||El sistema muestra la lista de cuentas de cheques USD y debe coincidir con el total de cuentas mostradas en el Dashboard en la sección "CUENTAS CHEQUE USD CONSOLIDADAS".</t>
+  </si>
+  <si>
+    <t>El usuario da clic en la opción "Ver consolidado".||El sistema muestra la sección "CUENTAS CHEQUE CONSOLIDADAS" con el número total de cuentas indicadas entre paréntesis y debe coincidir con el total de cuentas mostradas en el Dashboard en la sección "CUENTAS CHEQUE USD CONSOLIDADAS".</t>
+  </si>
+  <si>
+    <t>El usuario valida el monto mostrado en el campo "Saldo total".||El sistema debe mostrar el mismo monto que el mostrado en el Dashboard en la sección "CUENTAS CHEQUE USD CONSOLIDADAS"</t>
+  </si>
+  <si>
+    <t>El usuario valida el monto mostrado en el campo "Saldo disponible".||El sistema debe mostrar el mismo monto que el mostrado en el Dashboard en la sección "CUENTAS CHEQUE USD CONSOLIDADAS"</t>
+  </si>
+  <si>
+    <t>El usuario valida el monto mostrado en el campo "Saldo salvo buen cobro".||El sistema debe mostrar el mismo monto que el mostrado en el Dashboard en la sección "CUENTAS CHEQUE USD CONSOLIDADAS"</t>
+  </si>
+  <si>
+    <t>El usuario valida el formato mostrado en el campo "Saldo salvo buen cobro".||El sistema muestra el campo "Saldo salvo buen cobro" de forma correcta con el siguiente formato:
+-Formato de moneda con signo $
+-Separación de miles y millones con separador de coma (,)
+-Signo de punto para decimales (.)
+-2 decimales</t>
+  </si>
+  <si>
+    <t>El usuario valida el monto mostrado en el campo "Saldo salvo buen cobro".||El sistema debe mostrar el mismo monto que la suma de las cuentas de la columna "Saldo salvo buen cobro".</t>
+  </si>
+  <si>
+    <t>El usuario valida el monto mostrado en el campo "Cupo total de Sobregiros" con el del Dashboard
+"Saldo límite de sobregiro".||El sistema debe mostrar el mismo monto que el mostrado en el Dashboard en la sección "CUENTAS CHEQUE USD CONSOLIDADAS" en el campo "Saldo límite de sobregiro".</t>
+  </si>
+  <si>
+    <t>El usuario valida el formato mostrado en el campo "Cupo total de Sobregiros" con el del Dashboard "Saldo límite de sobregiro".||El sistema muestra el campo "Cupo total de Sobregiros" de forma correcta con el siguiente formato:
+-Formato de moneda con signo $
+-Separación de miles y millones con separador de coma (,)
+-Signo de punto para decimales (.)
+-2 decimales</t>
+  </si>
+  <si>
+    <t>El usuario valida el monto mostrado en el campo "Cupo total de Sobregiros".||El sistema debe mostrar el mismo monto que la suma de las cuentas de la columna "Cupo total de Sobregiros".</t>
+  </si>
+  <si>
+    <t>SC_002_77_administradorConsultaCuentasChequesMXNConsolidado</t>
+  </si>
+  <si>
+    <t>El usuario valida el total de cuentas mostradas entre paréntesis en la sección "CUENTAS CHEQUE MXN CONSOLIDADAS".||El sistema muestra el total de Cuentas Cheque MXN de forma correcta.</t>
+  </si>
+  <si>
+    <t>El usuario valida las cuentas de cheques de la pestaña "Cuentas Cheque MXN".||El sistema muestra la lista de cuentas de cheques MXN y debe coincidir con el total de cuentas mostradas en el Dashboard en la sección "CUENTAS CHEQUE MXN CONSOLIDADAS".</t>
+  </si>
+  <si>
+    <t>El usuario da clic en la opción "Ver consolidado".||El sistema muestra la sección "CUENTAS CHEQUE CONSOLIDADAS" con el número total de cuentas indicadas entre paréntesis y debe coincidir con el total de cuentas mostradas en el Dashboard en la sección "CUENTAS CHEQUE MXN CONSOLIDADAS".</t>
+  </si>
+  <si>
+    <t>El usuario valida el monto mostrado en el campo "Saldo total".||El sistema debe mostrar el mismo monto que el mostrado en el Dashboard en la sección "CUENTAS CHEQUE MXN CONSOLIDADAS"</t>
+  </si>
+  <si>
+    <t>El usuario valida el monto mostrado en el campo "Saldo disponible".||El sistema debe mostrar el mismo monto que el mostrado en el Dashboard en la sección "CUENTAS CHEQUE MXN CONSOLIDADAS"</t>
+  </si>
+  <si>
+    <t>El usuario valida el formato mostrado en el campo "Saldo disponible".El sistema muestra el campo "Saldo disponible" de forma correcta con el siguiente formato:
+-Formato de moneda con signo $
+-Separación de miles y millones con separador de coma (,)
+-Signo de punto para decimales (.)
+-2 decimales</t>
+  </si>
+  <si>
+    <t>El usuario valida el monto mostrado en el campo "Saldo salvo buen cobro".||El sistema debe mostrar el mismo monto que el mostrado en el Dashboard en la sección "CUENTAS CHEQUE MXN CONSOLIDADAS"</t>
+  </si>
+  <si>
+    <t>El usuario valida el monto mostrado en el campo "Saldo bloqueado".||El sistema debe mostrar el mismo monto que el mostrado en el Dashboard en la sección "CUENTAS CHEQUE MXN CONSOLIDADAS" en el campo "Saldo límite de sobregiro".</t>
+  </si>
+  <si>
+    <t>El usuario valida el formato mostrado en el campo "Saldo bloqueado".||El sistema muestra el campo "Saldo límite de sobregiro" de forma correcta con el siguiente formato:
+-Formato de moneda con signo $
+-Separación de miles y millones con separador de coma (,)
+-Signo de punto para decimales (.)
+-2 decimales</t>
+  </si>
+  <si>
+    <t>El usuario valida el monto mostrado en el campo "Saldo bloqueado".||El sistema debe mostrar el mismo monto que la suma de las cuentas de la columna "Saldo bloqueado".</t>
   </si>
 </sst>
 </file>
@@ -3271,7 +3998,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -3425,6 +4152,18 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -3803,8 +4542,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BC159"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N40" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="T94" sqref="T94"/>
+    <sheetView tabSelected="1" topLeftCell="A77" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="D78" sqref="D78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9858,28 +10597,68 @@
       <c r="AO71" s="3"/>
       <c r="AP71" s="3"/>
     </row>
-    <row r="72" spans="1:42" ht="204.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="2"/>
+    <row r="72" spans="1:42" ht="149.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A72" s="2" t="s">
+        <v>681</v>
+      </c>
       <c r="B72" s="2"/>
-      <c r="C72" s="2"/>
-      <c r="D72" s="2"/>
-      <c r="E72" s="2"/>
-      <c r="F72" s="2"/>
-      <c r="G72" s="2"/>
-      <c r="H72" s="2"/>
-      <c r="I72" s="2"/>
-      <c r="J72" s="2"/>
-      <c r="K72" s="2"/>
-      <c r="L72" s="2"/>
-      <c r="M72" s="16"/>
-      <c r="N72" s="16"/>
-      <c r="O72" s="16"/>
-      <c r="P72" s="16"/>
-      <c r="Q72" s="16"/>
-      <c r="R72" s="16"/>
-      <c r="S72" s="16"/>
-      <c r="T72" s="16"/>
-      <c r="U72" s="16"/>
+      <c r="C72" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D72" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="E72" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="F72" s="26" t="s">
+        <v>35</v>
+      </c>
+      <c r="G72" s="20" t="s">
+        <v>36</v>
+      </c>
+      <c r="H72" s="2" t="s">
+        <v>669</v>
+      </c>
+      <c r="I72" s="2" t="s">
+        <v>579</v>
+      </c>
+      <c r="J72" s="2" t="s">
+        <v>670</v>
+      </c>
+      <c r="K72" s="2" t="s">
+        <v>585</v>
+      </c>
+      <c r="L72" s="2" t="s">
+        <v>671</v>
+      </c>
+      <c r="M72" s="16" t="s">
+        <v>672</v>
+      </c>
+      <c r="N72" s="16" t="s">
+        <v>673</v>
+      </c>
+      <c r="O72" s="16" t="s">
+        <v>674</v>
+      </c>
+      <c r="P72" s="16" t="s">
+        <v>675</v>
+      </c>
+      <c r="Q72" s="16" t="s">
+        <v>676</v>
+      </c>
+      <c r="R72" s="16" t="s">
+        <v>677</v>
+      </c>
+      <c r="S72" s="16" t="s">
+        <v>678</v>
+      </c>
+      <c r="T72" s="16" t="s">
+        <v>679</v>
+      </c>
+      <c r="U72" s="16" t="s">
+        <v>680</v>
+      </c>
       <c r="V72" s="16"/>
       <c r="W72" s="16"/>
       <c r="X72" s="16"/>
@@ -9902,22 +10681,50 @@
       <c r="AO72" s="3"/>
       <c r="AP72" s="3"/>
     </row>
-    <row r="73" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A73" s="2"/>
+    <row r="73" spans="1:42" ht="135" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A73" s="2" t="s">
+        <v>682</v>
+      </c>
       <c r="B73" s="2"/>
-      <c r="C73" s="2"/>
-      <c r="D73" s="2"/>
-      <c r="E73" s="2"/>
-      <c r="F73" s="2"/>
-      <c r="G73" s="2"/>
-      <c r="H73" s="2"/>
-      <c r="I73" s="2"/>
-      <c r="J73" s="2"/>
-      <c r="K73" s="2"/>
-      <c r="L73" s="2"/>
-      <c r="M73" s="16"/>
-      <c r="N73" s="16"/>
-      <c r="O73" s="16"/>
+      <c r="C73" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D73" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="E73" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="F73" s="26" t="s">
+        <v>35</v>
+      </c>
+      <c r="G73" s="20" t="s">
+        <v>36</v>
+      </c>
+      <c r="H73" s="2" t="s">
+        <v>683</v>
+      </c>
+      <c r="I73" s="2" t="s">
+        <v>579</v>
+      </c>
+      <c r="J73" s="2" t="s">
+        <v>684</v>
+      </c>
+      <c r="K73" s="2" t="s">
+        <v>585</v>
+      </c>
+      <c r="L73" s="2" t="s">
+        <v>685</v>
+      </c>
+      <c r="M73" s="16" t="s">
+        <v>686</v>
+      </c>
+      <c r="N73" s="43" t="s">
+        <v>687</v>
+      </c>
+      <c r="O73" s="16" t="s">
+        <v>674</v>
+      </c>
       <c r="P73" s="16"/>
       <c r="Q73" s="16"/>
       <c r="R73" s="16"/>
@@ -9946,20 +10753,68 @@
       <c r="AO73" s="3"/>
       <c r="AP73" s="3"/>
     </row>
-    <row r="74" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A74" s="2"/>
+    <row r="74" spans="1:42" ht="155.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A74" s="2" t="s">
+        <v>688</v>
+      </c>
       <c r="B74" s="2"/>
-      <c r="C74" s="2"/>
-      <c r="D74" s="2"/>
-      <c r="E74" s="2"/>
-      <c r="F74" s="2"/>
-      <c r="G74" s="2"/>
-      <c r="H74" s="2"/>
-      <c r="I74" s="2"/>
-      <c r="J74" s="2"/>
-      <c r="K74" s="2"/>
-      <c r="L74" s="2"/>
-      <c r="N74" s="5"/>
+      <c r="C74" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D74" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="E74" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="F74" s="26" t="s">
+        <v>35</v>
+      </c>
+      <c r="G74" s="20" t="s">
+        <v>36</v>
+      </c>
+      <c r="H74" s="2" t="s">
+        <v>689</v>
+      </c>
+      <c r="I74" s="2" t="s">
+        <v>579</v>
+      </c>
+      <c r="J74" s="2" t="s">
+        <v>690</v>
+      </c>
+      <c r="K74" s="2" t="s">
+        <v>585</v>
+      </c>
+      <c r="L74" s="2" t="s">
+        <v>691</v>
+      </c>
+      <c r="M74" s="53" t="s">
+        <v>692</v>
+      </c>
+      <c r="N74" s="2" t="s">
+        <v>693</v>
+      </c>
+      <c r="O74" s="53" t="s">
+        <v>694</v>
+      </c>
+      <c r="P74" s="54" t="s">
+        <v>695</v>
+      </c>
+      <c r="Q74" s="54" t="s">
+        <v>696</v>
+      </c>
+      <c r="R74" s="54" t="s">
+        <v>697</v>
+      </c>
+      <c r="S74" s="54" t="s">
+        <v>698</v>
+      </c>
+      <c r="T74" s="53" t="s">
+        <v>699</v>
+      </c>
+      <c r="U74" s="54" t="s">
+        <v>700</v>
+      </c>
       <c r="AC74" s="5"/>
       <c r="AD74" s="3"/>
       <c r="AE74" s="3"/>
@@ -9975,20 +10830,50 @@
       <c r="AO74" s="3"/>
       <c r="AP74" s="3"/>
     </row>
-    <row r="75" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A75" s="2"/>
+    <row r="75" spans="1:42" ht="152.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A75" s="2" t="s">
+        <v>701</v>
+      </c>
       <c r="B75" s="2"/>
-      <c r="C75" s="2"/>
-      <c r="D75" s="2"/>
-      <c r="E75" s="2"/>
-      <c r="F75" s="2"/>
-      <c r="G75" s="2"/>
-      <c r="H75" s="2"/>
-      <c r="I75" s="2"/>
-      <c r="J75" s="2"/>
-      <c r="K75" s="2"/>
-      <c r="L75" s="2"/>
-      <c r="N75" s="5"/>
+      <c r="C75" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D75" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="E75" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="F75" s="26" t="s">
+        <v>35</v>
+      </c>
+      <c r="G75" s="20" t="s">
+        <v>36</v>
+      </c>
+      <c r="H75" s="2" t="s">
+        <v>702</v>
+      </c>
+      <c r="I75" s="2" t="s">
+        <v>579</v>
+      </c>
+      <c r="J75" s="2" t="s">
+        <v>703</v>
+      </c>
+      <c r="K75" s="2" t="s">
+        <v>585</v>
+      </c>
+      <c r="L75" s="2" t="s">
+        <v>704</v>
+      </c>
+      <c r="M75" s="53" t="s">
+        <v>705</v>
+      </c>
+      <c r="N75" s="2" t="s">
+        <v>706</v>
+      </c>
+      <c r="O75" s="53" t="s">
+        <v>707</v>
+      </c>
       <c r="AC75" s="5"/>
       <c r="AD75" s="3"/>
       <c r="AE75" s="3"/>
@@ -10004,20 +10889,68 @@
       <c r="AO75" s="3"/>
       <c r="AP75" s="3"/>
     </row>
-    <row r="76" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A76" s="2"/>
+    <row r="76" spans="1:42" ht="153" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A76" s="2" t="s">
+        <v>708</v>
+      </c>
       <c r="B76" s="2"/>
-      <c r="C76" s="2"/>
-      <c r="D76" s="2"/>
-      <c r="E76" s="2"/>
-      <c r="F76" s="2"/>
-      <c r="G76" s="2"/>
-      <c r="H76" s="2"/>
-      <c r="I76" s="2"/>
-      <c r="J76" s="2"/>
-      <c r="K76" s="2"/>
-      <c r="L76" s="2"/>
-      <c r="N76" s="5"/>
+      <c r="C76" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D76" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="E76" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="F76" s="26" t="s">
+        <v>35</v>
+      </c>
+      <c r="G76" s="20" t="s">
+        <v>36</v>
+      </c>
+      <c r="H76" s="2" t="s">
+        <v>709</v>
+      </c>
+      <c r="I76" s="2" t="s">
+        <v>579</v>
+      </c>
+      <c r="J76" s="2" t="s">
+        <v>710</v>
+      </c>
+      <c r="K76" s="2" t="s">
+        <v>585</v>
+      </c>
+      <c r="L76" s="2" t="s">
+        <v>711</v>
+      </c>
+      <c r="M76" s="53" t="s">
+        <v>712</v>
+      </c>
+      <c r="N76" s="2" t="s">
+        <v>713</v>
+      </c>
+      <c r="O76" s="53" t="s">
+        <v>714</v>
+      </c>
+      <c r="P76" s="55" t="s">
+        <v>715</v>
+      </c>
+      <c r="Q76" s="56" t="s">
+        <v>716</v>
+      </c>
+      <c r="R76" s="55" t="s">
+        <v>717</v>
+      </c>
+      <c r="S76" s="56" t="s">
+        <v>718</v>
+      </c>
+      <c r="T76" s="56" t="s">
+        <v>719</v>
+      </c>
+      <c r="U76" s="56" t="s">
+        <v>720</v>
+      </c>
       <c r="AC76" s="5"/>
       <c r="AD76" s="3"/>
       <c r="AE76" s="3"/>
@@ -10033,20 +10966,77 @@
       <c r="AO76" s="3"/>
       <c r="AP76" s="3"/>
     </row>
-    <row r="77" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A77" s="2"/>
+    <row r="77" spans="1:42" ht="164.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A77" s="2" t="s">
+        <v>721</v>
+      </c>
       <c r="B77" s="2"/>
-      <c r="C77" s="2"/>
-      <c r="D77" s="2"/>
-      <c r="E77" s="2"/>
-      <c r="F77" s="2"/>
-      <c r="G77" s="2"/>
-      <c r="H77" s="2"/>
-      <c r="I77" s="2"/>
-      <c r="J77" s="2"/>
-      <c r="K77" s="2"/>
-      <c r="L77" s="2"/>
-      <c r="N77" s="5"/>
+      <c r="C77" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D77" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="E77" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="F77" s="26" t="s">
+        <v>35</v>
+      </c>
+      <c r="G77" s="20" t="s">
+        <v>36</v>
+      </c>
+      <c r="H77" s="2" t="s">
+        <v>722</v>
+      </c>
+      <c r="I77" s="2" t="s">
+        <v>579</v>
+      </c>
+      <c r="J77" s="2" t="s">
+        <v>723</v>
+      </c>
+      <c r="K77" s="2" t="s">
+        <v>585</v>
+      </c>
+      <c r="L77" s="2" t="s">
+        <v>724</v>
+      </c>
+      <c r="M77" s="53" t="s">
+        <v>725</v>
+      </c>
+      <c r="N77" s="2" t="s">
+        <v>687</v>
+      </c>
+      <c r="O77" s="53" t="s">
+        <v>674</v>
+      </c>
+      <c r="P77" s="55" t="s">
+        <v>726</v>
+      </c>
+      <c r="Q77" s="56" t="s">
+        <v>713</v>
+      </c>
+      <c r="R77" s="55" t="s">
+        <v>714</v>
+      </c>
+      <c r="S77" s="56" t="s">
+        <v>727</v>
+      </c>
+      <c r="T77" s="56" t="s">
+        <v>728</v>
+      </c>
+      <c r="U77" s="56" t="s">
+        <v>729</v>
+      </c>
+      <c r="V77" s="2" t="s">
+        <v>730</v>
+      </c>
+      <c r="W77" s="2" t="s">
+        <v>731</v>
+      </c>
+      <c r="X77" s="56" t="s">
+        <v>732</v>
+      </c>
       <c r="AC77" s="5"/>
       <c r="AD77" s="3"/>
       <c r="AE77" s="3"/>
@@ -10062,20 +11052,77 @@
       <c r="AO77" s="3"/>
       <c r="AP77" s="3"/>
     </row>
-    <row r="78" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A78" s="2"/>
+    <row r="78" spans="1:42" ht="150.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A78" s="2" t="s">
+        <v>733</v>
+      </c>
       <c r="B78" s="2"/>
-      <c r="C78" s="2"/>
-      <c r="D78" s="2"/>
-      <c r="E78" s="2"/>
-      <c r="F78" s="2"/>
-      <c r="G78" s="2"/>
-      <c r="H78" s="2"/>
-      <c r="I78" s="2"/>
-      <c r="J78" s="2"/>
-      <c r="K78" s="2"/>
-      <c r="L78" s="2"/>
-      <c r="N78" s="5"/>
+      <c r="C78" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D78" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="E78" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="F78" s="26" t="s">
+        <v>35</v>
+      </c>
+      <c r="G78" s="20" t="s">
+        <v>36</v>
+      </c>
+      <c r="H78" s="2" t="s">
+        <v>734</v>
+      </c>
+      <c r="I78" s="2" t="s">
+        <v>579</v>
+      </c>
+      <c r="J78" s="2" t="s">
+        <v>735</v>
+      </c>
+      <c r="K78" s="2" t="s">
+        <v>585</v>
+      </c>
+      <c r="L78" s="2" t="s">
+        <v>736</v>
+      </c>
+      <c r="M78" s="53" t="s">
+        <v>737</v>
+      </c>
+      <c r="N78" s="2" t="s">
+        <v>687</v>
+      </c>
+      <c r="O78" s="53" t="s">
+        <v>674</v>
+      </c>
+      <c r="P78" s="55" t="s">
+        <v>738</v>
+      </c>
+      <c r="Q78" s="56" t="s">
+        <v>739</v>
+      </c>
+      <c r="R78" s="55" t="s">
+        <v>714</v>
+      </c>
+      <c r="S78" s="56" t="s">
+        <v>740</v>
+      </c>
+      <c r="T78" s="2" t="s">
+        <v>728</v>
+      </c>
+      <c r="U78" s="56" t="s">
+        <v>729</v>
+      </c>
+      <c r="V78" s="2" t="s">
+        <v>741</v>
+      </c>
+      <c r="W78" s="56" t="s">
+        <v>742</v>
+      </c>
+      <c r="X78" s="2" t="s">
+        <v>743</v>
+      </c>
       <c r="AC78" s="5"/>
       <c r="AD78" s="3"/>
       <c r="AE78" s="3"/>
@@ -10091,19 +11138,53 @@
       <c r="AO78" s="3"/>
       <c r="AP78" s="3"/>
     </row>
-    <row r="79" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A79" s="2"/>
+    <row r="79" spans="1:42" ht="150" x14ac:dyDescent="0.25">
+      <c r="A79" s="2" t="s">
+        <v>574</v>
+      </c>
       <c r="B79" s="2"/>
-      <c r="C79" s="2"/>
-      <c r="D79" s="2"/>
-      <c r="E79" s="2"/>
-      <c r="F79" s="2"/>
-      <c r="G79" s="2"/>
-      <c r="H79" s="2"/>
-      <c r="I79" s="2"/>
-      <c r="J79" s="2"/>
-      <c r="K79" s="2"/>
-      <c r="L79" s="2"/>
+      <c r="C79" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D79" s="2" t="s">
+        <v>575</v>
+      </c>
+      <c r="E79" s="2" t="s">
+        <v>576</v>
+      </c>
+      <c r="F79" s="2" t="s">
+        <v>577</v>
+      </c>
+      <c r="G79" s="2" t="s">
+        <v>578</v>
+      </c>
+      <c r="H79" s="2" t="s">
+        <v>579</v>
+      </c>
+      <c r="I79" s="2" t="s">
+        <v>580</v>
+      </c>
+      <c r="J79" s="2" t="s">
+        <v>581</v>
+      </c>
+      <c r="K79" s="2" t="s">
+        <v>582</v>
+      </c>
+      <c r="L79" s="2" t="s">
+        <v>583</v>
+      </c>
+      <c r="M79" s="2" t="s">
+        <v>584</v>
+      </c>
+      <c r="N79" s="2" t="s">
+        <v>523</v>
+      </c>
+      <c r="O79" s="2" t="s">
+        <v>585</v>
+      </c>
+      <c r="P79" s="2" t="s">
+        <v>586</v>
+      </c>
       <c r="AC79" s="5"/>
       <c r="AD79" s="3"/>
       <c r="AE79" s="3"/>
@@ -10119,19 +11200,53 @@
       <c r="AO79" s="3"/>
       <c r="AP79" s="3"/>
     </row>
-    <row r="80" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A80" s="2"/>
+    <row r="80" spans="1:42" ht="150" x14ac:dyDescent="0.25">
+      <c r="A80" s="2" t="s">
+        <v>587</v>
+      </c>
       <c r="B80" s="2"/>
-      <c r="C80" s="2"/>
-      <c r="D80" s="2"/>
-      <c r="E80" s="2"/>
-      <c r="F80" s="2"/>
-      <c r="G80" s="2"/>
-      <c r="H80" s="2"/>
-      <c r="I80" s="2"/>
-      <c r="J80" s="2"/>
-      <c r="K80" s="2"/>
-      <c r="L80" s="2"/>
+      <c r="C80" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D80" s="2" t="s">
+        <v>575</v>
+      </c>
+      <c r="E80" s="2" t="s">
+        <v>576</v>
+      </c>
+      <c r="F80" s="2" t="s">
+        <v>577</v>
+      </c>
+      <c r="G80" s="2" t="s">
+        <v>578</v>
+      </c>
+      <c r="H80" s="2" t="s">
+        <v>579</v>
+      </c>
+      <c r="I80" s="2" t="s">
+        <v>588</v>
+      </c>
+      <c r="J80" s="2" t="s">
+        <v>581</v>
+      </c>
+      <c r="K80" s="2" t="s">
+        <v>582</v>
+      </c>
+      <c r="L80" s="2" t="s">
+        <v>589</v>
+      </c>
+      <c r="M80" s="2" t="s">
+        <v>590</v>
+      </c>
+      <c r="N80" s="2" t="s">
+        <v>523</v>
+      </c>
+      <c r="O80" s="2" t="s">
+        <v>585</v>
+      </c>
+      <c r="P80" s="4" t="s">
+        <v>586</v>
+      </c>
       <c r="AC80" s="5"/>
       <c r="AD80" s="3"/>
       <c r="AE80" s="3"/>
@@ -10147,19 +11262,47 @@
       <c r="AO80" s="3"/>
       <c r="AP80" s="3"/>
     </row>
-    <row r="81" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A81" s="2"/>
+    <row r="81" spans="1:42" ht="135" x14ac:dyDescent="0.25">
+      <c r="A81" s="2" t="s">
+        <v>591</v>
+      </c>
       <c r="B81" s="2"/>
-      <c r="C81" s="2"/>
-      <c r="D81" s="2"/>
-      <c r="E81" s="2"/>
-      <c r="F81" s="2"/>
-      <c r="G81" s="2"/>
-      <c r="H81" s="2"/>
-      <c r="I81" s="2"/>
-      <c r="J81" s="2"/>
-      <c r="K81" s="2"/>
-      <c r="L81" s="2"/>
+      <c r="C81" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D81" s="2" t="s">
+        <v>575</v>
+      </c>
+      <c r="E81" s="2" t="s">
+        <v>576</v>
+      </c>
+      <c r="F81" s="2" t="s">
+        <v>577</v>
+      </c>
+      <c r="G81" s="2" t="s">
+        <v>578</v>
+      </c>
+      <c r="H81" s="2" t="s">
+        <v>579</v>
+      </c>
+      <c r="I81" s="2" t="s">
+        <v>592</v>
+      </c>
+      <c r="J81" s="2" t="s">
+        <v>593</v>
+      </c>
+      <c r="K81" s="2" t="s">
+        <v>594</v>
+      </c>
+      <c r="L81" s="2" t="s">
+        <v>523</v>
+      </c>
+      <c r="M81" s="2" t="s">
+        <v>585</v>
+      </c>
+      <c r="N81" s="2" t="s">
+        <v>586</v>
+      </c>
       <c r="AD81" s="4"/>
       <c r="AE81" s="4"/>
       <c r="AF81" s="4"/>
@@ -10174,83 +11317,253 @@
       <c r="AO81" s="3"/>
       <c r="AP81" s="3"/>
     </row>
-    <row r="82" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A82" s="2"/>
+    <row r="82" spans="1:42" ht="150" x14ac:dyDescent="0.25">
+      <c r="A82" s="2" t="s">
+        <v>595</v>
+      </c>
       <c r="B82" s="2"/>
-      <c r="C82" s="2"/>
-      <c r="D82" s="2"/>
-      <c r="E82" s="2"/>
-      <c r="F82" s="2"/>
-      <c r="G82" s="2"/>
-      <c r="H82" s="2"/>
-      <c r="I82" s="2"/>
-      <c r="J82" s="2"/>
-      <c r="K82" s="2"/>
-      <c r="L82" s="2"/>
+      <c r="C82" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D82" s="2" t="s">
+        <v>575</v>
+      </c>
+      <c r="E82" s="2" t="s">
+        <v>576</v>
+      </c>
+      <c r="F82" s="2" t="s">
+        <v>577</v>
+      </c>
+      <c r="G82" s="2" t="s">
+        <v>578</v>
+      </c>
+      <c r="H82" s="2" t="s">
+        <v>579</v>
+      </c>
+      <c r="I82" s="2" t="s">
+        <v>596</v>
+      </c>
+      <c r="J82" s="2" t="s">
+        <v>597</v>
+      </c>
+      <c r="K82" s="2" t="s">
+        <v>598</v>
+      </c>
+      <c r="L82" s="2" t="s">
+        <v>599</v>
+      </c>
+      <c r="M82" s="2" t="s">
+        <v>600</v>
+      </c>
+      <c r="N82" s="2" t="s">
+        <v>523</v>
+      </c>
+      <c r="O82" s="2" t="s">
+        <v>585</v>
+      </c>
+      <c r="P82" s="4" t="s">
+        <v>586</v>
+      </c>
       <c r="AO82" s="3"/>
       <c r="AP82" s="3"/>
     </row>
-    <row r="83" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A83" s="2"/>
+    <row r="83" spans="1:42" ht="150" x14ac:dyDescent="0.25">
+      <c r="A83" s="2" t="s">
+        <v>601</v>
+      </c>
       <c r="B83" s="2"/>
-      <c r="C83" s="2"/>
-      <c r="D83" s="2"/>
-      <c r="E83" s="2"/>
-      <c r="F83" s="2"/>
-      <c r="G83" s="2"/>
-      <c r="H83" s="2"/>
-      <c r="I83" s="2"/>
-      <c r="J83" s="2"/>
-      <c r="K83" s="2"/>
-      <c r="L83" s="2"/>
+      <c r="C83" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D83" s="2" t="s">
+        <v>575</v>
+      </c>
+      <c r="E83" s="2" t="s">
+        <v>576</v>
+      </c>
+      <c r="F83" s="2" t="s">
+        <v>577</v>
+      </c>
+      <c r="G83" s="2" t="s">
+        <v>578</v>
+      </c>
+      <c r="H83" s="2" t="s">
+        <v>579</v>
+      </c>
+      <c r="I83" s="2" t="s">
+        <v>602</v>
+      </c>
+      <c r="J83" s="2" t="s">
+        <v>593</v>
+      </c>
+      <c r="K83" s="2" t="s">
+        <v>603</v>
+      </c>
+      <c r="L83" s="2" t="s">
+        <v>523</v>
+      </c>
+      <c r="M83" s="2" t="s">
+        <v>585</v>
+      </c>
+      <c r="N83" s="4" t="s">
+        <v>586</v>
+      </c>
       <c r="AO83" s="3"/>
       <c r="AP83" s="3"/>
     </row>
-    <row r="84" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A84" s="2"/>
+    <row r="84" spans="1:42" ht="150" x14ac:dyDescent="0.25">
+      <c r="A84" s="2" t="s">
+        <v>604</v>
+      </c>
       <c r="B84" s="2"/>
-      <c r="C84" s="2"/>
-      <c r="D84" s="2"/>
-      <c r="E84" s="2"/>
-      <c r="F84" s="2"/>
-      <c r="G84" s="2"/>
-      <c r="H84" s="2"/>
-      <c r="I84" s="2"/>
-      <c r="J84" s="2"/>
-      <c r="K84" s="2"/>
-      <c r="L84" s="2"/>
+      <c r="C84" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D84" s="2" t="s">
+        <v>575</v>
+      </c>
+      <c r="E84" s="2" t="s">
+        <v>576</v>
+      </c>
+      <c r="F84" s="2" t="s">
+        <v>577</v>
+      </c>
+      <c r="G84" s="2" t="s">
+        <v>578</v>
+      </c>
+      <c r="H84" s="2" t="s">
+        <v>579</v>
+      </c>
+      <c r="I84" s="2" t="s">
+        <v>605</v>
+      </c>
+      <c r="J84" s="2" t="s">
+        <v>606</v>
+      </c>
+      <c r="K84" s="2" t="s">
+        <v>607</v>
+      </c>
+      <c r="L84" s="2" t="s">
+        <v>608</v>
+      </c>
+      <c r="M84" s="2" t="s">
+        <v>609</v>
+      </c>
+      <c r="N84" s="2" t="s">
+        <v>523</v>
+      </c>
+      <c r="O84" s="2" t="s">
+        <v>585</v>
+      </c>
+      <c r="P84" s="4" t="s">
+        <v>586</v>
+      </c>
       <c r="AO84" s="3"/>
       <c r="AP84" s="3"/>
     </row>
-    <row r="85" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A85" s="2"/>
+    <row r="85" spans="1:42" ht="150" x14ac:dyDescent="0.25">
+      <c r="A85" s="2" t="s">
+        <v>610</v>
+      </c>
       <c r="B85" s="2"/>
-      <c r="C85" s="2"/>
-      <c r="D85" s="2"/>
-      <c r="E85" s="2"/>
-      <c r="F85" s="2"/>
-      <c r="G85" s="2"/>
-      <c r="H85" s="2"/>
-      <c r="I85" s="2"/>
-      <c r="J85" s="2"/>
-      <c r="K85" s="2"/>
-      <c r="L85" s="2"/>
+      <c r="C85" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D85" s="2" t="s">
+        <v>575</v>
+      </c>
+      <c r="E85" s="2" t="s">
+        <v>576</v>
+      </c>
+      <c r="F85" s="2" t="s">
+        <v>577</v>
+      </c>
+      <c r="G85" s="2" t="s">
+        <v>578</v>
+      </c>
+      <c r="H85" s="2" t="s">
+        <v>579</v>
+      </c>
+      <c r="I85" s="2" t="s">
+        <v>611</v>
+      </c>
+      <c r="J85" s="2" t="s">
+        <v>612</v>
+      </c>
+      <c r="K85" s="2" t="s">
+        <v>613</v>
+      </c>
+      <c r="L85" s="2" t="s">
+        <v>614</v>
+      </c>
+      <c r="M85" s="2" t="s">
+        <v>615</v>
+      </c>
+      <c r="N85" s="2" t="s">
+        <v>616</v>
+      </c>
+      <c r="O85" s="2" t="s">
+        <v>523</v>
+      </c>
+      <c r="P85" s="2" t="s">
+        <v>585</v>
+      </c>
+      <c r="Q85" s="2" t="s">
+        <v>586</v>
+      </c>
       <c r="AO85" s="3"/>
       <c r="AP85" s="3"/>
     </row>
-    <row r="86" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A86" s="2"/>
+    <row r="86" spans="1:42" ht="135" x14ac:dyDescent="0.25">
+      <c r="A86" s="2" t="s">
+        <v>617</v>
+      </c>
       <c r="B86" s="2"/>
-      <c r="C86" s="2"/>
-      <c r="D86" s="2"/>
-      <c r="E86" s="2"/>
-      <c r="F86" s="2"/>
-      <c r="G86" s="2"/>
-      <c r="H86" s="2"/>
-      <c r="I86" s="2"/>
-      <c r="J86" s="2"/>
-      <c r="K86" s="2"/>
-      <c r="L86" s="2"/>
+      <c r="C86" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D86" s="2" t="s">
+        <v>575</v>
+      </c>
+      <c r="E86" s="2" t="s">
+        <v>576</v>
+      </c>
+      <c r="F86" s="2" t="s">
+        <v>577</v>
+      </c>
+      <c r="G86" s="2" t="s">
+        <v>578</v>
+      </c>
+      <c r="H86" s="2" t="s">
+        <v>579</v>
+      </c>
+      <c r="I86" s="2" t="s">
+        <v>618</v>
+      </c>
+      <c r="J86" s="2" t="s">
+        <v>612</v>
+      </c>
+      <c r="K86" s="2" t="s">
+        <v>613</v>
+      </c>
+      <c r="L86" s="2" t="s">
+        <v>619</v>
+      </c>
+      <c r="M86" s="4" t="s">
+        <v>620</v>
+      </c>
+      <c r="N86" s="4" t="s">
+        <v>621</v>
+      </c>
+      <c r="O86" s="2" t="s">
+        <v>523</v>
+      </c>
+      <c r="P86" s="2" t="s">
+        <v>585</v>
+      </c>
+      <c r="Q86" s="4" t="s">
+        <v>586</v>
+      </c>
       <c r="AO86" s="3"/>
       <c r="AP86" s="3"/>
     </row>
@@ -10750,156 +12063,358 @@
       <c r="AO94" s="3"/>
       <c r="AP94" s="3"/>
     </row>
-    <row r="95" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A95" s="2"/>
+    <row r="95" spans="1:42" ht="150" x14ac:dyDescent="0.25">
+      <c r="A95" s="2" t="s">
+        <v>622</v>
+      </c>
       <c r="B95" s="2"/>
-      <c r="C95" s="2"/>
-      <c r="D95" s="2"/>
-      <c r="E95" s="2"/>
-      <c r="F95" s="2"/>
-      <c r="G95" s="2"/>
-      <c r="H95" s="2"/>
-      <c r="I95" s="2"/>
-      <c r="J95" s="2"/>
-      <c r="K95" s="2"/>
-      <c r="L95" s="2"/>
+      <c r="C95" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D95" s="2" t="s">
+        <v>575</v>
+      </c>
+      <c r="E95" s="2" t="s">
+        <v>576</v>
+      </c>
+      <c r="F95" s="2" t="s">
+        <v>577</v>
+      </c>
+      <c r="G95" s="2" t="s">
+        <v>578</v>
+      </c>
+      <c r="H95" s="2" t="s">
+        <v>623</v>
+      </c>
+      <c r="I95" s="2" t="s">
+        <v>624</v>
+      </c>
+      <c r="J95" s="2" t="s">
+        <v>625</v>
+      </c>
+      <c r="K95" s="2" t="s">
+        <v>626</v>
+      </c>
+      <c r="L95" s="2" t="s">
+        <v>627</v>
+      </c>
       <c r="AO95" s="3"/>
       <c r="AP95" s="3"/>
     </row>
-    <row r="96" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A96" s="2"/>
+    <row r="96" spans="1:42" ht="135" x14ac:dyDescent="0.25">
+      <c r="A96" s="2" t="s">
+        <v>628</v>
+      </c>
       <c r="B96" s="2"/>
-      <c r="C96" s="2"/>
-      <c r="D96" s="2"/>
-      <c r="E96" s="2"/>
-      <c r="F96" s="2"/>
-      <c r="G96" s="2"/>
-      <c r="H96" s="2"/>
-      <c r="I96" s="2"/>
-      <c r="J96" s="2"/>
-      <c r="K96" s="2"/>
-      <c r="L96" s="2"/>
+      <c r="C96" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D96" s="2" t="s">
+        <v>575</v>
+      </c>
+      <c r="E96" s="2" t="s">
+        <v>576</v>
+      </c>
+      <c r="F96" s="2" t="s">
+        <v>577</v>
+      </c>
+      <c r="G96" s="2" t="s">
+        <v>578</v>
+      </c>
+      <c r="H96" s="2" t="s">
+        <v>629</v>
+      </c>
+      <c r="I96" s="2" t="s">
+        <v>630</v>
+      </c>
+      <c r="J96" s="2" t="s">
+        <v>631</v>
+      </c>
+      <c r="K96" s="2" t="s">
+        <v>632</v>
+      </c>
+      <c r="L96" s="2" t="s">
+        <v>633</v>
+      </c>
       <c r="AO96" s="3"/>
       <c r="AP96" s="3"/>
     </row>
-    <row r="97" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A97" s="2"/>
+    <row r="97" spans="1:42" ht="135" x14ac:dyDescent="0.25">
+      <c r="A97" s="2" t="s">
+        <v>634</v>
+      </c>
       <c r="B97" s="2"/>
-      <c r="C97" s="2"/>
-      <c r="D97" s="2"/>
-      <c r="E97" s="2"/>
-      <c r="F97" s="2"/>
-      <c r="G97" s="2"/>
-      <c r="H97" s="2"/>
-      <c r="I97" s="2"/>
-      <c r="J97" s="2"/>
+      <c r="C97" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D97" s="2" t="s">
+        <v>575</v>
+      </c>
+      <c r="E97" s="2" t="s">
+        <v>576</v>
+      </c>
+      <c r="F97" s="2" t="s">
+        <v>577</v>
+      </c>
+      <c r="G97" s="2" t="s">
+        <v>578</v>
+      </c>
+      <c r="H97" s="2" t="s">
+        <v>635</v>
+      </c>
+      <c r="I97" s="2" t="s">
+        <v>636</v>
+      </c>
+      <c r="J97" s="2" t="s">
+        <v>637</v>
+      </c>
       <c r="K97" s="2"/>
       <c r="L97" s="2"/>
       <c r="AO97" s="3"/>
       <c r="AP97" s="3"/>
     </row>
-    <row r="98" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A98" s="2"/>
+    <row r="98" spans="1:42" ht="150" x14ac:dyDescent="0.25">
+      <c r="A98" s="2" t="s">
+        <v>638</v>
+      </c>
       <c r="B98" s="2"/>
-      <c r="C98" s="2"/>
-      <c r="D98" s="2"/>
-      <c r="E98" s="2"/>
-      <c r="F98" s="2"/>
-      <c r="G98" s="2"/>
-      <c r="H98" s="2"/>
-      <c r="I98" s="2"/>
-      <c r="J98" s="2"/>
-      <c r="K98" s="2"/>
-      <c r="L98" s="2"/>
+      <c r="C98" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D98" s="2" t="s">
+        <v>575</v>
+      </c>
+      <c r="E98" s="2" t="s">
+        <v>576</v>
+      </c>
+      <c r="F98" s="2" t="s">
+        <v>577</v>
+      </c>
+      <c r="G98" s="2" t="s">
+        <v>578</v>
+      </c>
+      <c r="H98" s="2" t="s">
+        <v>639</v>
+      </c>
+      <c r="I98" s="2" t="s">
+        <v>640</v>
+      </c>
+      <c r="J98" s="2" t="s">
+        <v>641</v>
+      </c>
+      <c r="K98" s="2" t="s">
+        <v>642</v>
+      </c>
+      <c r="L98" s="2" t="s">
+        <v>643</v>
+      </c>
       <c r="AO98" s="3"/>
       <c r="AP98" s="3"/>
     </row>
-    <row r="99" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A99" s="2"/>
+    <row r="99" spans="1:42" ht="150" x14ac:dyDescent="0.25">
+      <c r="A99" s="2" t="s">
+        <v>644</v>
+      </c>
       <c r="B99" s="2"/>
-      <c r="C99" s="2"/>
-      <c r="D99" s="2"/>
-      <c r="E99" s="2"/>
-      <c r="F99" s="2"/>
-      <c r="G99" s="2"/>
-      <c r="H99" s="2"/>
-      <c r="I99" s="2"/>
-      <c r="J99" s="2"/>
+      <c r="C99" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D99" s="2" t="s">
+        <v>575</v>
+      </c>
+      <c r="E99" s="2" t="s">
+        <v>576</v>
+      </c>
+      <c r="F99" s="2" t="s">
+        <v>577</v>
+      </c>
+      <c r="G99" s="2" t="s">
+        <v>578</v>
+      </c>
+      <c r="H99" s="2" t="s">
+        <v>645</v>
+      </c>
+      <c r="I99" s="2" t="s">
+        <v>646</v>
+      </c>
+      <c r="J99" s="2" t="s">
+        <v>647</v>
+      </c>
       <c r="K99" s="2"/>
       <c r="L99" s="2"/>
       <c r="AO99" s="3"/>
       <c r="AP99" s="3"/>
     </row>
-    <row r="100" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A100" s="2"/>
+    <row r="100" spans="1:42" ht="135" x14ac:dyDescent="0.25">
+      <c r="A100" s="2" t="s">
+        <v>648</v>
+      </c>
       <c r="B100" s="2"/>
-      <c r="C100" s="2"/>
-      <c r="D100" s="2"/>
-      <c r="E100" s="2"/>
-      <c r="F100" s="2"/>
-      <c r="G100" s="2"/>
-      <c r="H100" s="2"/>
-      <c r="I100" s="2"/>
-      <c r="J100" s="2"/>
-      <c r="K100" s="2"/>
-      <c r="L100" s="2"/>
+      <c r="C100" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D100" s="2" t="s">
+        <v>575</v>
+      </c>
+      <c r="E100" s="2" t="s">
+        <v>576</v>
+      </c>
+      <c r="F100" s="2" t="s">
+        <v>577</v>
+      </c>
+      <c r="G100" s="2" t="s">
+        <v>578</v>
+      </c>
+      <c r="H100" s="2" t="s">
+        <v>649</v>
+      </c>
+      <c r="I100" s="2" t="s">
+        <v>650</v>
+      </c>
+      <c r="J100" s="2" t="s">
+        <v>651</v>
+      </c>
+      <c r="K100" s="2" t="s">
+        <v>652</v>
+      </c>
+      <c r="L100" s="2" t="s">
+        <v>653</v>
+      </c>
       <c r="AO100" s="3"/>
       <c r="AP100" s="3"/>
     </row>
-    <row r="101" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A101" s="2"/>
+    <row r="101" spans="1:42" ht="135" x14ac:dyDescent="0.25">
+      <c r="A101" s="2" t="s">
+        <v>654</v>
+      </c>
       <c r="B101" s="2"/>
-      <c r="C101" s="2"/>
-      <c r="D101" s="2"/>
-      <c r="E101" s="2"/>
-      <c r="F101" s="2"/>
-      <c r="G101" s="2"/>
-      <c r="H101" s="2"/>
-      <c r="I101" s="2"/>
-      <c r="J101" s="2"/>
-      <c r="K101" s="2"/>
-      <c r="L101" s="2"/>
+      <c r="C101" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D101" s="2" t="s">
+        <v>575</v>
+      </c>
+      <c r="E101" s="2" t="s">
+        <v>576</v>
+      </c>
+      <c r="F101" s="2" t="s">
+        <v>577</v>
+      </c>
+      <c r="G101" s="2" t="s">
+        <v>578</v>
+      </c>
+      <c r="H101" s="2" t="s">
+        <v>655</v>
+      </c>
+      <c r="I101" s="2" t="s">
+        <v>656</v>
+      </c>
+      <c r="J101" s="2" t="s">
+        <v>631</v>
+      </c>
+      <c r="K101" s="2" t="s">
+        <v>651</v>
+      </c>
+      <c r="L101" s="2" t="s">
+        <v>657</v>
+      </c>
+      <c r="M101" s="2" t="s">
+        <v>658</v>
+      </c>
       <c r="AO101" s="3"/>
       <c r="AP101" s="3"/>
     </row>
-    <row r="102" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A102" s="2"/>
+    <row r="102" spans="1:42" ht="135" x14ac:dyDescent="0.25">
+      <c r="A102" s="2" t="s">
+        <v>659</v>
+      </c>
       <c r="B102" s="2"/>
-      <c r="C102" s="2"/>
-      <c r="D102" s="2"/>
-      <c r="E102" s="2"/>
-      <c r="F102" s="2"/>
-      <c r="G102" s="2"/>
-      <c r="H102" s="2"/>
-      <c r="I102" s="2"/>
-      <c r="J102" s="2"/>
-      <c r="K102" s="2"/>
-      <c r="L102" s="2"/>
+      <c r="C102" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D102" s="2" t="s">
+        <v>575</v>
+      </c>
+      <c r="E102" s="2" t="s">
+        <v>576</v>
+      </c>
+      <c r="F102" s="2" t="s">
+        <v>577</v>
+      </c>
+      <c r="G102" s="2" t="s">
+        <v>578</v>
+      </c>
+      <c r="H102" s="2" t="s">
+        <v>660</v>
+      </c>
+      <c r="I102" s="2" t="s">
+        <v>661</v>
+      </c>
+      <c r="J102" s="2" t="s">
+        <v>631</v>
+      </c>
+      <c r="K102" s="2" t="s">
+        <v>662</v>
+      </c>
+      <c r="L102" s="2" t="s">
+        <v>663</v>
+      </c>
+      <c r="M102" s="4" t="s">
+        <v>664</v>
+      </c>
       <c r="AO102" s="3"/>
       <c r="AP102" s="3"/>
     </row>
-    <row r="103" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A103" s="2"/>
+    <row r="103" spans="1:42" ht="105" x14ac:dyDescent="0.25">
+      <c r="A103" s="2" t="s">
+        <v>665</v>
+      </c>
       <c r="B103" s="2"/>
-      <c r="C103" s="2"/>
-      <c r="D103" s="2"/>
-      <c r="E103" s="2"/>
-      <c r="F103" s="2"/>
-      <c r="G103" s="2"/>
-      <c r="H103" s="2"/>
-      <c r="I103" s="2"/>
+      <c r="C103" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D103" s="2" t="s">
+        <v>575</v>
+      </c>
+      <c r="E103" s="2" t="s">
+        <v>576</v>
+      </c>
+      <c r="F103" s="2" t="s">
+        <v>577</v>
+      </c>
+      <c r="G103" s="2" t="s">
+        <v>578</v>
+      </c>
+      <c r="H103" s="2" t="s">
+        <v>666</v>
+      </c>
+      <c r="I103" s="2" t="s">
+        <v>667</v>
+      </c>
       <c r="J103" s="2"/>
       <c r="K103" s="2"/>
       <c r="L103" s="2"/>
     </row>
-    <row r="104" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A104" s="2"/>
+    <row r="104" spans="1:42" ht="105" x14ac:dyDescent="0.25">
+      <c r="A104" s="2" t="s">
+        <v>668</v>
+      </c>
       <c r="B104" s="2"/>
-      <c r="C104" s="2"/>
-      <c r="D104" s="2"/>
-      <c r="E104" s="2"/>
-      <c r="F104" s="2"/>
-      <c r="G104" s="2"/>
+      <c r="C104" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D104" s="2" t="s">
+        <v>575</v>
+      </c>
+      <c r="E104" s="2" t="s">
+        <v>576</v>
+      </c>
+      <c r="F104" s="2" t="s">
+        <v>577</v>
+      </c>
+      <c r="G104" s="2" t="s">
+        <v>578</v>
+      </c>
       <c r="H104" s="2"/>
       <c r="I104" s="2"/>
       <c r="J104" s="2"/>

</xml_diff>

<commit_message>
refactorización de escenarios cucumber
</commit_message>
<xml_diff>
--- a/src/test/resources/Descriptions/DC_AUT_002_CashManagmentTest.xlsx
+++ b/src/test/resources/Descriptions/DC_AUT_002_CashManagmentTest.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20395"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96ED278F-C8E3-4663-93CD-22B9A9F42264}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDB74858-5732-4D41-8815-90217C3825A3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2264" uniqueCount="744">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2276" uniqueCount="755">
   <si>
     <t>Escenario</t>
   </si>
@@ -2407,9 +2407,6 @@
     <t>El usuario valida el campo "Tasa".||El sistema muestra la tasa de forma correcta.</t>
   </si>
   <si>
-    <t>TC_002_62_administradorConsultaCuentasLineaOperativaPDF</t>
-  </si>
-  <si>
     <t>El usuario valida el campo "Descripción del préstamo".||El sistema muestra la descripción del préstamo de forma correcta.</t>
   </si>
   <si>
@@ -2742,9 +2739,6 @@
 Columna "Saldo final importe de capital"</t>
   </si>
   <si>
-    <t>TC_002_63_administradorConsultaCuentasPrestamosPersonalesPDF</t>
-  </si>
-  <si>
     <t>TC_002_64_administradorConsultaCuentasFondosInversionPDF</t>
   </si>
   <si>
@@ -2956,33 +2950,12 @@
     <t>El usuario valida el monto mostrado en el campo "Importe autorizado".||El sistema debe mostrar el mismo monto que la suma de las cuentas de la columna "Importe autorizado".</t>
   </si>
   <si>
-    <t>TC_002_86_administradorConsultaCuentasLineaOperativaCSV</t>
-  </si>
-  <si>
     <t>El usuario da clic en la opción "Descarga".||El sistema muestra la página "Opciones de descarga" con las opciones "Manual" y "Plantilla".</t>
   </si>
   <si>
-    <t>TC_002_87_administradorConsultaCuentasPrestamosPersonalesTXT</t>
-  </si>
-  <si>
     <t>El usuario habilita la opción "Archivo con encabezado"||El sistema permite habilitar el radio botton de forma correcta.</t>
   </si>
   <si>
-    <t>TC_002_88_administradorConsultaCuentasFondosInversionCSV</t>
-  </si>
-  <si>
-    <t>TC_002_89_administradorConsultaCreditosHipotecarioTXT</t>
-  </si>
-  <si>
-    <t>TC_002_90_administradorConsultaCuentasInversionCSV</t>
-  </si>
-  <si>
-    <t>TC_002_91_administradorConsultaCuentasTDCMXNTXT</t>
-  </si>
-  <si>
-    <t>TC_002_92_administradorConsultaCuentasChequeUSDCSV</t>
-  </si>
-  <si>
     <t>El usuario da clic en la pestaña "Cuentas Cheque USD"||El sistema muestra la lista de Cuentas Cheque USD.</t>
   </si>
   <si>
@@ -2996,9 +2969,6 @@
   </si>
   <si>
     <t>El usuario da clic en el botón "Descargar".||El sistema permite descargar el reporte de Cuentas Cheque USD de forma correcta en formato CSV .</t>
-  </si>
-  <si>
-    <t>TC_002_93_administradorConsultaCuentasChequeMXNTXT</t>
   </si>
   <si>
     <t>El usuario valida las cuentas de cheques de la pestaña "Cuentas Cheque MXN"||El sistema muestra la lista de Cuentas Cheque MXN.</t>
@@ -3301,13 +3271,6 @@
     <t>El usuario valida que se muestre el link "Ver fondos&gt;" en la sección FONDOS DE INVERSIÓN CONSOLIDADOS.||El sistema muestra de forma correcta el link "Ver fondos&gt;".</t>
   </si>
   <si>
-    <t>El usuario valida que se muestre el campo "Saldo total".|El sistema muestra el campo "Saldo total" de forma correcta con formato de moneda:
--Signo $
--Separación de miles y millones con separador de coma (,)
--Signo de punto para decimales (.)
--2 decim</t>
-  </si>
-  <si>
     <t>TC_002_97_administradorConsultaCreditoHipotecarioFM</t>
   </si>
   <si>
@@ -3732,6 +3695,72 @@
   </si>
   <si>
     <t>El usuario valida el monto mostrado en el campo "Saldo bloqueado".||El sistema debe mostrar el mismo monto que la suma de las cuentas de la columna "Saldo bloqueado".</t>
+  </si>
+  <si>
+    <t>SC_002_63_administradorConsultaCuentasCreditosPrestamosPersonalesPDF</t>
+  </si>
+  <si>
+    <t>SC_002_62_administradorConsultaCuentasLineaOperativaPDF</t>
+  </si>
+  <si>
+    <t>Paso43</t>
+  </si>
+  <si>
+    <t>Paso44</t>
+  </si>
+  <si>
+    <t>Paso45</t>
+  </si>
+  <si>
+    <t>Paso46</t>
+  </si>
+  <si>
+    <t>Paso47</t>
+  </si>
+  <si>
+    <t>Paso48</t>
+  </si>
+  <si>
+    <t>Paso49</t>
+  </si>
+  <si>
+    <t>Paso50</t>
+  </si>
+  <si>
+    <t>Paso51</t>
+  </si>
+  <si>
+    <t>Paso52</t>
+  </si>
+  <si>
+    <t>Paso53</t>
+  </si>
+  <si>
+    <t>Paso54</t>
+  </si>
+  <si>
+    <t>SC_002_86_administradorConsultaCuentasLineaOperativaCSV</t>
+  </si>
+  <si>
+    <t>SC_002_87_administradorConsultaCuentasPrestamosPersonalesTXT</t>
+  </si>
+  <si>
+    <t>SC_002_88_administradorConsultaCuentasFondosInversionCSV</t>
+  </si>
+  <si>
+    <t>SC_002_89_administradorConsultaCreditosHipotecariosTXT</t>
+  </si>
+  <si>
+    <t>SC_002_90_administradorConsultaCuentasInversionCSV</t>
+  </si>
+  <si>
+    <t>SC_002_91_administradorConsultaCuentasTDCMXNTXT</t>
+  </si>
+  <si>
+    <t>SC_002_92_administradorConsultaCuentasChequeUSDCSV</t>
+  </si>
+  <si>
+    <t>SC_002_93_administradorConsultaCuentasChequeMXNTXT</t>
   </si>
 </sst>
 </file>
@@ -4540,10 +4569,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:BC159"/>
+  <dimension ref="A1:BD159"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A77" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="D78" sqref="D78"/>
+    <sheetView tabSelected="1" topLeftCell="D98" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="K99" sqref="K99"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4605,7 +4634,7 @@
     <col min="55" max="55" width="51.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4738,8 +4767,44 @@
       <c r="AR1" s="1" t="s">
         <v>317</v>
       </c>
-    </row>
-    <row r="2" spans="1:44" ht="225" x14ac:dyDescent="0.25">
+      <c r="AS1" s="1" t="s">
+        <v>735</v>
+      </c>
+      <c r="AT1" s="1" t="s">
+        <v>736</v>
+      </c>
+      <c r="AU1" s="1" t="s">
+        <v>737</v>
+      </c>
+      <c r="AV1" s="1" t="s">
+        <v>738</v>
+      </c>
+      <c r="AW1" s="1" t="s">
+        <v>739</v>
+      </c>
+      <c r="AX1" s="1" t="s">
+        <v>740</v>
+      </c>
+      <c r="AY1" s="1" t="s">
+        <v>741</v>
+      </c>
+      <c r="AZ1" s="1" t="s">
+        <v>742</v>
+      </c>
+      <c r="BA1" s="1" t="s">
+        <v>743</v>
+      </c>
+      <c r="BB1" s="1" t="s">
+        <v>744</v>
+      </c>
+      <c r="BC1" s="1" t="s">
+        <v>745</v>
+      </c>
+      <c r="BD1" s="1" t="s">
+        <v>746</v>
+      </c>
+    </row>
+    <row r="2" spans="1:56" ht="225" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>12</v>
       </c>
@@ -4802,7 +4867,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="3" spans="1:44" ht="255" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:56" ht="255" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>13</v>
       </c>
@@ -4862,7 +4927,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="4" spans="1:44" ht="390" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:56" ht="390" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>14</v>
       </c>
@@ -4955,7 +5020,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="5" spans="1:44" ht="360" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:56" ht="360" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>15</v>
       </c>
@@ -5033,7 +5098,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="6" spans="1:44" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:56" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>16</v>
       </c>
@@ -5135,7 +5200,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="7" spans="1:44" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:56" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>17</v>
       </c>
@@ -5213,7 +5278,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="8" spans="1:44" ht="195" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:56" ht="195" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>18</v>
       </c>
@@ -5276,7 +5341,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="9" spans="1:44" ht="195" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:56" ht="195" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>19</v>
       </c>
@@ -5339,7 +5404,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="10" spans="1:44" ht="195" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:56" ht="195" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>20</v>
       </c>
@@ -5402,7 +5467,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="11" spans="1:44" ht="195" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:56" ht="195" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>21</v>
       </c>
@@ -5465,7 +5530,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="12" spans="1:44" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:56" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>23</v>
       </c>
@@ -5525,7 +5590,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="13" spans="1:44" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:56" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>22</v>
       </c>
@@ -5594,7 +5659,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="14" spans="1:44" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:56" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>24</v>
       </c>
@@ -5660,7 +5725,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="15" spans="1:44" ht="405" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:56" ht="405" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>25</v>
       </c>
@@ -5726,7 +5791,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="16" spans="1:44" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:56" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>26</v>
       </c>
@@ -9544,7 +9609,7 @@
     </row>
     <row r="63" spans="1:55" ht="150" x14ac:dyDescent="0.25">
       <c r="A63" s="50" t="s">
-        <v>444</v>
+        <v>734</v>
       </c>
       <c r="B63" s="2"/>
       <c r="C63" s="6" t="s">
@@ -9670,7 +9735,7 @@
     </row>
     <row r="64" spans="1:55" ht="164.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="2" t="s">
-        <v>508</v>
+        <v>733</v>
       </c>
       <c r="B64" s="2"/>
       <c r="C64" s="6" t="s">
@@ -9728,64 +9793,64 @@
         <v>443</v>
       </c>
       <c r="U64" s="16" t="s">
+        <v>444</v>
+      </c>
+      <c r="V64" s="16" t="s">
         <v>445</v>
       </c>
-      <c r="V64" s="16" t="s">
+      <c r="W64" s="16" t="s">
         <v>446</v>
       </c>
-      <c r="W64" s="16" t="s">
+      <c r="X64" s="16" t="s">
         <v>447</v>
       </c>
-      <c r="X64" s="16" t="s">
+      <c r="Y64" s="16" t="s">
         <v>448</v>
       </c>
-      <c r="Y64" s="16" t="s">
+      <c r="Z64" s="16" t="s">
         <v>449</v>
       </c>
-      <c r="Z64" s="16" t="s">
+      <c r="AA64" s="16" t="s">
         <v>450</v>
       </c>
-      <c r="AA64" s="16" t="s">
+      <c r="AB64" s="16" t="s">
         <v>451</v>
       </c>
-      <c r="AB64" s="16" t="s">
+      <c r="AC64" s="3" t="s">
         <v>452</v>
       </c>
-      <c r="AC64" s="3" t="s">
+      <c r="AD64" s="3" t="s">
         <v>453</v>
       </c>
-      <c r="AD64" s="3" t="s">
+      <c r="AE64" s="3" t="s">
         <v>454</v>
       </c>
-      <c r="AE64" s="3" t="s">
+      <c r="AF64" s="3" t="s">
         <v>455</v>
       </c>
-      <c r="AF64" s="3" t="s">
+      <c r="AG64" s="3" t="s">
         <v>456</v>
       </c>
-      <c r="AG64" s="3" t="s">
+      <c r="AH64" s="3" t="s">
         <v>457</v>
       </c>
-      <c r="AH64" s="3" t="s">
+      <c r="AI64" s="3" t="s">
         <v>458</v>
       </c>
-      <c r="AI64" s="3" t="s">
+      <c r="AJ64" s="3" t="s">
         <v>459</v>
       </c>
-      <c r="AJ64" s="3" t="s">
+      <c r="AK64" s="3" t="s">
         <v>460</v>
       </c>
-      <c r="AK64" s="3" t="s">
+      <c r="AL64" s="3" t="s">
         <v>461</v>
       </c>
-      <c r="AL64" s="3" t="s">
+      <c r="AM64" s="3" t="s">
         <v>462</v>
       </c>
-      <c r="AM64" s="3" t="s">
+      <c r="AN64" s="3" t="s">
         <v>463</v>
-      </c>
-      <c r="AN64" s="3" t="s">
-        <v>464</v>
       </c>
       <c r="AO64" s="3" t="s">
         <v>423</v>
@@ -9812,10 +9877,10 @@
         <v>429</v>
       </c>
       <c r="AW64" s="3" t="s">
+        <v>464</v>
+      </c>
+      <c r="AX64" s="3" t="s">
         <v>465</v>
-      </c>
-      <c r="AX64" s="3" t="s">
-        <v>466</v>
       </c>
       <c r="AY64" s="3" t="s">
         <v>325</v>
@@ -9824,7 +9889,7 @@
         <v>432</v>
       </c>
       <c r="BA64" s="3" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="BB64" s="3" t="s">
         <v>434</v>
@@ -9835,7 +9900,7 @@
     </row>
     <row r="65" spans="1:42" ht="190.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="2" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="B65" s="2"/>
       <c r="C65" s="6" t="s">
@@ -9872,22 +9937,22 @@
         <v>436</v>
       </c>
       <c r="N65" s="16" t="s">
+        <v>467</v>
+      </c>
+      <c r="O65" s="43" t="s">
         <v>468</v>
       </c>
-      <c r="O65" s="43" t="s">
+      <c r="P65" s="43" t="s">
         <v>469</v>
       </c>
-      <c r="P65" s="43" t="s">
+      <c r="Q65" s="43" t="s">
         <v>470</v>
       </c>
-      <c r="Q65" s="43" t="s">
+      <c r="R65" s="43" t="s">
         <v>471</v>
       </c>
-      <c r="R65" s="43" t="s">
+      <c r="S65" s="43" t="s">
         <v>472</v>
-      </c>
-      <c r="S65" s="43" t="s">
-        <v>473</v>
       </c>
       <c r="T65" s="43" t="s">
         <v>423</v>
@@ -9905,22 +9970,22 @@
         <v>426</v>
       </c>
       <c r="Y65" s="43" t="s">
+        <v>473</v>
+      </c>
+      <c r="Z65" s="43" t="s">
         <v>474</v>
       </c>
-      <c r="Z65" s="43" t="s">
+      <c r="AA65" s="43" t="s">
         <v>475</v>
       </c>
-      <c r="AA65" s="43" t="s">
+      <c r="AB65" s="43" t="s">
         <v>476</v>
       </c>
-      <c r="AB65" s="43" t="s">
+      <c r="AC65" s="2" t="s">
         <v>477</v>
       </c>
-      <c r="AC65" s="2" t="s">
+      <c r="AD65" s="2" t="s">
         <v>478</v>
-      </c>
-      <c r="AD65" s="2" t="s">
-        <v>479</v>
       </c>
       <c r="AE65" s="3" t="s">
         <v>325</v>
@@ -9929,7 +9994,7 @@
         <v>432</v>
       </c>
       <c r="AG65" s="2" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="AH65" s="2" t="s">
         <v>434</v>
@@ -9947,7 +10012,7 @@
     </row>
     <row r="66" spans="1:42" ht="190.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="51" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="B66" s="2"/>
       <c r="C66" s="6" t="s">
@@ -9981,34 +10046,34 @@
         <v>442</v>
       </c>
       <c r="M66" s="43" t="s">
+        <v>481</v>
+      </c>
+      <c r="N66" s="43" t="s">
         <v>482</v>
       </c>
-      <c r="N66" s="43" t="s">
+      <c r="O66" s="43" t="s">
         <v>483</v>
       </c>
-      <c r="O66" s="43" t="s">
+      <c r="P66" s="43" t="s">
         <v>484</v>
       </c>
-      <c r="P66" s="43" t="s">
+      <c r="Q66" s="43" t="s">
         <v>485</v>
       </c>
-      <c r="Q66" s="43" t="s">
+      <c r="R66" s="43" t="s">
         <v>486</v>
       </c>
-      <c r="R66" s="43" t="s">
+      <c r="S66" s="16" t="s">
         <v>487</v>
       </c>
-      <c r="S66" s="16" t="s">
+      <c r="T66" s="43" t="s">
         <v>488</v>
       </c>
-      <c r="T66" s="43" t="s">
+      <c r="U66" s="43" t="s">
         <v>489</v>
       </c>
-      <c r="U66" s="43" t="s">
-        <v>490</v>
-      </c>
       <c r="V66" s="16" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="W66" s="16" t="s">
         <v>423</v>
@@ -10029,16 +10094,16 @@
         <v>427</v>
       </c>
       <c r="AC66" s="2" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="AD66" s="2" t="s">
         <v>428</v>
       </c>
       <c r="AE66" s="2" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="AF66" s="2" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="AG66" s="2" t="s">
         <v>325</v>
@@ -10047,7 +10112,7 @@
         <v>432</v>
       </c>
       <c r="AI66" s="2" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="AJ66" s="2" t="s">
         <v>434</v>
@@ -10063,7 +10128,7 @@
     </row>
     <row r="67" spans="1:42" ht="197.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="51" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="B67" s="2"/>
       <c r="C67" s="6" t="s">
@@ -10094,13 +10159,13 @@
         <v>357</v>
       </c>
       <c r="L67" s="2" t="s">
+        <v>494</v>
+      </c>
+      <c r="M67" s="43" t="s">
         <v>495</v>
       </c>
-      <c r="M67" s="43" t="s">
+      <c r="N67" s="43" t="s">
         <v>496</v>
-      </c>
-      <c r="N67" s="43" t="s">
-        <v>497</v>
       </c>
       <c r="O67" s="43" t="s">
         <v>407</v>
@@ -10109,31 +10174,31 @@
         <v>408</v>
       </c>
       <c r="Q67" s="43" t="s">
+        <v>497</v>
+      </c>
+      <c r="R67" s="43" t="s">
         <v>498</v>
       </c>
-      <c r="R67" s="43" t="s">
+      <c r="S67" s="16" t="s">
         <v>499</v>
       </c>
-      <c r="S67" s="16" t="s">
+      <c r="T67" s="43" t="s">
         <v>500</v>
       </c>
-      <c r="T67" s="43" t="s">
+      <c r="U67" s="43" t="s">
         <v>501</v>
       </c>
-      <c r="U67" s="43" t="s">
+      <c r="V67" s="43" t="s">
         <v>502</v>
       </c>
-      <c r="V67" s="43" t="s">
+      <c r="W67" s="43" t="s">
         <v>503</v>
       </c>
-      <c r="W67" s="43" t="s">
+      <c r="X67" s="43" t="s">
         <v>504</v>
       </c>
-      <c r="X67" s="43" t="s">
+      <c r="Y67" s="16" t="s">
         <v>505</v>
-      </c>
-      <c r="Y67" s="16" t="s">
-        <v>506</v>
       </c>
       <c r="Z67" s="43" t="s">
         <v>325</v>
@@ -10142,7 +10207,7 @@
         <v>432</v>
       </c>
       <c r="AB67" s="43" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="AC67" s="2" t="s">
         <v>434</v>
@@ -10165,7 +10230,7 @@
     </row>
     <row r="68" spans="1:42" ht="195" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="2" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
       <c r="B68" s="2"/>
       <c r="C68" s="6" t="s">
@@ -10193,49 +10258,49 @@
         <v>403</v>
       </c>
       <c r="K68" s="2" t="s">
+        <v>509</v>
+      </c>
+      <c r="L68" s="2" t="s">
+        <v>510</v>
+      </c>
+      <c r="M68" s="16" t="s">
         <v>511</v>
       </c>
-      <c r="L68" s="2" t="s">
+      <c r="N68" s="43" t="s">
         <v>512</v>
       </c>
-      <c r="M68" s="16" t="s">
+      <c r="O68" s="43" t="s">
         <v>513</v>
       </c>
-      <c r="N68" s="43" t="s">
+      <c r="P68" s="43" t="s">
         <v>514</v>
       </c>
-      <c r="O68" s="43" t="s">
+      <c r="Q68" s="43" t="s">
         <v>515</v>
       </c>
-      <c r="P68" s="43" t="s">
+      <c r="R68" s="43" t="s">
         <v>516</v>
       </c>
-      <c r="Q68" s="43" t="s">
+      <c r="S68" s="43" t="s">
         <v>517</v>
       </c>
-      <c r="R68" s="43" t="s">
+      <c r="T68" s="43" t="s">
         <v>518</v>
       </c>
-      <c r="S68" s="43" t="s">
+      <c r="U68" s="43" t="s">
         <v>519</v>
       </c>
-      <c r="T68" s="43" t="s">
+      <c r="V68" s="43" t="s">
         <v>520</v>
       </c>
-      <c r="U68" s="43" t="s">
+      <c r="W68" s="43" t="s">
         <v>521</v>
       </c>
-      <c r="V68" s="43" t="s">
+      <c r="X68" s="43" t="s">
         <v>522</v>
       </c>
-      <c r="W68" s="43" t="s">
+      <c r="Y68" s="16" t="s">
         <v>523</v>
-      </c>
-      <c r="X68" s="43" t="s">
-        <v>524</v>
-      </c>
-      <c r="Y68" s="16" t="s">
-        <v>525</v>
       </c>
       <c r="Z68" s="43" t="s">
         <v>325</v>
@@ -10247,25 +10312,25 @@
         <v>425</v>
       </c>
       <c r="AC68" s="3" t="s">
+        <v>523</v>
+      </c>
+      <c r="AD68" s="3" t="s">
+        <v>473</v>
+      </c>
+      <c r="AE68" s="2" t="s">
+        <v>524</v>
+      </c>
+      <c r="AF68" s="3" t="s">
         <v>525</v>
       </c>
-      <c r="AD68" s="3" t="s">
-        <v>474</v>
-      </c>
-      <c r="AE68" s="2" t="s">
+      <c r="AG68" s="3" t="s">
         <v>526</v>
       </c>
-      <c r="AF68" s="3" t="s">
+      <c r="AH68" s="2" t="s">
+        <v>476</v>
+      </c>
+      <c r="AI68" s="3" t="s">
         <v>527</v>
-      </c>
-      <c r="AG68" s="3" t="s">
-        <v>528</v>
-      </c>
-      <c r="AH68" s="2" t="s">
-        <v>477</v>
-      </c>
-      <c r="AI68" s="3" t="s">
-        <v>529</v>
       </c>
       <c r="AJ68" s="2" t="s">
         <v>325</v>
@@ -10274,7 +10339,7 @@
         <v>432</v>
       </c>
       <c r="AL68" s="2" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="AM68" s="2" t="s">
         <v>434</v>
@@ -10287,7 +10352,7 @@
     </row>
     <row r="69" spans="1:42" ht="200.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" s="51" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
       <c r="B69" s="2"/>
       <c r="C69" s="6" t="s">
@@ -10318,31 +10383,31 @@
         <v>365</v>
       </c>
       <c r="L69" s="2" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
       <c r="M69" s="43" t="s">
         <v>436</v>
       </c>
       <c r="N69" s="43" t="s">
+        <v>531</v>
+      </c>
+      <c r="O69" s="43" t="s">
+        <v>532</v>
+      </c>
+      <c r="P69" s="43" t="s">
         <v>533</v>
       </c>
-      <c r="O69" s="43" t="s">
+      <c r="Q69" s="43" t="s">
         <v>534</v>
       </c>
-      <c r="P69" s="43" t="s">
+      <c r="R69" s="43" t="s">
         <v>535</v>
       </c>
-      <c r="Q69" s="43" t="s">
+      <c r="S69" s="43" t="s">
         <v>536</v>
       </c>
-      <c r="R69" s="43" t="s">
+      <c r="T69" s="43" t="s">
         <v>537</v>
-      </c>
-      <c r="S69" s="43" t="s">
-        <v>538</v>
-      </c>
-      <c r="T69" s="43" t="s">
-        <v>539</v>
       </c>
       <c r="U69" s="43" t="s">
         <v>423</v>
@@ -10363,19 +10428,19 @@
         <v>427</v>
       </c>
       <c r="AA69" s="43" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="AB69" s="43" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
       <c r="AC69" s="2" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="AD69" s="3" t="s">
-        <v>541</v>
+        <v>539</v>
       </c>
       <c r="AE69" s="2" t="s">
-        <v>529</v>
+        <v>527</v>
       </c>
       <c r="AF69" s="3" t="s">
         <v>325</v>
@@ -10384,7 +10449,7 @@
         <v>432</v>
       </c>
       <c r="AH69" s="2" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="AI69" s="3" t="s">
         <v>434</v>
@@ -10401,7 +10466,7 @@
     </row>
     <row r="70" spans="1:42" ht="203.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" s="51" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="B70" s="2"/>
       <c r="C70" s="6" t="s">
@@ -10432,31 +10497,31 @@
         <v>371</v>
       </c>
       <c r="L70" s="2" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
       <c r="M70" s="43" t="s">
         <v>436</v>
       </c>
       <c r="N70" s="43" t="s">
+        <v>531</v>
+      </c>
+      <c r="O70" s="43" t="s">
+        <v>532</v>
+      </c>
+      <c r="P70" s="43" t="s">
         <v>533</v>
       </c>
-      <c r="O70" s="43" t="s">
+      <c r="Q70" s="43" t="s">
         <v>534</v>
       </c>
-      <c r="P70" s="43" t="s">
+      <c r="R70" s="43" t="s">
         <v>535</v>
       </c>
-      <c r="Q70" s="43" t="s">
+      <c r="S70" s="43" t="s">
         <v>536</v>
       </c>
-      <c r="R70" s="43" t="s">
+      <c r="T70" s="43" t="s">
         <v>537</v>
-      </c>
-      <c r="S70" s="43" t="s">
-        <v>538</v>
-      </c>
-      <c r="T70" s="43" t="s">
-        <v>539</v>
       </c>
       <c r="U70" s="43" t="s">
         <v>423</v>
@@ -10471,25 +10536,25 @@
         <v>425</v>
       </c>
       <c r="Y70" s="43" t="s">
-        <v>525</v>
+        <v>523</v>
       </c>
       <c r="Z70" s="43" t="s">
         <v>427</v>
       </c>
       <c r="AA70" s="43" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="AB70" s="43" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
       <c r="AC70" s="2" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="AD70" s="3" t="s">
-        <v>541</v>
+        <v>539</v>
       </c>
       <c r="AE70" s="2" t="s">
-        <v>529</v>
+        <v>527</v>
       </c>
       <c r="AF70" s="3" t="s">
         <v>325</v>
@@ -10498,7 +10563,7 @@
         <v>432</v>
       </c>
       <c r="AH70" s="2" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="AI70" s="3" t="s">
         <v>434</v>
@@ -10515,7 +10580,7 @@
     </row>
     <row r="71" spans="1:42" ht="205.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" s="51" t="s">
-        <v>544</v>
+        <v>542</v>
       </c>
       <c r="B71" s="2"/>
       <c r="C71" s="6" t="s">
@@ -10534,46 +10599,46 @@
         <v>36</v>
       </c>
       <c r="H71" s="2" t="s">
-        <v>545</v>
+        <v>543</v>
       </c>
       <c r="I71" s="2" t="s">
         <v>321</v>
       </c>
       <c r="J71" s="2" t="s">
+        <v>544</v>
+      </c>
+      <c r="K71" s="2" t="s">
+        <v>522</v>
+      </c>
+      <c r="L71" s="2" t="s">
+        <v>545</v>
+      </c>
+      <c r="M71" s="16" t="s">
         <v>546</v>
       </c>
-      <c r="K71" s="2" t="s">
-        <v>524</v>
-      </c>
-      <c r="L71" s="2" t="s">
+      <c r="N71" s="43" t="s">
         <v>547</v>
       </c>
-      <c r="M71" s="16" t="s">
+      <c r="O71" s="16" t="s">
         <v>548</v>
       </c>
-      <c r="N71" s="43" t="s">
+      <c r="P71" s="43" t="s">
         <v>549</v>
       </c>
-      <c r="O71" s="16" t="s">
+      <c r="Q71" s="43" t="s">
         <v>550</v>
       </c>
-      <c r="P71" s="43" t="s">
+      <c r="R71" s="43" t="s">
         <v>551</v>
       </c>
-      <c r="Q71" s="43" t="s">
+      <c r="S71" s="43" t="s">
         <v>552</v>
       </c>
-      <c r="R71" s="43" t="s">
+      <c r="T71" s="16" t="s">
         <v>553</v>
       </c>
-      <c r="S71" s="43" t="s">
+      <c r="U71" s="43" t="s">
         <v>554</v>
-      </c>
-      <c r="T71" s="16" t="s">
-        <v>555</v>
-      </c>
-      <c r="U71" s="43" t="s">
-        <v>556</v>
       </c>
       <c r="V71" s="16"/>
       <c r="W71" s="16"/>
@@ -10599,7 +10664,7 @@
     </row>
     <row r="72" spans="1:42" ht="149.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" s="2" t="s">
-        <v>681</v>
+        <v>670</v>
       </c>
       <c r="B72" s="2"/>
       <c r="C72" s="2" t="s">
@@ -10618,46 +10683,46 @@
         <v>36</v>
       </c>
       <c r="H72" s="2" t="s">
+        <v>658</v>
+      </c>
+      <c r="I72" s="2" t="s">
+        <v>569</v>
+      </c>
+      <c r="J72" s="2" t="s">
+        <v>659</v>
+      </c>
+      <c r="K72" s="2" t="s">
+        <v>575</v>
+      </c>
+      <c r="L72" s="2" t="s">
+        <v>660</v>
+      </c>
+      <c r="M72" s="16" t="s">
+        <v>661</v>
+      </c>
+      <c r="N72" s="16" t="s">
+        <v>662</v>
+      </c>
+      <c r="O72" s="16" t="s">
+        <v>663</v>
+      </c>
+      <c r="P72" s="16" t="s">
+        <v>664</v>
+      </c>
+      <c r="Q72" s="16" t="s">
+        <v>665</v>
+      </c>
+      <c r="R72" s="16" t="s">
+        <v>666</v>
+      </c>
+      <c r="S72" s="16" t="s">
+        <v>667</v>
+      </c>
+      <c r="T72" s="16" t="s">
+        <v>668</v>
+      </c>
+      <c r="U72" s="16" t="s">
         <v>669</v>
-      </c>
-      <c r="I72" s="2" t="s">
-        <v>579</v>
-      </c>
-      <c r="J72" s="2" t="s">
-        <v>670</v>
-      </c>
-      <c r="K72" s="2" t="s">
-        <v>585</v>
-      </c>
-      <c r="L72" s="2" t="s">
-        <v>671</v>
-      </c>
-      <c r="M72" s="16" t="s">
-        <v>672</v>
-      </c>
-      <c r="N72" s="16" t="s">
-        <v>673</v>
-      </c>
-      <c r="O72" s="16" t="s">
-        <v>674</v>
-      </c>
-      <c r="P72" s="16" t="s">
-        <v>675</v>
-      </c>
-      <c r="Q72" s="16" t="s">
-        <v>676</v>
-      </c>
-      <c r="R72" s="16" t="s">
-        <v>677</v>
-      </c>
-      <c r="S72" s="16" t="s">
-        <v>678</v>
-      </c>
-      <c r="T72" s="16" t="s">
-        <v>679</v>
-      </c>
-      <c r="U72" s="16" t="s">
-        <v>680</v>
       </c>
       <c r="V72" s="16"/>
       <c r="W72" s="16"/>
@@ -10683,7 +10748,7 @@
     </row>
     <row r="73" spans="1:42" ht="135" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" s="2" t="s">
-        <v>682</v>
+        <v>671</v>
       </c>
       <c r="B73" s="2"/>
       <c r="C73" s="2" t="s">
@@ -10702,28 +10767,28 @@
         <v>36</v>
       </c>
       <c r="H73" s="2" t="s">
-        <v>683</v>
+        <v>672</v>
       </c>
       <c r="I73" s="2" t="s">
-        <v>579</v>
+        <v>569</v>
       </c>
       <c r="J73" s="2" t="s">
-        <v>684</v>
+        <v>673</v>
       </c>
       <c r="K73" s="2" t="s">
-        <v>585</v>
+        <v>575</v>
       </c>
       <c r="L73" s="2" t="s">
-        <v>685</v>
+        <v>674</v>
       </c>
       <c r="M73" s="16" t="s">
-        <v>686</v>
+        <v>675</v>
       </c>
       <c r="N73" s="43" t="s">
-        <v>687</v>
+        <v>676</v>
       </c>
       <c r="O73" s="16" t="s">
-        <v>674</v>
+        <v>663</v>
       </c>
       <c r="P73" s="16"/>
       <c r="Q73" s="16"/>
@@ -10755,7 +10820,7 @@
     </row>
     <row r="74" spans="1:42" ht="155.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" s="2" t="s">
-        <v>688</v>
+        <v>677</v>
       </c>
       <c r="B74" s="2"/>
       <c r="C74" s="2" t="s">
@@ -10774,46 +10839,46 @@
         <v>36</v>
       </c>
       <c r="H74" s="2" t="s">
+        <v>678</v>
+      </c>
+      <c r="I74" s="2" t="s">
+        <v>569</v>
+      </c>
+      <c r="J74" s="2" t="s">
+        <v>679</v>
+      </c>
+      <c r="K74" s="2" t="s">
+        <v>575</v>
+      </c>
+      <c r="L74" s="2" t="s">
+        <v>680</v>
+      </c>
+      <c r="M74" s="53" t="s">
+        <v>681</v>
+      </c>
+      <c r="N74" s="2" t="s">
+        <v>682</v>
+      </c>
+      <c r="O74" s="53" t="s">
+        <v>683</v>
+      </c>
+      <c r="P74" s="54" t="s">
+        <v>684</v>
+      </c>
+      <c r="Q74" s="54" t="s">
+        <v>685</v>
+      </c>
+      <c r="R74" s="54" t="s">
+        <v>686</v>
+      </c>
+      <c r="S74" s="54" t="s">
+        <v>687</v>
+      </c>
+      <c r="T74" s="53" t="s">
+        <v>688</v>
+      </c>
+      <c r="U74" s="54" t="s">
         <v>689</v>
-      </c>
-      <c r="I74" s="2" t="s">
-        <v>579</v>
-      </c>
-      <c r="J74" s="2" t="s">
-        <v>690</v>
-      </c>
-      <c r="K74" s="2" t="s">
-        <v>585</v>
-      </c>
-      <c r="L74" s="2" t="s">
-        <v>691</v>
-      </c>
-      <c r="M74" s="53" t="s">
-        <v>692</v>
-      </c>
-      <c r="N74" s="2" t="s">
-        <v>693</v>
-      </c>
-      <c r="O74" s="53" t="s">
-        <v>694</v>
-      </c>
-      <c r="P74" s="54" t="s">
-        <v>695</v>
-      </c>
-      <c r="Q74" s="54" t="s">
-        <v>696</v>
-      </c>
-      <c r="R74" s="54" t="s">
-        <v>697</v>
-      </c>
-      <c r="S74" s="54" t="s">
-        <v>698</v>
-      </c>
-      <c r="T74" s="53" t="s">
-        <v>699</v>
-      </c>
-      <c r="U74" s="54" t="s">
-        <v>700</v>
       </c>
       <c r="AC74" s="5"/>
       <c r="AD74" s="3"/>
@@ -10832,7 +10897,7 @@
     </row>
     <row r="75" spans="1:42" ht="152.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" s="2" t="s">
-        <v>701</v>
+        <v>690</v>
       </c>
       <c r="B75" s="2"/>
       <c r="C75" s="2" t="s">
@@ -10851,28 +10916,28 @@
         <v>36</v>
       </c>
       <c r="H75" s="2" t="s">
-        <v>702</v>
+        <v>691</v>
       </c>
       <c r="I75" s="2" t="s">
-        <v>579</v>
+        <v>569</v>
       </c>
       <c r="J75" s="2" t="s">
-        <v>703</v>
+        <v>692</v>
       </c>
       <c r="K75" s="2" t="s">
-        <v>585</v>
+        <v>575</v>
       </c>
       <c r="L75" s="2" t="s">
-        <v>704</v>
+        <v>693</v>
       </c>
       <c r="M75" s="53" t="s">
-        <v>705</v>
+        <v>694</v>
       </c>
       <c r="N75" s="2" t="s">
-        <v>706</v>
+        <v>695</v>
       </c>
       <c r="O75" s="53" t="s">
-        <v>707</v>
+        <v>696</v>
       </c>
       <c r="AC75" s="5"/>
       <c r="AD75" s="3"/>
@@ -10891,7 +10956,7 @@
     </row>
     <row r="76" spans="1:42" ht="153" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" s="2" t="s">
-        <v>708</v>
+        <v>697</v>
       </c>
       <c r="B76" s="2"/>
       <c r="C76" s="2" t="s">
@@ -10910,46 +10975,46 @@
         <v>36</v>
       </c>
       <c r="H76" s="2" t="s">
+        <v>698</v>
+      </c>
+      <c r="I76" s="2" t="s">
+        <v>569</v>
+      </c>
+      <c r="J76" s="2" t="s">
+        <v>699</v>
+      </c>
+      <c r="K76" s="2" t="s">
+        <v>575</v>
+      </c>
+      <c r="L76" s="2" t="s">
+        <v>700</v>
+      </c>
+      <c r="M76" s="53" t="s">
+        <v>701</v>
+      </c>
+      <c r="N76" s="2" t="s">
+        <v>702</v>
+      </c>
+      <c r="O76" s="53" t="s">
+        <v>703</v>
+      </c>
+      <c r="P76" s="55" t="s">
+        <v>704</v>
+      </c>
+      <c r="Q76" s="56" t="s">
+        <v>705</v>
+      </c>
+      <c r="R76" s="55" t="s">
+        <v>706</v>
+      </c>
+      <c r="S76" s="56" t="s">
+        <v>707</v>
+      </c>
+      <c r="T76" s="56" t="s">
+        <v>708</v>
+      </c>
+      <c r="U76" s="56" t="s">
         <v>709</v>
-      </c>
-      <c r="I76" s="2" t="s">
-        <v>579</v>
-      </c>
-      <c r="J76" s="2" t="s">
-        <v>710</v>
-      </c>
-      <c r="K76" s="2" t="s">
-        <v>585</v>
-      </c>
-      <c r="L76" s="2" t="s">
-        <v>711</v>
-      </c>
-      <c r="M76" s="53" t="s">
-        <v>712</v>
-      </c>
-      <c r="N76" s="2" t="s">
-        <v>713</v>
-      </c>
-      <c r="O76" s="53" t="s">
-        <v>714</v>
-      </c>
-      <c r="P76" s="55" t="s">
-        <v>715</v>
-      </c>
-      <c r="Q76" s="56" t="s">
-        <v>716</v>
-      </c>
-      <c r="R76" s="55" t="s">
-        <v>717</v>
-      </c>
-      <c r="S76" s="56" t="s">
-        <v>718</v>
-      </c>
-      <c r="T76" s="56" t="s">
-        <v>719</v>
-      </c>
-      <c r="U76" s="56" t="s">
-        <v>720</v>
       </c>
       <c r="AC76" s="5"/>
       <c r="AD76" s="3"/>
@@ -10968,7 +11033,7 @@
     </row>
     <row r="77" spans="1:42" ht="164.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77" s="2" t="s">
-        <v>721</v>
+        <v>710</v>
       </c>
       <c r="B77" s="2"/>
       <c r="C77" s="2" t="s">
@@ -10987,55 +11052,55 @@
         <v>36</v>
       </c>
       <c r="H77" s="2" t="s">
-        <v>722</v>
+        <v>711</v>
       </c>
       <c r="I77" s="2" t="s">
-        <v>579</v>
+        <v>569</v>
       </c>
       <c r="J77" s="2" t="s">
-        <v>723</v>
+        <v>712</v>
       </c>
       <c r="K77" s="2" t="s">
-        <v>585</v>
+        <v>575</v>
       </c>
       <c r="L77" s="2" t="s">
-        <v>724</v>
+        <v>713</v>
       </c>
       <c r="M77" s="53" t="s">
-        <v>725</v>
+        <v>714</v>
       </c>
       <c r="N77" s="2" t="s">
-        <v>687</v>
+        <v>676</v>
       </c>
       <c r="O77" s="53" t="s">
-        <v>674</v>
+        <v>663</v>
       </c>
       <c r="P77" s="55" t="s">
-        <v>726</v>
+        <v>715</v>
       </c>
       <c r="Q77" s="56" t="s">
-        <v>713</v>
+        <v>702</v>
       </c>
       <c r="R77" s="55" t="s">
-        <v>714</v>
+        <v>703</v>
       </c>
       <c r="S77" s="56" t="s">
-        <v>727</v>
+        <v>716</v>
       </c>
       <c r="T77" s="56" t="s">
-        <v>728</v>
+        <v>717</v>
       </c>
       <c r="U77" s="56" t="s">
-        <v>729</v>
+        <v>718</v>
       </c>
       <c r="V77" s="2" t="s">
-        <v>730</v>
+        <v>719</v>
       </c>
       <c r="W77" s="2" t="s">
-        <v>731</v>
+        <v>720</v>
       </c>
       <c r="X77" s="56" t="s">
-        <v>732</v>
+        <v>721</v>
       </c>
       <c r="AC77" s="5"/>
       <c r="AD77" s="3"/>
@@ -11054,7 +11119,7 @@
     </row>
     <row r="78" spans="1:42" ht="150.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78" s="2" t="s">
-        <v>733</v>
+        <v>722</v>
       </c>
       <c r="B78" s="2"/>
       <c r="C78" s="2" t="s">
@@ -11073,55 +11138,55 @@
         <v>36</v>
       </c>
       <c r="H78" s="2" t="s">
-        <v>734</v>
+        <v>723</v>
       </c>
       <c r="I78" s="2" t="s">
-        <v>579</v>
+        <v>569</v>
       </c>
       <c r="J78" s="2" t="s">
-        <v>735</v>
+        <v>724</v>
       </c>
       <c r="K78" s="2" t="s">
-        <v>585</v>
+        <v>575</v>
       </c>
       <c r="L78" s="2" t="s">
-        <v>736</v>
+        <v>725</v>
       </c>
       <c r="M78" s="53" t="s">
-        <v>737</v>
+        <v>726</v>
       </c>
       <c r="N78" s="2" t="s">
-        <v>687</v>
+        <v>676</v>
       </c>
       <c r="O78" s="53" t="s">
-        <v>674</v>
+        <v>663</v>
       </c>
       <c r="P78" s="55" t="s">
-        <v>738</v>
+        <v>727</v>
       </c>
       <c r="Q78" s="56" t="s">
-        <v>739</v>
+        <v>728</v>
       </c>
       <c r="R78" s="55" t="s">
-        <v>714</v>
+        <v>703</v>
       </c>
       <c r="S78" s="56" t="s">
-        <v>740</v>
+        <v>729</v>
       </c>
       <c r="T78" s="2" t="s">
-        <v>728</v>
+        <v>717</v>
       </c>
       <c r="U78" s="56" t="s">
-        <v>729</v>
+        <v>718</v>
       </c>
       <c r="V78" s="2" t="s">
-        <v>741</v>
+        <v>730</v>
       </c>
       <c r="W78" s="56" t="s">
-        <v>742</v>
+        <v>731</v>
       </c>
       <c r="X78" s="2" t="s">
-        <v>743</v>
+        <v>732</v>
       </c>
       <c r="AC78" s="5"/>
       <c r="AD78" s="3"/>
@@ -11140,50 +11205,50 @@
     </row>
     <row r="79" spans="1:42" ht="150" x14ac:dyDescent="0.25">
       <c r="A79" s="2" t="s">
-        <v>574</v>
+        <v>564</v>
       </c>
       <c r="B79" s="2"/>
       <c r="C79" s="2" t="s">
         <v>32</v>
       </c>
       <c r="D79" s="2" t="s">
+        <v>565</v>
+      </c>
+      <c r="E79" s="2" t="s">
+        <v>566</v>
+      </c>
+      <c r="F79" s="2" t="s">
+        <v>567</v>
+      </c>
+      <c r="G79" s="2" t="s">
+        <v>568</v>
+      </c>
+      <c r="H79" s="2" t="s">
+        <v>569</v>
+      </c>
+      <c r="I79" s="2" t="s">
+        <v>570</v>
+      </c>
+      <c r="J79" s="2" t="s">
+        <v>571</v>
+      </c>
+      <c r="K79" s="2" t="s">
+        <v>572</v>
+      </c>
+      <c r="L79" s="2" t="s">
+        <v>573</v>
+      </c>
+      <c r="M79" s="2" t="s">
+        <v>574</v>
+      </c>
+      <c r="N79" s="2" t="s">
+        <v>521</v>
+      </c>
+      <c r="O79" s="2" t="s">
         <v>575</v>
       </c>
-      <c r="E79" s="2" t="s">
+      <c r="P79" s="2" t="s">
         <v>576</v>
-      </c>
-      <c r="F79" s="2" t="s">
-        <v>577</v>
-      </c>
-      <c r="G79" s="2" t="s">
-        <v>578</v>
-      </c>
-      <c r="H79" s="2" t="s">
-        <v>579</v>
-      </c>
-      <c r="I79" s="2" t="s">
-        <v>580</v>
-      </c>
-      <c r="J79" s="2" t="s">
-        <v>581</v>
-      </c>
-      <c r="K79" s="2" t="s">
-        <v>582</v>
-      </c>
-      <c r="L79" s="2" t="s">
-        <v>583</v>
-      </c>
-      <c r="M79" s="2" t="s">
-        <v>584</v>
-      </c>
-      <c r="N79" s="2" t="s">
-        <v>523</v>
-      </c>
-      <c r="O79" s="2" t="s">
-        <v>585</v>
-      </c>
-      <c r="P79" s="2" t="s">
-        <v>586</v>
       </c>
       <c r="AC79" s="5"/>
       <c r="AD79" s="3"/>
@@ -11202,50 +11267,50 @@
     </row>
     <row r="80" spans="1:42" ht="150" x14ac:dyDescent="0.25">
       <c r="A80" s="2" t="s">
-        <v>587</v>
+        <v>577</v>
       </c>
       <c r="B80" s="2"/>
       <c r="C80" s="2" t="s">
         <v>32</v>
       </c>
       <c r="D80" s="2" t="s">
+        <v>565</v>
+      </c>
+      <c r="E80" s="2" t="s">
+        <v>566</v>
+      </c>
+      <c r="F80" s="2" t="s">
+        <v>567</v>
+      </c>
+      <c r="G80" s="2" t="s">
+        <v>568</v>
+      </c>
+      <c r="H80" s="2" t="s">
+        <v>569</v>
+      </c>
+      <c r="I80" s="2" t="s">
+        <v>578</v>
+      </c>
+      <c r="J80" s="2" t="s">
+        <v>571</v>
+      </c>
+      <c r="K80" s="2" t="s">
+        <v>572</v>
+      </c>
+      <c r="L80" s="2" t="s">
+        <v>579</v>
+      </c>
+      <c r="M80" s="2" t="s">
+        <v>580</v>
+      </c>
+      <c r="N80" s="2" t="s">
+        <v>521</v>
+      </c>
+      <c r="O80" s="2" t="s">
         <v>575</v>
       </c>
-      <c r="E80" s="2" t="s">
+      <c r="P80" s="4" t="s">
         <v>576</v>
-      </c>
-      <c r="F80" s="2" t="s">
-        <v>577</v>
-      </c>
-      <c r="G80" s="2" t="s">
-        <v>578</v>
-      </c>
-      <c r="H80" s="2" t="s">
-        <v>579</v>
-      </c>
-      <c r="I80" s="2" t="s">
-        <v>588</v>
-      </c>
-      <c r="J80" s="2" t="s">
-        <v>581</v>
-      </c>
-      <c r="K80" s="2" t="s">
-        <v>582</v>
-      </c>
-      <c r="L80" s="2" t="s">
-        <v>589</v>
-      </c>
-      <c r="M80" s="2" t="s">
-        <v>590</v>
-      </c>
-      <c r="N80" s="2" t="s">
-        <v>523</v>
-      </c>
-      <c r="O80" s="2" t="s">
-        <v>585</v>
-      </c>
-      <c r="P80" s="4" t="s">
-        <v>586</v>
       </c>
       <c r="AC80" s="5"/>
       <c r="AD80" s="3"/>
@@ -11264,44 +11329,44 @@
     </row>
     <row r="81" spans="1:42" ht="135" x14ac:dyDescent="0.25">
       <c r="A81" s="2" t="s">
-        <v>591</v>
+        <v>581</v>
       </c>
       <c r="B81" s="2"/>
       <c r="C81" s="2" t="s">
         <v>32</v>
       </c>
       <c r="D81" s="2" t="s">
+        <v>565</v>
+      </c>
+      <c r="E81" s="2" t="s">
+        <v>566</v>
+      </c>
+      <c r="F81" s="2" t="s">
+        <v>567</v>
+      </c>
+      <c r="G81" s="2" t="s">
+        <v>568</v>
+      </c>
+      <c r="H81" s="2" t="s">
+        <v>569</v>
+      </c>
+      <c r="I81" s="2" t="s">
+        <v>582</v>
+      </c>
+      <c r="J81" s="2" t="s">
+        <v>583</v>
+      </c>
+      <c r="K81" s="2" t="s">
+        <v>584</v>
+      </c>
+      <c r="L81" s="2" t="s">
+        <v>521</v>
+      </c>
+      <c r="M81" s="2" t="s">
         <v>575</v>
       </c>
-      <c r="E81" s="2" t="s">
+      <c r="N81" s="2" t="s">
         <v>576</v>
-      </c>
-      <c r="F81" s="2" t="s">
-        <v>577</v>
-      </c>
-      <c r="G81" s="2" t="s">
-        <v>578</v>
-      </c>
-      <c r="H81" s="2" t="s">
-        <v>579</v>
-      </c>
-      <c r="I81" s="2" t="s">
-        <v>592</v>
-      </c>
-      <c r="J81" s="2" t="s">
-        <v>593</v>
-      </c>
-      <c r="K81" s="2" t="s">
-        <v>594</v>
-      </c>
-      <c r="L81" s="2" t="s">
-        <v>523</v>
-      </c>
-      <c r="M81" s="2" t="s">
-        <v>585</v>
-      </c>
-      <c r="N81" s="2" t="s">
-        <v>586</v>
       </c>
       <c r="AD81" s="4"/>
       <c r="AE81" s="4"/>
@@ -11319,257 +11384,257 @@
     </row>
     <row r="82" spans="1:42" ht="150" x14ac:dyDescent="0.25">
       <c r="A82" s="2" t="s">
-        <v>595</v>
+        <v>585</v>
       </c>
       <c r="B82" s="2"/>
       <c r="C82" s="2" t="s">
         <v>32</v>
       </c>
       <c r="D82" s="2" t="s">
+        <v>565</v>
+      </c>
+      <c r="E82" s="2" t="s">
+        <v>566</v>
+      </c>
+      <c r="F82" s="2" t="s">
+        <v>567</v>
+      </c>
+      <c r="G82" s="2" t="s">
+        <v>568</v>
+      </c>
+      <c r="H82" s="2" t="s">
+        <v>569</v>
+      </c>
+      <c r="I82" s="2" t="s">
+        <v>586</v>
+      </c>
+      <c r="J82" s="2" t="s">
+        <v>587</v>
+      </c>
+      <c r="K82" s="2" t="s">
+        <v>588</v>
+      </c>
+      <c r="L82" s="2" t="s">
+        <v>589</v>
+      </c>
+      <c r="M82" s="2" t="s">
+        <v>590</v>
+      </c>
+      <c r="N82" s="2" t="s">
+        <v>521</v>
+      </c>
+      <c r="O82" s="2" t="s">
         <v>575</v>
       </c>
-      <c r="E82" s="2" t="s">
+      <c r="P82" s="4" t="s">
         <v>576</v>
-      </c>
-      <c r="F82" s="2" t="s">
-        <v>577</v>
-      </c>
-      <c r="G82" s="2" t="s">
-        <v>578</v>
-      </c>
-      <c r="H82" s="2" t="s">
-        <v>579</v>
-      </c>
-      <c r="I82" s="2" t="s">
-        <v>596</v>
-      </c>
-      <c r="J82" s="2" t="s">
-        <v>597</v>
-      </c>
-      <c r="K82" s="2" t="s">
-        <v>598</v>
-      </c>
-      <c r="L82" s="2" t="s">
-        <v>599</v>
-      </c>
-      <c r="M82" s="2" t="s">
-        <v>600</v>
-      </c>
-      <c r="N82" s="2" t="s">
-        <v>523</v>
-      </c>
-      <c r="O82" s="2" t="s">
-        <v>585</v>
-      </c>
-      <c r="P82" s="4" t="s">
-        <v>586</v>
       </c>
       <c r="AO82" s="3"/>
       <c r="AP82" s="3"/>
     </row>
     <row r="83" spans="1:42" ht="150" x14ac:dyDescent="0.25">
       <c r="A83" s="2" t="s">
-        <v>601</v>
+        <v>591</v>
       </c>
       <c r="B83" s="2"/>
       <c r="C83" s="2" t="s">
         <v>32</v>
       </c>
       <c r="D83" s="2" t="s">
+        <v>565</v>
+      </c>
+      <c r="E83" s="2" t="s">
+        <v>566</v>
+      </c>
+      <c r="F83" s="2" t="s">
+        <v>567</v>
+      </c>
+      <c r="G83" s="2" t="s">
+        <v>568</v>
+      </c>
+      <c r="H83" s="2" t="s">
+        <v>569</v>
+      </c>
+      <c r="I83" s="2" t="s">
+        <v>592</v>
+      </c>
+      <c r="J83" s="2" t="s">
+        <v>583</v>
+      </c>
+      <c r="K83" s="2" t="s">
+        <v>593</v>
+      </c>
+      <c r="L83" s="2" t="s">
+        <v>521</v>
+      </c>
+      <c r="M83" s="2" t="s">
         <v>575</v>
       </c>
-      <c r="E83" s="2" t="s">
+      <c r="N83" s="4" t="s">
         <v>576</v>
-      </c>
-      <c r="F83" s="2" t="s">
-        <v>577</v>
-      </c>
-      <c r="G83" s="2" t="s">
-        <v>578</v>
-      </c>
-      <c r="H83" s="2" t="s">
-        <v>579</v>
-      </c>
-      <c r="I83" s="2" t="s">
-        <v>602</v>
-      </c>
-      <c r="J83" s="2" t="s">
-        <v>593</v>
-      </c>
-      <c r="K83" s="2" t="s">
-        <v>603</v>
-      </c>
-      <c r="L83" s="2" t="s">
-        <v>523</v>
-      </c>
-      <c r="M83" s="2" t="s">
-        <v>585</v>
-      </c>
-      <c r="N83" s="4" t="s">
-        <v>586</v>
       </c>
       <c r="AO83" s="3"/>
       <c r="AP83" s="3"/>
     </row>
     <row r="84" spans="1:42" ht="150" x14ac:dyDescent="0.25">
       <c r="A84" s="2" t="s">
-        <v>604</v>
+        <v>594</v>
       </c>
       <c r="B84" s="2"/>
       <c r="C84" s="2" t="s">
         <v>32</v>
       </c>
       <c r="D84" s="2" t="s">
+        <v>565</v>
+      </c>
+      <c r="E84" s="2" t="s">
+        <v>566</v>
+      </c>
+      <c r="F84" s="2" t="s">
+        <v>567</v>
+      </c>
+      <c r="G84" s="2" t="s">
+        <v>568</v>
+      </c>
+      <c r="H84" s="2" t="s">
+        <v>569</v>
+      </c>
+      <c r="I84" s="2" t="s">
+        <v>595</v>
+      </c>
+      <c r="J84" s="2" t="s">
+        <v>596</v>
+      </c>
+      <c r="K84" s="2" t="s">
+        <v>597</v>
+      </c>
+      <c r="L84" s="2" t="s">
+        <v>598</v>
+      </c>
+      <c r="M84" s="2" t="s">
+        <v>599</v>
+      </c>
+      <c r="N84" s="2" t="s">
+        <v>521</v>
+      </c>
+      <c r="O84" s="2" t="s">
         <v>575</v>
       </c>
-      <c r="E84" s="2" t="s">
+      <c r="P84" s="4" t="s">
         <v>576</v>
-      </c>
-      <c r="F84" s="2" t="s">
-        <v>577</v>
-      </c>
-      <c r="G84" s="2" t="s">
-        <v>578</v>
-      </c>
-      <c r="H84" s="2" t="s">
-        <v>579</v>
-      </c>
-      <c r="I84" s="2" t="s">
-        <v>605</v>
-      </c>
-      <c r="J84" s="2" t="s">
-        <v>606</v>
-      </c>
-      <c r="K84" s="2" t="s">
-        <v>607</v>
-      </c>
-      <c r="L84" s="2" t="s">
-        <v>608</v>
-      </c>
-      <c r="M84" s="2" t="s">
-        <v>609</v>
-      </c>
-      <c r="N84" s="2" t="s">
-        <v>523</v>
-      </c>
-      <c r="O84" s="2" t="s">
-        <v>585</v>
-      </c>
-      <c r="P84" s="4" t="s">
-        <v>586</v>
       </c>
       <c r="AO84" s="3"/>
       <c r="AP84" s="3"/>
     </row>
     <row r="85" spans="1:42" ht="150" x14ac:dyDescent="0.25">
       <c r="A85" s="2" t="s">
-        <v>610</v>
+        <v>600</v>
       </c>
       <c r="B85" s="2"/>
       <c r="C85" s="2" t="s">
         <v>32</v>
       </c>
       <c r="D85" s="2" t="s">
+        <v>565</v>
+      </c>
+      <c r="E85" s="2" t="s">
+        <v>566</v>
+      </c>
+      <c r="F85" s="2" t="s">
+        <v>567</v>
+      </c>
+      <c r="G85" s="2" t="s">
+        <v>568</v>
+      </c>
+      <c r="H85" s="2" t="s">
+        <v>569</v>
+      </c>
+      <c r="I85" s="2" t="s">
+        <v>601</v>
+      </c>
+      <c r="J85" s="2" t="s">
+        <v>602</v>
+      </c>
+      <c r="K85" s="2" t="s">
+        <v>603</v>
+      </c>
+      <c r="L85" s="2" t="s">
+        <v>604</v>
+      </c>
+      <c r="M85" s="2" t="s">
+        <v>605</v>
+      </c>
+      <c r="N85" s="2" t="s">
+        <v>606</v>
+      </c>
+      <c r="O85" s="2" t="s">
+        <v>521</v>
+      </c>
+      <c r="P85" s="2" t="s">
         <v>575</v>
       </c>
-      <c r="E85" s="2" t="s">
+      <c r="Q85" s="2" t="s">
         <v>576</v>
-      </c>
-      <c r="F85" s="2" t="s">
-        <v>577</v>
-      </c>
-      <c r="G85" s="2" t="s">
-        <v>578</v>
-      </c>
-      <c r="H85" s="2" t="s">
-        <v>579</v>
-      </c>
-      <c r="I85" s="2" t="s">
-        <v>611</v>
-      </c>
-      <c r="J85" s="2" t="s">
-        <v>612</v>
-      </c>
-      <c r="K85" s="2" t="s">
-        <v>613</v>
-      </c>
-      <c r="L85" s="2" t="s">
-        <v>614</v>
-      </c>
-      <c r="M85" s="2" t="s">
-        <v>615</v>
-      </c>
-      <c r="N85" s="2" t="s">
-        <v>616</v>
-      </c>
-      <c r="O85" s="2" t="s">
-        <v>523</v>
-      </c>
-      <c r="P85" s="2" t="s">
-        <v>585</v>
-      </c>
-      <c r="Q85" s="2" t="s">
-        <v>586</v>
       </c>
       <c r="AO85" s="3"/>
       <c r="AP85" s="3"/>
     </row>
     <row r="86" spans="1:42" ht="135" x14ac:dyDescent="0.25">
       <c r="A86" s="2" t="s">
-        <v>617</v>
+        <v>607</v>
       </c>
       <c r="B86" s="2"/>
       <c r="C86" s="2" t="s">
         <v>32</v>
       </c>
       <c r="D86" s="2" t="s">
+        <v>565</v>
+      </c>
+      <c r="E86" s="2" t="s">
+        <v>566</v>
+      </c>
+      <c r="F86" s="2" t="s">
+        <v>567</v>
+      </c>
+      <c r="G86" s="2" t="s">
+        <v>568</v>
+      </c>
+      <c r="H86" s="2" t="s">
+        <v>569</v>
+      </c>
+      <c r="I86" s="2" t="s">
+        <v>608</v>
+      </c>
+      <c r="J86" s="2" t="s">
+        <v>602</v>
+      </c>
+      <c r="K86" s="2" t="s">
+        <v>603</v>
+      </c>
+      <c r="L86" s="2" t="s">
+        <v>609</v>
+      </c>
+      <c r="M86" s="4" t="s">
+        <v>610</v>
+      </c>
+      <c r="N86" s="4" t="s">
+        <v>611</v>
+      </c>
+      <c r="O86" s="2" t="s">
+        <v>521</v>
+      </c>
+      <c r="P86" s="2" t="s">
         <v>575</v>
       </c>
-      <c r="E86" s="2" t="s">
+      <c r="Q86" s="4" t="s">
         <v>576</v>
-      </c>
-      <c r="F86" s="2" t="s">
-        <v>577</v>
-      </c>
-      <c r="G86" s="2" t="s">
-        <v>578</v>
-      </c>
-      <c r="H86" s="2" t="s">
-        <v>579</v>
-      </c>
-      <c r="I86" s="2" t="s">
-        <v>618</v>
-      </c>
-      <c r="J86" s="2" t="s">
-        <v>612</v>
-      </c>
-      <c r="K86" s="2" t="s">
-        <v>613</v>
-      </c>
-      <c r="L86" s="2" t="s">
-        <v>619</v>
-      </c>
-      <c r="M86" s="4" t="s">
-        <v>620</v>
-      </c>
-      <c r="N86" s="4" t="s">
-        <v>621</v>
-      </c>
-      <c r="O86" s="2" t="s">
-        <v>523</v>
-      </c>
-      <c r="P86" s="2" t="s">
-        <v>585</v>
-      </c>
-      <c r="Q86" s="4" t="s">
-        <v>586</v>
       </c>
       <c r="AO86" s="3"/>
       <c r="AP86" s="3"/>
     </row>
     <row r="87" spans="1:42" ht="212.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A87" s="2" t="s">
-        <v>557</v>
+        <v>747</v>
       </c>
       <c r="B87" s="2"/>
       <c r="C87" s="6" t="s">
@@ -11594,7 +11659,7 @@
         <v>322</v>
       </c>
       <c r="J87" s="2" t="s">
-        <v>558</v>
+        <v>555</v>
       </c>
       <c r="K87" s="2" t="s">
         <v>376</v>
@@ -11631,7 +11696,7 @@
     </row>
     <row r="88" spans="1:42" ht="214.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A88" s="2" t="s">
-        <v>559</v>
+        <v>748</v>
       </c>
       <c r="B88" s="2"/>
       <c r="C88" s="6" t="s">
@@ -11656,7 +11721,7 @@
         <v>340</v>
       </c>
       <c r="J88" s="52" t="s">
-        <v>558</v>
+        <v>555</v>
       </c>
       <c r="K88" s="2" t="s">
         <v>376</v>
@@ -11677,7 +11742,7 @@
         <v>381</v>
       </c>
       <c r="Q88" s="2" t="s">
-        <v>560</v>
+        <v>556</v>
       </c>
       <c r="R88" s="2" t="s">
         <v>383</v>
@@ -11693,7 +11758,7 @@
     </row>
     <row r="89" spans="1:42" ht="210" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A89" s="2" t="s">
-        <v>561</v>
+        <v>749</v>
       </c>
       <c r="B89" s="2"/>
       <c r="C89" s="6" t="s">
@@ -11718,7 +11783,7 @@
         <v>345</v>
       </c>
       <c r="J89" s="52" t="s">
-        <v>558</v>
+        <v>555</v>
       </c>
       <c r="K89" s="2" t="s">
         <v>376</v>
@@ -11739,7 +11804,7 @@
         <v>381</v>
       </c>
       <c r="Q89" s="2" t="s">
-        <v>560</v>
+        <v>556</v>
       </c>
       <c r="R89" s="2" t="s">
         <v>383</v>
@@ -11755,7 +11820,7 @@
     </row>
     <row r="90" spans="1:42" ht="213" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A90" s="2" t="s">
-        <v>562</v>
+        <v>750</v>
       </c>
       <c r="B90" s="2"/>
       <c r="C90" s="6" t="s">
@@ -11780,7 +11845,7 @@
         <v>350</v>
       </c>
       <c r="J90" s="52" t="s">
-        <v>558</v>
+        <v>555</v>
       </c>
       <c r="K90" s="2" t="s">
         <v>376</v>
@@ -11801,7 +11866,7 @@
         <v>381</v>
       </c>
       <c r="Q90" s="2" t="s">
-        <v>560</v>
+        <v>556</v>
       </c>
       <c r="R90" s="2" t="s">
         <v>383</v>
@@ -11810,14 +11875,14 @@
         <v>384</v>
       </c>
       <c r="T90" s="2" t="s">
-        <v>567</v>
+        <v>558</v>
       </c>
       <c r="AO90" s="3"/>
       <c r="AP90" s="3"/>
     </row>
     <row r="91" spans="1:42" ht="212.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A91" s="2" t="s">
-        <v>563</v>
+        <v>751</v>
       </c>
       <c r="B91" s="2"/>
       <c r="C91" s="6" t="s">
@@ -11842,7 +11907,7 @@
         <v>355</v>
       </c>
       <c r="J91" s="52" t="s">
-        <v>558</v>
+        <v>555</v>
       </c>
       <c r="K91" s="2" t="s">
         <v>376</v>
@@ -11863,7 +11928,7 @@
         <v>381</v>
       </c>
       <c r="Q91" s="2" t="s">
-        <v>560</v>
+        <v>556</v>
       </c>
       <c r="R91" s="2" t="s">
         <v>383</v>
@@ -11872,14 +11937,14 @@
         <v>384</v>
       </c>
       <c r="T91" s="2" t="s">
-        <v>568</v>
+        <v>559</v>
       </c>
       <c r="AO91" s="3"/>
       <c r="AP91" s="3"/>
     </row>
     <row r="92" spans="1:42" ht="210.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A92" s="2" t="s">
-        <v>564</v>
+        <v>752</v>
       </c>
       <c r="B92" s="2"/>
       <c r="C92" s="6" t="s">
@@ -11904,7 +11969,7 @@
         <v>402</v>
       </c>
       <c r="J92" s="52" t="s">
-        <v>558</v>
+        <v>555</v>
       </c>
       <c r="K92" s="2" t="s">
         <v>376</v>
@@ -11925,7 +11990,7 @@
         <v>381</v>
       </c>
       <c r="Q92" s="2" t="s">
-        <v>560</v>
+        <v>556</v>
       </c>
       <c r="R92" s="2" t="s">
         <v>383</v>
@@ -11934,14 +11999,14 @@
         <v>384</v>
       </c>
       <c r="T92" s="2" t="s">
-        <v>569</v>
+        <v>560</v>
       </c>
       <c r="AO92" s="3"/>
       <c r="AP92" s="3"/>
     </row>
     <row r="93" spans="1:42" ht="213" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A93" s="2" t="s">
-        <v>565</v>
+        <v>753</v>
       </c>
       <c r="B93" s="2"/>
       <c r="C93" s="6" t="s">
@@ -11963,10 +12028,10 @@
         <v>321</v>
       </c>
       <c r="I93" s="2" t="s">
-        <v>566</v>
+        <v>557</v>
       </c>
       <c r="J93" s="52" t="s">
-        <v>558</v>
+        <v>555</v>
       </c>
       <c r="K93" s="2" t="s">
         <v>376</v>
@@ -11987,7 +12052,7 @@
         <v>381</v>
       </c>
       <c r="Q93" s="2" t="s">
-        <v>560</v>
+        <v>556</v>
       </c>
       <c r="R93" s="2" t="s">
         <v>383</v>
@@ -11996,14 +12061,14 @@
         <v>384</v>
       </c>
       <c r="T93" s="2" t="s">
-        <v>570</v>
+        <v>561</v>
       </c>
       <c r="AO93" s="3"/>
       <c r="AP93" s="3"/>
     </row>
     <row r="94" spans="1:42" ht="215.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A94" s="2" t="s">
-        <v>571</v>
+        <v>754</v>
       </c>
       <c r="B94" s="2"/>
       <c r="C94" s="6" t="s">
@@ -12025,10 +12090,10 @@
         <v>321</v>
       </c>
       <c r="I94" s="2" t="s">
-        <v>572</v>
+        <v>562</v>
       </c>
       <c r="J94" s="52" t="s">
-        <v>558</v>
+        <v>555</v>
       </c>
       <c r="K94" s="2" t="s">
         <v>376</v>
@@ -12049,7 +12114,7 @@
         <v>381</v>
       </c>
       <c r="Q94" s="2" t="s">
-        <v>560</v>
+        <v>556</v>
       </c>
       <c r="R94" s="2" t="s">
         <v>383</v>
@@ -12058,115 +12123,115 @@
         <v>384</v>
       </c>
       <c r="T94" s="2" t="s">
-        <v>573</v>
+        <v>563</v>
       </c>
       <c r="AO94" s="3"/>
       <c r="AP94" s="3"/>
     </row>
     <row r="95" spans="1:42" ht="150" x14ac:dyDescent="0.25">
       <c r="A95" s="2" t="s">
-        <v>622</v>
+        <v>612</v>
       </c>
       <c r="B95" s="2"/>
       <c r="C95" s="2" t="s">
         <v>32</v>
       </c>
       <c r="D95" s="2" t="s">
-        <v>575</v>
+        <v>565</v>
       </c>
       <c r="E95" s="2" t="s">
-        <v>576</v>
+        <v>566</v>
       </c>
       <c r="F95" s="2" t="s">
-        <v>577</v>
+        <v>567</v>
       </c>
       <c r="G95" s="2" t="s">
-        <v>578</v>
+        <v>568</v>
       </c>
       <c r="H95" s="2" t="s">
-        <v>623</v>
+        <v>613</v>
       </c>
       <c r="I95" s="2" t="s">
-        <v>624</v>
+        <v>614</v>
       </c>
       <c r="J95" s="2" t="s">
-        <v>625</v>
+        <v>615</v>
       </c>
       <c r="K95" s="2" t="s">
-        <v>626</v>
+        <v>616</v>
       </c>
       <c r="L95" s="2" t="s">
-        <v>627</v>
+        <v>617</v>
       </c>
       <c r="AO95" s="3"/>
       <c r="AP95" s="3"/>
     </row>
     <row r="96" spans="1:42" ht="135" x14ac:dyDescent="0.25">
       <c r="A96" s="2" t="s">
-        <v>628</v>
+        <v>618</v>
       </c>
       <c r="B96" s="2"/>
       <c r="C96" s="2" t="s">
         <v>32</v>
       </c>
       <c r="D96" s="2" t="s">
-        <v>575</v>
+        <v>565</v>
       </c>
       <c r="E96" s="2" t="s">
-        <v>576</v>
+        <v>566</v>
       </c>
       <c r="F96" s="2" t="s">
-        <v>577</v>
+        <v>567</v>
       </c>
       <c r="G96" s="2" t="s">
-        <v>578</v>
+        <v>568</v>
       </c>
       <c r="H96" s="2" t="s">
-        <v>629</v>
+        <v>619</v>
       </c>
       <c r="I96" s="2" t="s">
-        <v>630</v>
+        <v>620</v>
       </c>
       <c r="J96" s="2" t="s">
-        <v>631</v>
+        <v>621</v>
       </c>
       <c r="K96" s="2" t="s">
-        <v>632</v>
+        <v>622</v>
       </c>
       <c r="L96" s="2" t="s">
-        <v>633</v>
+        <v>623</v>
       </c>
       <c r="AO96" s="3"/>
       <c r="AP96" s="3"/>
     </row>
     <row r="97" spans="1:42" ht="135" x14ac:dyDescent="0.25">
       <c r="A97" s="2" t="s">
-        <v>634</v>
+        <v>624</v>
       </c>
       <c r="B97" s="2"/>
       <c r="C97" s="2" t="s">
         <v>32</v>
       </c>
       <c r="D97" s="2" t="s">
-        <v>575</v>
+        <v>565</v>
       </c>
       <c r="E97" s="2" t="s">
-        <v>576</v>
+        <v>566</v>
       </c>
       <c r="F97" s="2" t="s">
-        <v>577</v>
+        <v>567</v>
       </c>
       <c r="G97" s="2" t="s">
-        <v>578</v>
+        <v>568</v>
       </c>
       <c r="H97" s="2" t="s">
-        <v>635</v>
+        <v>625</v>
       </c>
       <c r="I97" s="2" t="s">
-        <v>636</v>
+        <v>626</v>
       </c>
       <c r="J97" s="2" t="s">
-        <v>637</v>
+        <v>621</v>
       </c>
       <c r="K97" s="2"/>
       <c r="L97" s="2"/>
@@ -12175,70 +12240,70 @@
     </row>
     <row r="98" spans="1:42" ht="150" x14ac:dyDescent="0.25">
       <c r="A98" s="2" t="s">
-        <v>638</v>
+        <v>627</v>
       </c>
       <c r="B98" s="2"/>
       <c r="C98" s="2" t="s">
         <v>32</v>
       </c>
       <c r="D98" s="2" t="s">
-        <v>575</v>
+        <v>565</v>
       </c>
       <c r="E98" s="2" t="s">
-        <v>576</v>
+        <v>566</v>
       </c>
       <c r="F98" s="2" t="s">
-        <v>577</v>
+        <v>567</v>
       </c>
       <c r="G98" s="2" t="s">
-        <v>578</v>
+        <v>568</v>
       </c>
       <c r="H98" s="2" t="s">
-        <v>639</v>
+        <v>628</v>
       </c>
       <c r="I98" s="2" t="s">
-        <v>640</v>
+        <v>629</v>
       </c>
       <c r="J98" s="2" t="s">
-        <v>641</v>
+        <v>630</v>
       </c>
       <c r="K98" s="2" t="s">
-        <v>642</v>
+        <v>631</v>
       </c>
       <c r="L98" s="2" t="s">
-        <v>643</v>
+        <v>632</v>
       </c>
       <c r="AO98" s="3"/>
       <c r="AP98" s="3"/>
     </row>
     <row r="99" spans="1:42" ht="150" x14ac:dyDescent="0.25">
       <c r="A99" s="2" t="s">
-        <v>644</v>
+        <v>633</v>
       </c>
       <c r="B99" s="2"/>
       <c r="C99" s="2" t="s">
         <v>32</v>
       </c>
       <c r="D99" s="2" t="s">
-        <v>575</v>
+        <v>565</v>
       </c>
       <c r="E99" s="2" t="s">
-        <v>576</v>
+        <v>566</v>
       </c>
       <c r="F99" s="2" t="s">
-        <v>577</v>
+        <v>567</v>
       </c>
       <c r="G99" s="2" t="s">
-        <v>578</v>
+        <v>568</v>
       </c>
       <c r="H99" s="2" t="s">
-        <v>645</v>
+        <v>634</v>
       </c>
       <c r="I99" s="2" t="s">
-        <v>646</v>
+        <v>635</v>
       </c>
       <c r="J99" s="2" t="s">
-        <v>647</v>
+        <v>636</v>
       </c>
       <c r="K99" s="2"/>
       <c r="L99" s="2"/>
@@ -12247,149 +12312,149 @@
     </row>
     <row r="100" spans="1:42" ht="135" x14ac:dyDescent="0.25">
       <c r="A100" s="2" t="s">
-        <v>648</v>
+        <v>637</v>
       </c>
       <c r="B100" s="2"/>
       <c r="C100" s="2" t="s">
         <v>32</v>
       </c>
       <c r="D100" s="2" t="s">
-        <v>575</v>
+        <v>565</v>
       </c>
       <c r="E100" s="2" t="s">
-        <v>576</v>
+        <v>566</v>
       </c>
       <c r="F100" s="2" t="s">
-        <v>577</v>
+        <v>567</v>
       </c>
       <c r="G100" s="2" t="s">
-        <v>578</v>
+        <v>568</v>
       </c>
       <c r="H100" s="2" t="s">
-        <v>649</v>
+        <v>638</v>
       </c>
       <c r="I100" s="2" t="s">
-        <v>650</v>
+        <v>639</v>
       </c>
       <c r="J100" s="2" t="s">
-        <v>651</v>
+        <v>640</v>
       </c>
       <c r="K100" s="2" t="s">
-        <v>652</v>
+        <v>641</v>
       </c>
       <c r="L100" s="2" t="s">
-        <v>653</v>
+        <v>642</v>
       </c>
       <c r="AO100" s="3"/>
       <c r="AP100" s="3"/>
     </row>
     <row r="101" spans="1:42" ht="135" x14ac:dyDescent="0.25">
       <c r="A101" s="2" t="s">
-        <v>654</v>
+        <v>643</v>
       </c>
       <c r="B101" s="2"/>
       <c r="C101" s="2" t="s">
         <v>32</v>
       </c>
       <c r="D101" s="2" t="s">
-        <v>575</v>
+        <v>565</v>
       </c>
       <c r="E101" s="2" t="s">
-        <v>576</v>
+        <v>566</v>
       </c>
       <c r="F101" s="2" t="s">
-        <v>577</v>
+        <v>567</v>
       </c>
       <c r="G101" s="2" t="s">
-        <v>578</v>
+        <v>568</v>
       </c>
       <c r="H101" s="2" t="s">
-        <v>655</v>
+        <v>644</v>
       </c>
       <c r="I101" s="2" t="s">
-        <v>656</v>
+        <v>645</v>
       </c>
       <c r="J101" s="2" t="s">
-        <v>631</v>
+        <v>621</v>
       </c>
       <c r="K101" s="2" t="s">
-        <v>651</v>
+        <v>640</v>
       </c>
       <c r="L101" s="2" t="s">
-        <v>657</v>
+        <v>646</v>
       </c>
       <c r="M101" s="2" t="s">
-        <v>658</v>
+        <v>647</v>
       </c>
       <c r="AO101" s="3"/>
       <c r="AP101" s="3"/>
     </row>
     <row r="102" spans="1:42" ht="135" x14ac:dyDescent="0.25">
       <c r="A102" s="2" t="s">
-        <v>659</v>
+        <v>648</v>
       </c>
       <c r="B102" s="2"/>
       <c r="C102" s="2" t="s">
         <v>32</v>
       </c>
       <c r="D102" s="2" t="s">
-        <v>575</v>
+        <v>565</v>
       </c>
       <c r="E102" s="2" t="s">
-        <v>576</v>
+        <v>566</v>
       </c>
       <c r="F102" s="2" t="s">
-        <v>577</v>
+        <v>567</v>
       </c>
       <c r="G102" s="2" t="s">
-        <v>578</v>
+        <v>568</v>
       </c>
       <c r="H102" s="2" t="s">
-        <v>660</v>
+        <v>649</v>
       </c>
       <c r="I102" s="2" t="s">
-        <v>661</v>
+        <v>650</v>
       </c>
       <c r="J102" s="2" t="s">
-        <v>631</v>
+        <v>621</v>
       </c>
       <c r="K102" s="2" t="s">
-        <v>662</v>
+        <v>651</v>
       </c>
       <c r="L102" s="2" t="s">
-        <v>663</v>
+        <v>652</v>
       </c>
       <c r="M102" s="4" t="s">
-        <v>664</v>
+        <v>653</v>
       </c>
       <c r="AO102" s="3"/>
       <c r="AP102" s="3"/>
     </row>
     <row r="103" spans="1:42" ht="105" x14ac:dyDescent="0.25">
       <c r="A103" s="2" t="s">
-        <v>665</v>
+        <v>654</v>
       </c>
       <c r="B103" s="2"/>
       <c r="C103" s="2" t="s">
         <v>32</v>
       </c>
       <c r="D103" s="2" t="s">
-        <v>575</v>
+        <v>565</v>
       </c>
       <c r="E103" s="2" t="s">
-        <v>576</v>
+        <v>566</v>
       </c>
       <c r="F103" s="2" t="s">
-        <v>577</v>
+        <v>567</v>
       </c>
       <c r="G103" s="2" t="s">
-        <v>578</v>
+        <v>568</v>
       </c>
       <c r="H103" s="2" t="s">
-        <v>666</v>
+        <v>655</v>
       </c>
       <c r="I103" s="2" t="s">
-        <v>667</v>
+        <v>656</v>
       </c>
       <c r="J103" s="2"/>
       <c r="K103" s="2"/>
@@ -12397,23 +12462,23 @@
     </row>
     <row r="104" spans="1:42" ht="105" x14ac:dyDescent="0.25">
       <c r="A104" s="2" t="s">
-        <v>668</v>
+        <v>657</v>
       </c>
       <c r="B104" s="2"/>
       <c r="C104" s="2" t="s">
         <v>32</v>
       </c>
       <c r="D104" s="2" t="s">
-        <v>575</v>
+        <v>565</v>
       </c>
       <c r="E104" s="2" t="s">
-        <v>576</v>
+        <v>566</v>
       </c>
       <c r="F104" s="2" t="s">
-        <v>577</v>
+        <v>567</v>
       </c>
       <c r="G104" s="2" t="s">
-        <v>578</v>
+        <v>568</v>
       </c>
       <c r="H104" s="2"/>
       <c r="I104" s="2"/>

</xml_diff>